<commit_message>
Revert "edited graphs "
This reverts commit 219dcad986589a0c4513221d1591f771bb7b7c80.
</commit_message>
<xml_diff>
--- a/Documentation/Graphs.xlsx
+++ b/Documentation/Graphs.xlsx
@@ -118,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -131,9 +131,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,7 +470,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -856,7 +852,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1239,7 +1234,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1390,34 +1384,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>83701.666666666672</c:v>
+                  <c:v>33701.666666666664</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74521</c:v>
+                  <c:v>54657.666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77314.666666666672</c:v>
+                  <c:v>57314.666666666664</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86650.333333333328</c:v>
+                  <c:v>73317</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>95310</c:v>
+                  <c:v>78643.333333333328</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>106130.33333333333</c:v>
+                  <c:v>89463.666666666672</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>103323.66666666667</c:v>
+                  <c:v>136657</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>119496.66666666667</c:v>
+                  <c:v>155212</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>109322</c:v>
+                  <c:v>122655.33333333333</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>129170.33333333333</c:v>
+                  <c:v>188503.66666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1620,38 +1614,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1773,34 +1735,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>174699.33333333334</c:v>
+                  <c:v>104399.33333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>311359.33333333331</c:v>
+                  <c:v>140015.33333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>417391.33333333331</c:v>
+                  <c:v>191367.33333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>413401.33333333331</c:v>
+                  <c:v>243375.66666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>256566.33333333334</c:v>
+                  <c:v>327276.33333333331</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>474023</c:v>
+                  <c:v>389049.66666666669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>628526</c:v>
+                  <c:v>479518</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>888267.66666666663</c:v>
+                  <c:v>491636.66666666669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1249738.3333333333</c:v>
+                  <c:v>525924.66666666663</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1351802.3333333333</c:v>
+                  <c:v>620588.66666666663</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2003,38 +1965,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2159,28 +2089,28 @@
                   <c:v>78646.666666666672</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>115976.33333333333</c:v>
+                  <c:v>102643</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>108425.66666666667</c:v>
+                  <c:v>198425.66666666666</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>132003</c:v>
+                  <c:v>181669.66666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>173877.66666666666</c:v>
+                  <c:v>207211</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>189603</c:v>
+                  <c:v>266269.66666666669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>197209.33333333334</c:v>
+                  <c:v>290542.66666666669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>234010.33333333334</c:v>
+                  <c:v>367343.66666666669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>185650.33333333334</c:v>
+                  <c:v>218983.66666666666</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>185053.33333333334</c:v>
@@ -2386,38 +2316,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -7458,16 +7356,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7561,33 +7459,33 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>88536</v>
+        <v>28536</v>
       </c>
       <c r="C4">
-        <v>70109</v>
+        <v>40109</v>
       </c>
       <c r="D4">
-        <v>92460</v>
+        <v>32460</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E13" si="0">AVERAGE(B4:D4)</f>
-        <v>83701.666666666672</v>
+        <v>33701.666666666664</v>
       </c>
       <c r="G4">
         <v>100</v>
       </c>
       <c r="H4">
-        <v>420012</v>
+        <v>176712</v>
       </c>
       <c r="I4">
-        <v>50083</v>
-      </c>
-      <c r="J4" s="5">
-        <v>54003</v>
+        <v>68483</v>
+      </c>
+      <c r="J4">
+        <v>68003</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K13" si="1">AVERAGE(H4:J4)</f>
-        <v>174699.33333333334</v>
+        <v>104399.33333333333</v>
       </c>
       <c r="M4">
         <v>10</v>
@@ -7611,33 +7509,33 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>79984</v>
+        <v>55984</v>
       </c>
       <c r="C5">
-        <v>69986</v>
+        <v>55986</v>
       </c>
       <c r="D5">
-        <v>73593</v>
+        <v>52003</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>74521</v>
+        <v>54657.666666666664</v>
       </c>
       <c r="G5">
         <v>200</v>
       </c>
       <c r="H5">
-        <v>480778</v>
+        <v>180778</v>
       </c>
       <c r="I5">
-        <v>385297</v>
-      </c>
-      <c r="J5" s="5">
-        <v>68003</v>
+        <v>115297</v>
+      </c>
+      <c r="J5">
+        <v>123971</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>311359.33333333331</v>
+        <v>140015.33333333334</v>
       </c>
       <c r="M5">
         <v>20</v>
@@ -7646,14 +7544,14 @@
         <v>227954</v>
       </c>
       <c r="O5">
-        <v>75986</v>
+        <v>35986</v>
       </c>
       <c r="P5">
         <v>43989</v>
       </c>
       <c r="Q5">
         <f t="shared" ref="Q5:Q13" si="2">AVERAGE(N5:P5)</f>
-        <v>115976.33333333333</v>
+        <v>102643</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -7661,49 +7559,49 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>75988</v>
+        <v>55988</v>
       </c>
       <c r="C6">
-        <v>79986</v>
+        <v>59986</v>
       </c>
       <c r="D6">
-        <v>75970</v>
+        <v>55970</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>77314.666666666672</v>
+        <v>57314.666666666664</v>
       </c>
       <c r="G6">
         <v>300</v>
       </c>
       <c r="H6">
-        <v>589971</v>
+        <v>187971</v>
       </c>
       <c r="I6">
-        <v>594200</v>
-      </c>
-      <c r="J6" s="5">
-        <v>68003</v>
+        <v>194200</v>
+      </c>
+      <c r="J6">
+        <v>191931</v>
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>417391.33333333331</v>
+        <v>191367.33333333334</v>
       </c>
       <c r="M6">
         <v>30</v>
       </c>
       <c r="N6">
-        <v>233306</v>
+        <v>423306</v>
       </c>
       <c r="O6">
-        <v>41984</v>
+        <v>91984</v>
       </c>
       <c r="P6">
-        <v>49987</v>
+        <v>79987</v>
       </c>
       <c r="Q6">
         <f t="shared" si="2"/>
-        <v>108425.66666666667</v>
+        <v>198425.66666666666</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -7711,33 +7609,33 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>87981</v>
+        <v>67981</v>
       </c>
       <c r="C7">
-        <v>89979</v>
+        <v>79979</v>
       </c>
       <c r="D7">
-        <v>81991</v>
+        <v>71991</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>86650.333333333328</v>
+        <v>73317</v>
       </c>
       <c r="G7">
         <v>400</v>
       </c>
       <c r="H7">
-        <v>534052</v>
+        <v>234052</v>
       </c>
       <c r="I7">
-        <v>638149</v>
-      </c>
-      <c r="J7" s="5">
-        <v>68003</v>
+        <v>238149</v>
+      </c>
+      <c r="J7">
+        <v>257926</v>
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
-        <v>413401.33333333331</v>
+        <v>243375.66666666666</v>
       </c>
       <c r="M7">
         <v>40</v>
@@ -7746,14 +7644,14 @@
         <v>321060</v>
       </c>
       <c r="O7">
-        <v>61965</v>
+        <v>111965</v>
       </c>
       <c r="P7">
-        <v>12984</v>
+        <v>111984</v>
       </c>
       <c r="Q7">
         <f t="shared" si="2"/>
-        <v>132003</v>
+        <v>181669.66666666666</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -7761,17 +7659,17 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>99982</v>
+        <v>79982</v>
       </c>
       <c r="C8">
-        <v>89980</v>
+        <v>79980</v>
       </c>
       <c r="D8">
-        <v>95968</v>
+        <v>75968</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>95310</v>
+        <v>78643.333333333328</v>
       </c>
       <c r="G8">
         <v>500</v>
@@ -7782,18 +7680,18 @@
       <c r="I8">
         <v>398157</v>
       </c>
-      <c r="J8" s="5">
-        <v>68003</v>
+      <c r="J8">
+        <v>280133</v>
       </c>
       <c r="K8">
         <f t="shared" si="1"/>
-        <v>256566.33333333334</v>
+        <v>327276.33333333331</v>
       </c>
       <c r="M8">
         <v>50</v>
       </c>
       <c r="N8">
-        <v>365693</v>
+        <v>465693</v>
       </c>
       <c r="O8">
         <v>79980</v>
@@ -7803,7 +7701,7 @@
       </c>
       <c r="Q8">
         <f t="shared" si="2"/>
-        <v>173877.66666666666</v>
+        <v>207211</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -7811,49 +7709,49 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>107997</v>
+        <v>87997</v>
       </c>
       <c r="C9">
-        <v>98418</v>
+        <v>88418</v>
       </c>
       <c r="D9">
-        <v>111976</v>
+        <v>91976</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>106130.33333333333</v>
+        <v>89463.666666666672</v>
       </c>
       <c r="G9">
         <v>600</v>
       </c>
       <c r="H9">
-        <v>661113</v>
+        <v>361113</v>
       </c>
       <c r="I9">
-        <v>692953</v>
-      </c>
-      <c r="J9" s="5">
-        <v>68003</v>
+        <v>412953</v>
+      </c>
+      <c r="J9">
+        <v>393083</v>
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
-        <v>474023</v>
+        <v>389049.66666666669</v>
       </c>
       <c r="M9">
         <v>60</v>
       </c>
       <c r="N9">
-        <v>407504</v>
+        <v>607504</v>
       </c>
       <c r="O9">
-        <v>79997</v>
+        <v>99997</v>
       </c>
       <c r="P9">
-        <v>81308</v>
+        <v>91308</v>
       </c>
       <c r="Q9">
         <f t="shared" si="2"/>
-        <v>189603</v>
+        <v>266269.66666666669</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -7861,7 +7759,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>110310</v>
+        <v>210310</v>
       </c>
       <c r="C10">
         <v>103993</v>
@@ -7871,39 +7769,39 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>103323.66666666667</v>
+        <v>136657</v>
       </c>
       <c r="G10">
         <v>700</v>
       </c>
       <c r="H10">
-        <v>917966</v>
+        <v>417966</v>
       </c>
       <c r="I10">
-        <v>899609</v>
-      </c>
-      <c r="J10" s="5">
-        <v>68003</v>
+        <v>429609</v>
+      </c>
+      <c r="J10">
+        <v>590979</v>
       </c>
       <c r="K10">
         <f t="shared" si="1"/>
-        <v>628526</v>
+        <v>479518</v>
       </c>
       <c r="M10">
         <v>70</v>
       </c>
       <c r="N10">
-        <v>427837</v>
+        <v>627837</v>
       </c>
       <c r="O10">
-        <v>81951</v>
+        <v>111951</v>
       </c>
       <c r="P10">
-        <v>81840</v>
+        <v>131840</v>
       </c>
       <c r="Q10">
         <f t="shared" si="2"/>
-        <v>197209.33333333334</v>
+        <v>290542.66666666669</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -7911,49 +7809,49 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>121814</v>
+        <v>151814</v>
       </c>
       <c r="C11">
-        <v>124673</v>
+        <v>201819</v>
       </c>
       <c r="D11">
         <v>112003</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>119496.66666666667</v>
+        <v>155212</v>
       </c>
       <c r="G11">
         <v>800</v>
       </c>
       <c r="H11">
-        <v>1143364</v>
+        <v>483364</v>
       </c>
       <c r="I11">
-        <v>1453436</v>
-      </c>
-      <c r="J11" s="5">
-        <v>68003</v>
+        <v>453436</v>
+      </c>
+      <c r="J11">
+        <v>538110</v>
       </c>
       <c r="K11">
         <f t="shared" si="1"/>
-        <v>888267.66666666663</v>
+        <v>491636.66666666669</v>
       </c>
       <c r="M11">
         <v>80</v>
       </c>
       <c r="N11">
-        <v>522805</v>
+        <v>822805</v>
       </c>
       <c r="O11">
-        <v>82668</v>
+        <v>132668</v>
       </c>
       <c r="P11">
-        <v>96558</v>
+        <v>146558</v>
       </c>
       <c r="Q11">
         <f t="shared" si="2"/>
-        <v>234010.33333333334</v>
+        <v>367343.66666666669</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -7967,27 +7865,27 @@
         <v>104445</v>
       </c>
       <c r="D12">
-        <v>111852</v>
+        <v>151852</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>109322</v>
+        <v>122655.33333333333</v>
       </c>
       <c r="G12">
         <v>900</v>
       </c>
       <c r="H12">
-        <v>1730170</v>
+        <v>530170</v>
       </c>
       <c r="I12">
-        <v>1951042</v>
-      </c>
-      <c r="J12" s="5">
-        <v>68003</v>
+        <v>551042</v>
+      </c>
+      <c r="J12">
+        <v>496562</v>
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>1249738.3333333333</v>
+        <v>525924.66666666663</v>
       </c>
       <c r="M12">
         <v>90</v>
@@ -7996,14 +7894,14 @@
         <v>306868</v>
       </c>
       <c r="O12">
-        <v>114116</v>
+        <v>214116</v>
       </c>
       <c r="P12">
         <v>135967</v>
       </c>
       <c r="Q12">
         <f t="shared" si="2"/>
-        <v>185650.33333333334</v>
+        <v>218983.66666666666</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -8014,30 +7912,30 @@
         <v>135701</v>
       </c>
       <c r="C13">
-        <v>120926</v>
+        <v>198926</v>
       </c>
       <c r="D13">
-        <v>130884</v>
+        <v>230884</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>129170.33333333333</v>
+        <v>188503.66666666666</v>
       </c>
       <c r="G13">
         <v>1000</v>
       </c>
       <c r="H13">
-        <v>1994803</v>
+        <v>594803</v>
       </c>
       <c r="I13">
-        <v>1992601</v>
-      </c>
-      <c r="J13" s="5">
-        <v>68003</v>
+        <v>672601</v>
+      </c>
+      <c r="J13">
+        <v>594362</v>
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>1351802.3333333333</v>
+        <v>620588.66666666663</v>
       </c>
       <c r="M13">
         <v>100</v>

</xml_diff>

<commit_message>
Changes in graphs and comment added in code
</commit_message>
<xml_diff>
--- a/Documentation/Graphs.xlsx
+++ b/Documentation/Graphs.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shalin\Desktop\project-pyteam\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="sphere" sheetId="1" r:id="rId1"/>
     <sheet name="rastrigin" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="16">
   <si>
     <t>T1 (ms)</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>T3 (ms)</t>
-  </si>
-  <si>
-    <t>Average</t>
   </si>
   <si>
     <t>Num_Iterations</t>
@@ -71,11 +68,17 @@
   <si>
     <t>------</t>
   </si>
+  <si>
+    <t>Average (s)</t>
+  </si>
+  <si>
+    <t>Average(s)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -118,11 +121,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -155,7 +159,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -235,43 +239,43 @@
             <c:numRef>
               <c:f>sphere!$K$5:$K$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>117511.33333333333</c:v>
+                  <c:v>117.51133333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>288097.66666666669</c:v>
+                  <c:v>288.09766666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>355190.33333333331</c:v>
+                  <c:v>355.19033333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>387130.66666666669</c:v>
+                  <c:v>387.13066666666668</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>386874.33333333331</c:v>
+                  <c:v>386.87433333333331</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>488589.66666666669</c:v>
+                  <c:v>488.58966666666669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>807372</c:v>
+                  <c:v>807.37200000000007</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1369390</c:v>
+                  <c:v>1369.39</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1297286.3333333333</c:v>
+                  <c:v>1297.2863333333332</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1386414</c:v>
+                  <c:v>1386.414</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-A408-42EC-ABB5-BED3ED326330}"/>
             </c:ext>
@@ -302,40 +306,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>303475.66666666669</c:v>
+                  <c:v>303.47566666666671</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>511795.66666666669</c:v>
+                  <c:v>511.7956666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>710549.33333333337</c:v>
+                  <c:v>710.54933333333338</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>826788</c:v>
+                  <c:v>826.78800000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>752781</c:v>
+                  <c:v>752.78100000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1212891.3333333333</c:v>
+                  <c:v>1212.8913333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1559120</c:v>
+                  <c:v>1559.1200000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1650092.6666666667</c:v>
+                  <c:v>1650.0926666666667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1780338.3333333333</c:v>
+                  <c:v>1780.3383333333334</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1469181</c:v>
+                  <c:v>1469.181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-A408-42EC-ABB5-BED3ED326330}"/>
             </c:ext>
@@ -350,11 +354,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1739611807"/>
-        <c:axId val="1739598079"/>
+        <c:axId val="-225676304"/>
+        <c:axId val="-225681200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1739611807"/>
+        <c:axId val="-225676304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -397,7 +401,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1739598079"/>
+        <c:crossAx val="-225681200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -405,7 +409,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1739598079"/>
+        <c:axId val="-225681200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -425,7 +429,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -456,7 +460,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1739611807"/>
+        <c:crossAx val="-225676304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -470,6 +474,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -537,7 +542,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -617,43 +622,43 @@
             <c:numRef>
               <c:f>sphere!$Q$5:$Q$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>23992.333333333332</c:v>
+                  <c:v>23.992333333333331</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45418</c:v>
+                  <c:v>45.417999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>93180.666666666672</c:v>
+                  <c:v>93.180666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>113995</c:v>
+                  <c:v>113.995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>95912</c:v>
+                  <c:v>95.912000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>85162.666666666672</c:v>
+                  <c:v>85.162666666666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>114931</c:v>
+                  <c:v>114.931</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>168129</c:v>
+                  <c:v>168.12899999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>139852.33333333334</c:v>
+                  <c:v>139.85233333333335</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>191386.66666666666</c:v>
+                  <c:v>191.38666666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-232C-407E-B5B4-E4B6B5F1FCF8}"/>
             </c:ext>
@@ -684,40 +689,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>362141</c:v>
+                  <c:v>362.14100000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140492.33333333334</c:v>
+                  <c:v>140.49233333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>122090.66666666667</c:v>
+                  <c:v>122.09066666666668</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>144584</c:v>
+                  <c:v>144.584</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>135255.33333333334</c:v>
+                  <c:v>135.25533333333334</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>218541.66666666666</c:v>
+                  <c:v>218.54166666666666</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>163240</c:v>
+                  <c:v>163.24</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>155911</c:v>
+                  <c:v>155.911</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>166238</c:v>
+                  <c:v>166.238</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>159271.66666666666</c:v>
+                  <c:v>159.27166666666665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-232C-407E-B5B4-E4B6B5F1FCF8}"/>
             </c:ext>
@@ -732,11 +737,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="631263200"/>
-        <c:axId val="631239872"/>
+        <c:axId val="-225672496"/>
+        <c:axId val="-225673584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="631263200"/>
+        <c:axId val="-225672496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -779,7 +784,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="631239872"/>
+        <c:crossAx val="-225673584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -787,7 +792,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="631239872"/>
+        <c:axId val="-225673584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -807,7 +812,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -838,7 +843,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="631263200"/>
+        <c:crossAx val="-225672496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -852,6 +857,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -919,7 +925,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -999,43 +1005,43 @@
             <c:numRef>
               <c:f>sphere!$E$5:$E$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>112123</c:v>
+                  <c:v>112.123</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87129.333333333328</c:v>
+                  <c:v>87.129333333333335</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>155576.66666666666</c:v>
+                  <c:v>155.57666666666665</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>164572.33333333334</c:v>
+                  <c:v>164.57233333333335</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>168520.33333333334</c:v>
+                  <c:v>168.52033333333335</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>177025</c:v>
+                  <c:v>177.02500000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>163325</c:v>
+                  <c:v>163.32500000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>177784.33333333334</c:v>
+                  <c:v>177.78433333333334</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>175626.66666666666</c:v>
+                  <c:v>175.62666666666667</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>139633.33333333334</c:v>
+                  <c:v>139.63333333333335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-F513-46A0-B3A6-FA237D53372E}"/>
             </c:ext>
@@ -1066,40 +1072,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>133575</c:v>
+                  <c:v>133.57499999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>118257.66666666667</c:v>
+                  <c:v>118.25766666666668</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>128594.33333333333</c:v>
+                  <c:v>128.59433333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128594.33333333333</c:v>
+                  <c:v>128.59433333333334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>140918</c:v>
+                  <c:v>140.91800000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>143257</c:v>
+                  <c:v>143.25700000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>130918.66666666667</c:v>
+                  <c:v>130.91866666666667</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>152246.33333333334</c:v>
+                  <c:v>152.24633333333335</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>139920.33333333334</c:v>
+                  <c:v>139.92033333333333</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>127929.33333333333</c:v>
+                  <c:v>127.92933333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-F513-46A0-B3A6-FA237D53372E}"/>
             </c:ext>
@@ -1114,11 +1120,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1781671488"/>
-        <c:axId val="1781662752"/>
+        <c:axId val="-225680656"/>
+        <c:axId val="-225684464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1781671488"/>
+        <c:axId val="-225680656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1161,7 +1167,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1781662752"/>
+        <c:crossAx val="-225684464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1169,7 +1175,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1781662752"/>
+        <c:axId val="-225684464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1189,7 +1195,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1220,7 +1226,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1781671488"/>
+        <c:crossAx val="-225680656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1234,6 +1240,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1301,7 +1308,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1381,43 +1388,43 @@
             <c:numRef>
               <c:f>rastrigin!$E$4:$E$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>33701.666666666664</c:v>
+                  <c:v>33.701666666666668</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54657.666666666664</c:v>
+                  <c:v>54.657666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57314.666666666664</c:v>
+                  <c:v>57.314666666666668</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>73317</c:v>
+                  <c:v>73.317000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>78643.333333333328</c:v>
+                  <c:v>78.643333333333331</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89463.666666666672</c:v>
+                  <c:v>89.463666666666668</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>136657</c:v>
+                  <c:v>136.65700000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>155212</c:v>
+                  <c:v>155.21199999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>122655.33333333333</c:v>
+                  <c:v>122.65533333333333</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>188503.66666666666</c:v>
+                  <c:v>188.50366666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C4E8-4CD1-8088-5EC56B161007}"/>
             </c:ext>
@@ -1445,43 +1452,43 @@
             <c:numRef>
               <c:f>rastrigin!$E$20:$E$29</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>134862.66666666666</c:v>
+                  <c:v>134.86266666666666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>125261.66666666667</c:v>
+                  <c:v>125.26166666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>124268.33333333333</c:v>
+                  <c:v>124.26833333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>129181.33333333333</c:v>
+                  <c:v>129.18133333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>122929.33333333333</c:v>
+                  <c:v>122.92933333333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>174567.66666666666</c:v>
+                  <c:v>174.56766666666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>136915.33333333334</c:v>
+                  <c:v>136.91533333333334</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>131591.33333333334</c:v>
+                  <c:v>131.59133333333335</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>130311</c:v>
+                  <c:v>130.31100000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>131501</c:v>
+                  <c:v>131.501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C4E8-4CD1-8088-5EC56B161007}"/>
             </c:ext>
@@ -1496,16 +1503,77 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="472434272"/>
-        <c:axId val="472435104"/>
+        <c:axId val="-225671952"/>
+        <c:axId val="-225682288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="472434272"/>
+        <c:axId val="-225671952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> of dimensions</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1543,7 +1611,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472435104"/>
+        <c:crossAx val="-225682288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1551,27 +1619,74 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="472435104"/>
+        <c:axId val="-225682288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1602,7 +1717,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472434272"/>
+        <c:crossAx val="-225671952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1614,6 +1729,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1652,7 +1799,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1732,43 +1879,43 @@
             <c:numRef>
               <c:f>rastrigin!$K$4:$K$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>104399.33333333333</c:v>
+                  <c:v>104.39933333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140015.33333333334</c:v>
+                  <c:v>140.01533333333336</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>191367.33333333334</c:v>
+                  <c:v>191.36733333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>243375.66666666666</c:v>
+                  <c:v>243.37566666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>327276.33333333331</c:v>
+                  <c:v>327.2763333333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>389049.66666666669</c:v>
+                  <c:v>389.04966666666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>479518</c:v>
+                  <c:v>479.51800000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>491636.66666666669</c:v>
+                  <c:v>491.63666666666671</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>525924.66666666663</c:v>
+                  <c:v>525.92466666666667</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>620588.66666666663</c:v>
+                  <c:v>620.58866666666665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FD71-45DE-A95F-3F39F3CB0F11}"/>
             </c:ext>
@@ -1796,43 +1943,43 @@
             <c:numRef>
               <c:f>rastrigin!$K$20:$K$29</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>234391</c:v>
+                  <c:v>234.39099999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>424889.66666666669</c:v>
+                  <c:v>424.8896666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>611086.66666666663</c:v>
+                  <c:v>611.08666666666659</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>805378</c:v>
+                  <c:v>805.37800000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>434236.33333333331</c:v>
+                  <c:v>434.23633333333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1226032.3333333333</c:v>
+                  <c:v>1226.0323333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1360642.6666666667</c:v>
+                  <c:v>1360.6426666666669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1547532</c:v>
+                  <c:v>1547.5319999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1753845.3333333333</c:v>
+                  <c:v>1753.8453333333332</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1956096.3333333333</c:v>
+                  <c:v>1956.0963333333334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FD71-45DE-A95F-3F39F3CB0F11}"/>
             </c:ext>
@@ -1847,16 +1994,77 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="136844063"/>
-        <c:axId val="136848223"/>
+        <c:axId val="-225674672"/>
+        <c:axId val="-225670320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="136844063"/>
+        <c:axId val="-225674672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> of Iterations</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1894,7 +2102,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136848223"/>
+        <c:crossAx val="-225670320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1902,27 +2110,74 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136848223"/>
+        <c:axId val="-225670320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1953,7 +2208,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136844063"/>
+        <c:crossAx val="-225674672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1965,6 +2220,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2003,7 +2290,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2083,43 +2370,43 @@
             <c:numRef>
               <c:f>rastrigin!$Q$4:$Q$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>78646.666666666672</c:v>
+                  <c:v>78.646666666666675</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>102643</c:v>
+                  <c:v>102.643</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>198425.66666666666</c:v>
+                  <c:v>198.42566666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>181669.66666666666</c:v>
+                  <c:v>181.66966666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>207211</c:v>
+                  <c:v>207.21100000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>266269.66666666669</c:v>
+                  <c:v>266.26966666666669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>290542.66666666669</c:v>
+                  <c:v>290.54266666666672</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>367343.66666666669</c:v>
+                  <c:v>367.34366666666671</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>218983.66666666666</c:v>
+                  <c:v>218.98366666666666</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>185053.33333333334</c:v>
+                  <c:v>185.05333333333334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-283A-41CF-863C-842CB246F13C}"/>
             </c:ext>
@@ -2147,43 +2434,43 @@
             <c:numRef>
               <c:f>rastrigin!$Q$20:$Q$29</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>272114.66666666669</c:v>
+                  <c:v>272.11466666666666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>116752</c:v>
+                  <c:v>116.752</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>114156.33333333333</c:v>
+                  <c:v>114.15633333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110660</c:v>
+                  <c:v>110.66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>124141.66666666667</c:v>
+                  <c:v>124.14166666666668</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>117139.66666666667</c:v>
+                  <c:v>117.13966666666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>126302.33333333333</c:v>
+                  <c:v>126.30233333333334</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>138922</c:v>
+                  <c:v>138.922</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>128258.33333333333</c:v>
+                  <c:v>128.25833333333333</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>136706.33333333334</c:v>
+                  <c:v>136.70633333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-283A-41CF-863C-842CB246F13C}"/>
             </c:ext>
@@ -2198,16 +2485,77 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1749584687"/>
-        <c:axId val="1749590095"/>
+        <c:axId val="-225674128"/>
+        <c:axId val="-77673552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1749584687"/>
+        <c:axId val="-225674128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Numbe</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t>r of Particles</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2245,7 +2593,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1749590095"/>
+        <c:crossAx val="-77673552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2253,27 +2601,74 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1749590095"/>
+        <c:axId val="-77673552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> (s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2304,7 +2699,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1749584687"/>
+        <c:crossAx val="-225674128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2316,6 +2711,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -5789,15 +6216,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5818,16 +6245,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5848,15 +6275,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6144,8 +6571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="K48" sqref="K48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6156,42 +6583,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="H3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="N3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="H3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="N3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -6207,10 +6634,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
         <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
       </c>
       <c r="H4" t="s">
         <v>0</v>
@@ -6222,10 +6649,10 @@
         <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="M4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N4" t="s">
         <v>0</v>
@@ -6237,7 +6664,7 @@
         <v>3</v>
       </c>
       <c r="Q4" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -6253,9 +6680,9 @@
       <c r="D5">
         <v>30456</v>
       </c>
-      <c r="E5">
-        <f>AVERAGE(B5:D5)</f>
-        <v>112123</v>
+      <c r="E5" s="2">
+        <f>AVERAGE(B5:D5)*0.001</f>
+        <v>112.123</v>
       </c>
       <c r="G5">
         <v>100</v>
@@ -6269,9 +6696,9 @@
       <c r="J5">
         <v>64562</v>
       </c>
-      <c r="K5">
-        <f>AVERAGE(H5:J5)</f>
-        <v>117511.33333333333</v>
+      <c r="K5" s="2">
+        <f>AVERAGE(H5:J5)*0.001</f>
+        <v>117.51133333333333</v>
       </c>
       <c r="M5">
         <v>10</v>
@@ -6285,9 +6712,9 @@
       <c r="P5">
         <v>19990</v>
       </c>
-      <c r="Q5">
-        <f>AVERAGE(N5:P5)</f>
-        <v>23992.333333333332</v>
+      <c r="Q5" s="2">
+        <f>AVERAGE(N5:P5)*0.001</f>
+        <v>23.992333333333331</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -6303,9 +6730,9 @@
       <c r="D6">
         <v>43991</v>
       </c>
-      <c r="E6">
-        <f t="shared" ref="E6:E14" si="0">AVERAGE(B6:D6)</f>
-        <v>87129.333333333328</v>
+      <c r="E6" s="2">
+        <f t="shared" ref="E6:E14" si="0">AVERAGE(B6:D6)*0.001</f>
+        <v>87.129333333333335</v>
       </c>
       <c r="G6">
         <v>200</v>
@@ -6319,9 +6746,9 @@
       <c r="J6">
         <v>299936</v>
       </c>
-      <c r="K6">
-        <f t="shared" ref="K6:K14" si="1">AVERAGE(H6:J6)</f>
-        <v>288097.66666666669</v>
+      <c r="K6" s="2">
+        <f t="shared" ref="K6:K14" si="1">AVERAGE(H6:J6)*0.001</f>
+        <v>288.09766666666667</v>
       </c>
       <c r="M6">
         <v>20</v>
@@ -6335,9 +6762,9 @@
       <c r="P6">
         <v>39991</v>
       </c>
-      <c r="Q6">
-        <f t="shared" ref="Q6:Q14" si="2">AVERAGE(N6:P6)</f>
-        <v>45418</v>
+      <c r="Q6" s="2">
+        <f t="shared" ref="Q6:Q14" si="2">AVERAGE(N6:P6)*0.001</f>
+        <v>45.417999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -6353,9 +6780,9 @@
       <c r="D7">
         <v>60002</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>155576.66666666666</v>
+        <v>155.57666666666665</v>
       </c>
       <c r="G7">
         <v>300</v>
@@ -6369,9 +6796,9 @@
       <c r="J7">
         <v>367506</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="2">
         <f t="shared" si="1"/>
-        <v>355190.33333333331</v>
+        <v>355.19033333333334</v>
       </c>
       <c r="M7">
         <v>30</v>
@@ -6385,9 +6812,9 @@
       <c r="P7">
         <v>99993</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="2">
         <f t="shared" si="2"/>
-        <v>93180.666666666672</v>
+        <v>93.180666666666667</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -6403,9 +6830,9 @@
       <c r="D8">
         <v>63984</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>164572.33333333334</v>
+        <v>164.57233333333335</v>
       </c>
       <c r="G8">
         <v>400</v>
@@ -6419,9 +6846,9 @@
       <c r="J8">
         <v>374083</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="2">
         <f t="shared" si="1"/>
-        <v>387130.66666666669</v>
+        <v>387.13066666666668</v>
       </c>
       <c r="M8">
         <v>40</v>
@@ -6435,9 +6862,9 @@
       <c r="P8">
         <v>73560</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="2">
         <f t="shared" si="2"/>
-        <v>113995</v>
+        <v>113.995</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -6453,9 +6880,9 @@
       <c r="D9">
         <v>83957</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>168520.33333333334</v>
+        <v>168.52033333333335</v>
       </c>
       <c r="G9">
         <v>500</v>
@@ -6469,9 +6896,9 @@
       <c r="J9">
         <v>374086</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="2">
         <f t="shared" si="1"/>
-        <v>386874.33333333331</v>
+        <v>386.87433333333331</v>
       </c>
       <c r="M9">
         <v>50</v>
@@ -6485,9 +6912,9 @@
       <c r="P9">
         <v>68006</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="2">
         <f t="shared" si="2"/>
-        <v>95912</v>
+        <v>95.912000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -6503,9 +6930,9 @@
       <c r="D10">
         <v>84001</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>177025</v>
+        <v>177.02500000000001</v>
       </c>
       <c r="G10">
         <v>600</v>
@@ -6519,9 +6946,9 @@
       <c r="J10">
         <v>475145</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="2">
         <f t="shared" si="1"/>
-        <v>488589.66666666669</v>
+        <v>488.58966666666669</v>
       </c>
       <c r="M10">
         <v>60</v>
@@ -6535,9 +6962,9 @@
       <c r="P10">
         <v>79657</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="2">
         <f t="shared" si="2"/>
-        <v>85162.666666666672</v>
+        <v>85.162666666666667</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -6553,9 +6980,9 @@
       <c r="D11">
         <v>87993</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>163325</v>
+        <v>163.32500000000002</v>
       </c>
       <c r="G11">
         <v>700</v>
@@ -6569,9 +6996,9 @@
       <c r="J11">
         <v>762988</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="2">
         <f t="shared" si="1"/>
-        <v>807372</v>
+        <v>807.37200000000007</v>
       </c>
       <c r="M11">
         <v>70</v>
@@ -6585,9 +7012,9 @@
       <c r="P11">
         <v>103533</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="2">
         <f t="shared" si="2"/>
-        <v>114931</v>
+        <v>114.931</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -6603,9 +7030,9 @@
       <c r="D12">
         <v>113674</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>177784.33333333334</v>
+        <v>177.78433333333334</v>
       </c>
       <c r="G12">
         <v>800</v>
@@ -6619,9 +7046,9 @@
       <c r="J12">
         <v>1165094</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="2">
         <f t="shared" si="1"/>
-        <v>1369390</v>
+        <v>1369.39</v>
       </c>
       <c r="M12">
         <v>80</v>
@@ -6635,9 +7062,9 @@
       <c r="P12">
         <v>111951</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="2">
         <f t="shared" si="2"/>
-        <v>168129</v>
+        <v>168.12899999999999</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -6653,9 +7080,9 @@
       <c r="D13">
         <v>143337</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>175626.66666666666</v>
+        <v>175.62666666666667</v>
       </c>
       <c r="G13">
         <v>900</v>
@@ -6669,9 +7096,9 @@
       <c r="J13">
         <v>1476125</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="2">
         <f t="shared" si="1"/>
-        <v>1297286.3333333333</v>
+        <v>1297.2863333333332</v>
       </c>
       <c r="M13">
         <v>90</v>
@@ -6685,9 +7112,9 @@
       <c r="P13">
         <v>120163</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="2">
         <f t="shared" si="2"/>
-        <v>139852.33333333334</v>
+        <v>139.85233333333335</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -6703,9 +7130,9 @@
       <c r="D14">
         <v>144410</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>139633.33333333334</v>
+        <v>139.63333333333335</v>
       </c>
       <c r="G14">
         <v>1000</v>
@@ -6719,9 +7146,9 @@
       <c r="J14">
         <v>1372999</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="2">
         <f t="shared" si="1"/>
-        <v>1386414</v>
+        <v>1386.414</v>
       </c>
       <c r="M14">
         <v>100</v>
@@ -6735,48 +7162,48 @@
       <c r="P14">
         <v>147269</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="2">
         <f t="shared" si="2"/>
-        <v>191386.66666666666</v>
+        <v>191.38666666666666</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
+      <c r="A17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="H19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="N19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
+      <c r="B19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="H19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="N19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -6792,10 +7219,10 @@
         <v>3</v>
       </c>
       <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" t="s">
         <v>4</v>
-      </c>
-      <c r="G20" t="s">
-        <v>5</v>
       </c>
       <c r="H20" t="s">
         <v>0</v>
@@ -6807,10 +7234,10 @@
         <v>3</v>
       </c>
       <c r="K20" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="M20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N20" t="s">
         <v>0</v>
@@ -6822,7 +7249,7 @@
         <v>3</v>
       </c>
       <c r="Q20" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -6839,8 +7266,8 @@
         <v>113889</v>
       </c>
       <c r="E21">
-        <f>AVERAGE(B21:D21)</f>
-        <v>133575</v>
+        <f>AVERAGE(B21:D21)*0.001</f>
+        <v>133.57499999999999</v>
       </c>
       <c r="G21">
         <v>100</v>
@@ -6855,8 +7282,8 @@
         <v>288194</v>
       </c>
       <c r="K21">
-        <f>AVERAGE(H21:J21)</f>
-        <v>303475.66666666669</v>
+        <f>AVERAGE(H21:J21)*0.001</f>
+        <v>303.47566666666671</v>
       </c>
       <c r="M21">
         <v>10</v>
@@ -6871,8 +7298,8 @@
         <v>450085</v>
       </c>
       <c r="Q21">
-        <f>AVERAGE(N21:P21)</f>
-        <v>362141</v>
+        <f>AVERAGE(N21:P21)*0.001</f>
+        <v>362.14100000000002</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -6889,8 +7316,8 @@
         <v>111913</v>
       </c>
       <c r="E22">
-        <f t="shared" ref="E22:E30" si="3">AVERAGE(B22:D22)</f>
-        <v>118257.66666666667</v>
+        <f t="shared" ref="E22:E30" si="3">AVERAGE(B22:D22)*0.001</f>
+        <v>118.25766666666668</v>
       </c>
       <c r="G22">
         <v>200</v>
@@ -6905,8 +7332,8 @@
         <v>512353</v>
       </c>
       <c r="K22">
-        <f t="shared" ref="K22:K30" si="4">AVERAGE(H22:J22)</f>
-        <v>511795.66666666669</v>
+        <f t="shared" ref="K22:K30" si="4">AVERAGE(H22:J22)*0.001</f>
+        <v>511.7956666666667</v>
       </c>
       <c r="M22">
         <v>20</v>
@@ -6921,8 +7348,8 @@
         <v>155918</v>
       </c>
       <c r="Q22">
-        <f t="shared" ref="Q22:Q30" si="5">AVERAGE(N22:P22)</f>
-        <v>140492.33333333334</v>
+        <f t="shared" ref="Q22:Q30" si="5">AVERAGE(N22:P22)*0.001</f>
+        <v>140.49233333333333</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -6940,7 +7367,7 @@
       </c>
       <c r="E23">
         <f t="shared" si="3"/>
-        <v>128594.33333333333</v>
+        <v>128.59433333333334</v>
       </c>
       <c r="G23">
         <v>300</v>
@@ -6956,7 +7383,7 @@
       </c>
       <c r="K23">
         <f t="shared" si="4"/>
-        <v>710549.33333333337</v>
+        <v>710.54933333333338</v>
       </c>
       <c r="M23">
         <v>30</v>
@@ -6972,7 +7399,7 @@
       </c>
       <c r="Q23">
         <f t="shared" si="5"/>
-        <v>122090.66666666667</v>
+        <v>122.09066666666668</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -6990,7 +7417,7 @@
       </c>
       <c r="E24">
         <f t="shared" si="3"/>
-        <v>128594.33333333333</v>
+        <v>128.59433333333334</v>
       </c>
       <c r="G24">
         <v>400</v>
@@ -7006,7 +7433,7 @@
       </c>
       <c r="K24">
         <f t="shared" si="4"/>
-        <v>826788</v>
+        <v>826.78800000000001</v>
       </c>
       <c r="M24">
         <v>40</v>
@@ -7022,7 +7449,7 @@
       </c>
       <c r="Q24">
         <f t="shared" si="5"/>
-        <v>144584</v>
+        <v>144.584</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -7040,7 +7467,7 @@
       </c>
       <c r="E25">
         <f t="shared" si="3"/>
-        <v>140918</v>
+        <v>140.91800000000001</v>
       </c>
       <c r="G25">
         <v>500</v>
@@ -7056,7 +7483,7 @@
       </c>
       <c r="K25">
         <f t="shared" si="4"/>
-        <v>752781</v>
+        <v>752.78100000000006</v>
       </c>
       <c r="M25">
         <v>50</v>
@@ -7072,7 +7499,7 @@
       </c>
       <c r="Q25">
         <f t="shared" si="5"/>
-        <v>135255.33333333334</v>
+        <v>135.25533333333334</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -7090,7 +7517,7 @@
       </c>
       <c r="E26">
         <f t="shared" si="3"/>
-        <v>143257</v>
+        <v>143.25700000000001</v>
       </c>
       <c r="G26">
         <v>600</v>
@@ -7106,7 +7533,7 @@
       </c>
       <c r="K26">
         <f t="shared" si="4"/>
-        <v>1212891.3333333333</v>
+        <v>1212.8913333333333</v>
       </c>
       <c r="M26">
         <v>60</v>
@@ -7122,7 +7549,7 @@
       </c>
       <c r="Q26">
         <f t="shared" si="5"/>
-        <v>218541.66666666666</v>
+        <v>218.54166666666666</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -7140,7 +7567,7 @@
       </c>
       <c r="E27">
         <f t="shared" si="3"/>
-        <v>130918.66666666667</v>
+        <v>130.91866666666667</v>
       </c>
       <c r="G27">
         <v>700</v>
@@ -7156,7 +7583,7 @@
       </c>
       <c r="K27">
         <f t="shared" si="4"/>
-        <v>1559120</v>
+        <v>1559.1200000000001</v>
       </c>
       <c r="M27">
         <v>70</v>
@@ -7172,7 +7599,7 @@
       </c>
       <c r="Q27">
         <f t="shared" si="5"/>
-        <v>163240</v>
+        <v>163.24</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -7190,7 +7617,7 @@
       </c>
       <c r="E28">
         <f t="shared" si="3"/>
-        <v>152246.33333333334</v>
+        <v>152.24633333333335</v>
       </c>
       <c r="G28">
         <v>800</v>
@@ -7206,7 +7633,7 @@
       </c>
       <c r="K28">
         <f t="shared" si="4"/>
-        <v>1650092.6666666667</v>
+        <v>1650.0926666666667</v>
       </c>
       <c r="M28">
         <v>80</v>
@@ -7222,7 +7649,7 @@
       </c>
       <c r="Q28">
         <f t="shared" si="5"/>
-        <v>155911</v>
+        <v>155.911</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -7240,7 +7667,7 @@
       </c>
       <c r="E29">
         <f t="shared" si="3"/>
-        <v>139920.33333333334</v>
+        <v>139.92033333333333</v>
       </c>
       <c r="G29">
         <v>900</v>
@@ -7256,7 +7683,7 @@
       </c>
       <c r="K29">
         <f t="shared" si="4"/>
-        <v>1780338.3333333333</v>
+        <v>1780.3383333333334</v>
       </c>
       <c r="M29">
         <v>90</v>
@@ -7272,7 +7699,7 @@
       </c>
       <c r="Q29">
         <f t="shared" si="5"/>
-        <v>166238</v>
+        <v>166.238</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -7290,7 +7717,7 @@
       </c>
       <c r="E30">
         <f t="shared" si="3"/>
-        <v>127929.33333333333</v>
+        <v>127.92933333333333</v>
       </c>
       <c r="G30">
         <v>1000</v>
@@ -7306,7 +7733,7 @@
       </c>
       <c r="K30">
         <f t="shared" si="4"/>
-        <v>1469181</v>
+        <v>1469.181</v>
       </c>
       <c r="M30">
         <v>100</v>
@@ -7322,18 +7749,18 @@
       </c>
       <c r="Q30">
         <f t="shared" si="5"/>
-        <v>159271.66666666666</v>
+        <v>159.27166666666665</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -7348,7 +7775,8 @@
     <mergeCell ref="H3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7356,13 +7784,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
-      <selection activeCell="N48" sqref="N48"/>
+    <sheetView topLeftCell="F22" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.140625" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
@@ -7370,42 +7799,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="H2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="H2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="N2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="N2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -7421,10 +7850,10 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
         <v>0</v>
@@ -7436,10 +7865,10 @@
         <v>3</v>
       </c>
       <c r="K3" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="M3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N3" t="s">
         <v>0</v>
@@ -7451,7 +7880,7 @@
         <v>3</v>
       </c>
       <c r="Q3" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -7467,9 +7896,9 @@
       <c r="D4">
         <v>32460</v>
       </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E13" si="0">AVERAGE(B4:D4)</f>
-        <v>33701.666666666664</v>
+      <c r="E4" s="2">
+        <f>AVERAGE(B4:D4) * 0.001</f>
+        <v>33.701666666666668</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -7483,9 +7912,9 @@
       <c r="J4">
         <v>68003</v>
       </c>
-      <c r="K4">
-        <f t="shared" ref="K4:K13" si="1">AVERAGE(H4:J4)</f>
-        <v>104399.33333333333</v>
+      <c r="K4" s="2">
+        <f>AVERAGE(H4:J4)*0.001</f>
+        <v>104.39933333333333</v>
       </c>
       <c r="M4">
         <v>10</v>
@@ -7499,9 +7928,9 @@
       <c r="P4">
         <v>35991</v>
       </c>
-      <c r="Q4">
-        <f>AVERAGE(N4:P4)</f>
-        <v>78646.666666666672</v>
+      <c r="Q4" s="2">
+        <f>AVERAGE(N4:P4)*0.001</f>
+        <v>78.646666666666675</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -7517,9 +7946,9 @@
       <c r="D5">
         <v>52003</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>54657.666666666664</v>
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:E13" si="0">AVERAGE(B5:D5) * 0.001</f>
+        <v>54.657666666666664</v>
       </c>
       <c r="G5">
         <v>200</v>
@@ -7533,9 +7962,9 @@
       <c r="J5">
         <v>123971</v>
       </c>
-      <c r="K5">
-        <f t="shared" si="1"/>
-        <v>140015.33333333334</v>
+      <c r="K5" s="2">
+        <f t="shared" ref="K5:K13" si="1">AVERAGE(H5:J5)*0.001</f>
+        <v>140.01533333333336</v>
       </c>
       <c r="M5">
         <v>20</v>
@@ -7549,9 +7978,9 @@
       <c r="P5">
         <v>43989</v>
       </c>
-      <c r="Q5">
-        <f t="shared" ref="Q5:Q13" si="2">AVERAGE(N5:P5)</f>
-        <v>102643</v>
+      <c r="Q5" s="2">
+        <f t="shared" ref="Q5:Q13" si="2">AVERAGE(N5:P5)*0.001</f>
+        <v>102.643</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -7567,9 +7996,9 @@
       <c r="D6">
         <v>55970</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>57314.666666666664</v>
+        <v>57.314666666666668</v>
       </c>
       <c r="G6">
         <v>300</v>
@@ -7583,9 +8012,9 @@
       <c r="J6">
         <v>191931</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="2">
         <f t="shared" si="1"/>
-        <v>191367.33333333334</v>
+        <v>191.36733333333333</v>
       </c>
       <c r="M6">
         <v>30</v>
@@ -7599,9 +8028,9 @@
       <c r="P6">
         <v>79987</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="2">
         <f t="shared" si="2"/>
-        <v>198425.66666666666</v>
+        <v>198.42566666666667</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -7617,9 +8046,9 @@
       <c r="D7">
         <v>71991</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>73317</v>
+        <v>73.317000000000007</v>
       </c>
       <c r="G7">
         <v>400</v>
@@ -7633,9 +8062,9 @@
       <c r="J7">
         <v>257926</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="2">
         <f t="shared" si="1"/>
-        <v>243375.66666666666</v>
+        <v>243.37566666666666</v>
       </c>
       <c r="M7">
         <v>40</v>
@@ -7649,9 +8078,9 @@
       <c r="P7">
         <v>111984</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="2">
         <f t="shared" si="2"/>
-        <v>181669.66666666666</v>
+        <v>181.66966666666667</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -7667,9 +8096,9 @@
       <c r="D8">
         <v>75968</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>78643.333333333328</v>
+        <v>78.643333333333331</v>
       </c>
       <c r="G8">
         <v>500</v>
@@ -7683,9 +8112,9 @@
       <c r="J8">
         <v>280133</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="2">
         <f t="shared" si="1"/>
-        <v>327276.33333333331</v>
+        <v>327.2763333333333</v>
       </c>
       <c r="M8">
         <v>50</v>
@@ -7699,9 +8128,9 @@
       <c r="P8">
         <v>75960</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="2">
         <f t="shared" si="2"/>
-        <v>207211</v>
+        <v>207.21100000000001</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -7717,9 +8146,9 @@
       <c r="D9">
         <v>91976</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>89463.666666666672</v>
+        <v>89.463666666666668</v>
       </c>
       <c r="G9">
         <v>600</v>
@@ -7733,9 +8162,9 @@
       <c r="J9">
         <v>393083</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="2">
         <f t="shared" si="1"/>
-        <v>389049.66666666669</v>
+        <v>389.04966666666667</v>
       </c>
       <c r="M9">
         <v>60</v>
@@ -7749,9 +8178,9 @@
       <c r="P9">
         <v>91308</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="2">
         <f t="shared" si="2"/>
-        <v>266269.66666666669</v>
+        <v>266.26966666666669</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -7767,9 +8196,9 @@
       <c r="D10">
         <v>95668</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <f t="shared" si="0"/>
-        <v>136657</v>
+        <v>136.65700000000001</v>
       </c>
       <c r="G10">
         <v>700</v>
@@ -7783,9 +8212,9 @@
       <c r="J10">
         <v>590979</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="2">
         <f t="shared" si="1"/>
-        <v>479518</v>
+        <v>479.51800000000003</v>
       </c>
       <c r="M10">
         <v>70</v>
@@ -7799,9 +8228,9 @@
       <c r="P10">
         <v>131840</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="2">
         <f t="shared" si="2"/>
-        <v>290542.66666666669</v>
+        <v>290.54266666666672</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -7817,9 +8246,9 @@
       <c r="D11">
         <v>112003</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>155212</v>
+        <v>155.21199999999999</v>
       </c>
       <c r="G11">
         <v>800</v>
@@ -7833,9 +8262,9 @@
       <c r="J11">
         <v>538110</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="2">
         <f t="shared" si="1"/>
-        <v>491636.66666666669</v>
+        <v>491.63666666666671</v>
       </c>
       <c r="M11">
         <v>80</v>
@@ -7849,9 +8278,9 @@
       <c r="P11">
         <v>146558</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="2">
         <f t="shared" si="2"/>
-        <v>367343.66666666669</v>
+        <v>367.34366666666671</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -7867,9 +8296,9 @@
       <c r="D12">
         <v>151852</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <f t="shared" si="0"/>
-        <v>122655.33333333333</v>
+        <v>122.65533333333333</v>
       </c>
       <c r="G12">
         <v>900</v>
@@ -7883,9 +8312,9 @@
       <c r="J12">
         <v>496562</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="2">
         <f t="shared" si="1"/>
-        <v>525924.66666666663</v>
+        <v>525.92466666666667</v>
       </c>
       <c r="M12">
         <v>90</v>
@@ -7899,9 +8328,9 @@
       <c r="P12">
         <v>135967</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="2">
         <f t="shared" si="2"/>
-        <v>218983.66666666666</v>
+        <v>218.98366666666666</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -7917,9 +8346,9 @@
       <c r="D13">
         <v>230884</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>188503.66666666666</v>
+        <v>188.50366666666667</v>
       </c>
       <c r="G13">
         <v>1000</v>
@@ -7933,9 +8362,9 @@
       <c r="J13">
         <v>594362</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="2">
         <f t="shared" si="1"/>
-        <v>620588.66666666663</v>
+        <v>620.58866666666665</v>
       </c>
       <c r="M13">
         <v>100</v>
@@ -7949,48 +8378,48 @@
       <c r="P13">
         <v>151941</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="2">
         <f t="shared" si="2"/>
-        <v>185053.33333333334</v>
+        <v>185.05333333333334</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
+      <c r="A16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="H18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="H18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="N18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="N18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -8006,10 +8435,10 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H19" t="s">
         <v>0</v>
@@ -8021,10 +8450,10 @@
         <v>3</v>
       </c>
       <c r="K19" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="M19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N19" t="s">
         <v>0</v>
@@ -8036,7 +8465,7 @@
         <v>3</v>
       </c>
       <c r="Q19" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -8052,9 +8481,9 @@
       <c r="D20">
         <v>125751</v>
       </c>
-      <c r="E20">
-        <f t="shared" ref="E20:E29" si="3">AVERAGE(B20:D20)</f>
-        <v>134862.66666666666</v>
+      <c r="E20" s="2">
+        <f>AVERAGE(B20:D20)*0.001</f>
+        <v>134.86266666666666</v>
       </c>
       <c r="G20">
         <v>100</v>
@@ -8068,9 +8497,9 @@
       <c r="J20">
         <v>233865</v>
       </c>
-      <c r="K20">
-        <f t="shared" ref="K20:K29" si="4">AVERAGE(H20:J20)</f>
-        <v>234391</v>
+      <c r="K20" s="2">
+        <f>AVERAGE(H20:J20)*0.001</f>
+        <v>234.39099999999999</v>
       </c>
       <c r="M20">
         <v>10</v>
@@ -8084,9 +8513,9 @@
       <c r="P20">
         <v>254674</v>
       </c>
-      <c r="Q20">
-        <f t="shared" ref="Q20:Q29" si="5">AVERAGE(N20:P20)</f>
-        <v>272114.66666666669</v>
+      <c r="Q20" s="2">
+        <f>AVERAGE(N20:P20)*0.001</f>
+        <v>272.11466666666666</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -8102,9 +8531,9 @@
       <c r="D21">
         <v>132925</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="3"/>
-        <v>125261.66666666667</v>
+      <c r="E21" s="2">
+        <f t="shared" ref="E21:E29" si="3">AVERAGE(B21:D21)*0.001</f>
+        <v>125.26166666666667</v>
       </c>
       <c r="G21">
         <v>200</v>
@@ -8118,9 +8547,9 @@
       <c r="J21">
         <v>423914</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="4"/>
-        <v>424889.66666666669</v>
+      <c r="K21" s="2">
+        <f t="shared" ref="K21:K29" si="4">AVERAGE(H21:J21)*0.001</f>
+        <v>424.8896666666667</v>
       </c>
       <c r="M21">
         <v>20</v>
@@ -8134,9 +8563,9 @@
       <c r="P21">
         <v>115723</v>
       </c>
-      <c r="Q21">
-        <f t="shared" si="5"/>
-        <v>116752</v>
+      <c r="Q21" s="2">
+        <f t="shared" ref="Q21:Q29" si="5">AVERAGE(N21:P21)*0.001</f>
+        <v>116.752</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -8152,9 +8581,9 @@
       <c r="D22">
         <v>122929</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <f t="shared" si="3"/>
-        <v>124268.33333333333</v>
+        <v>124.26833333333333</v>
       </c>
       <c r="G22">
         <v>300</v>
@@ -8168,9 +8597,9 @@
       <c r="J22">
         <v>613485</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="2">
         <f t="shared" si="4"/>
-        <v>611086.66666666663</v>
+        <v>611.08666666666659</v>
       </c>
       <c r="M22">
         <v>30</v>
@@ -8184,9 +8613,9 @@
       <c r="P22">
         <v>111935</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="2">
         <f t="shared" si="5"/>
-        <v>114156.33333333333</v>
+        <v>114.15633333333334</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -8202,9 +8631,9 @@
       <c r="D23">
         <v>124692</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <f t="shared" si="3"/>
-        <v>129181.33333333333</v>
+        <v>129.18133333333333</v>
       </c>
       <c r="G23">
         <v>400</v>
@@ -8218,9 +8647,9 @@
       <c r="J23">
         <v>812709</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="2">
         <f t="shared" si="4"/>
-        <v>805378</v>
+        <v>805.37800000000004</v>
       </c>
       <c r="M23">
         <v>40</v>
@@ -8234,9 +8663,9 @@
       <c r="P23">
         <v>112157</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="2">
         <f t="shared" si="5"/>
-        <v>110660</v>
+        <v>110.66</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -8252,9 +8681,9 @@
       <c r="D24">
         <v>117933</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <f t="shared" si="3"/>
-        <v>122929.33333333333</v>
+        <v>122.92933333333333</v>
       </c>
       <c r="G24">
         <v>500</v>
@@ -8268,9 +8697,9 @@
       <c r="J24">
         <v>131466</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="2">
         <f t="shared" si="4"/>
-        <v>434236.33333333331</v>
+        <v>434.23633333333333</v>
       </c>
       <c r="M24">
         <v>50</v>
@@ -8284,9 +8713,9 @@
       <c r="P24">
         <v>129926</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="2">
         <f t="shared" si="5"/>
-        <v>124141.66666666667</v>
+        <v>124.14166666666668</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -8302,9 +8731,9 @@
       <c r="D25">
         <v>151912</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <f t="shared" si="3"/>
-        <v>174567.66666666666</v>
+        <v>174.56766666666667</v>
       </c>
       <c r="G25">
         <v>600</v>
@@ -8318,9 +8747,9 @@
       <c r="J25">
         <v>1263482</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="2">
         <f t="shared" si="4"/>
-        <v>1226032.3333333333</v>
+        <v>1226.0323333333333</v>
       </c>
       <c r="M25">
         <v>60</v>
@@ -8334,9 +8763,9 @@
       <c r="P25">
         <v>112866</v>
       </c>
-      <c r="Q25">
+      <c r="Q25" s="2">
         <f t="shared" si="5"/>
-        <v>117139.66666666667</v>
+        <v>117.13966666666667</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -8352,9 +8781,9 @@
       <c r="D26">
         <v>131925</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <f t="shared" si="3"/>
-        <v>136915.33333333334</v>
+        <v>136.91533333333334</v>
       </c>
       <c r="G26">
         <v>700</v>
@@ -8368,9 +8797,9 @@
       <c r="J26">
         <v>1374165</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="2">
         <f t="shared" si="4"/>
-        <v>1360642.6666666667</v>
+        <v>1360.6426666666669</v>
       </c>
       <c r="M26">
         <v>70</v>
@@ -8384,9 +8813,9 @@
       <c r="P26">
         <v>114935</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="2">
         <f t="shared" si="5"/>
-        <v>126302.33333333333</v>
+        <v>126.30233333333334</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -8402,9 +8831,9 @@
       <c r="D27">
         <v>118932</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <f t="shared" si="3"/>
-        <v>131591.33333333334</v>
+        <v>131.59133333333335</v>
       </c>
       <c r="G27">
         <v>800</v>
@@ -8418,9 +8847,9 @@
       <c r="J27">
         <v>1535428</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="2">
         <f t="shared" si="4"/>
-        <v>1547532</v>
+        <v>1547.5319999999999</v>
       </c>
       <c r="M27">
         <v>80</v>
@@ -8434,9 +8863,9 @@
       <c r="P27">
         <v>149917</v>
       </c>
-      <c r="Q27">
+      <c r="Q27" s="2">
         <f t="shared" si="5"/>
-        <v>138922</v>
+        <v>138.922</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -8452,9 +8881,9 @@
       <c r="D28">
         <v>147916</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <f t="shared" si="3"/>
-        <v>130311</v>
+        <v>130.31100000000001</v>
       </c>
       <c r="G28">
         <v>900</v>
@@ -8468,9 +8897,9 @@
       <c r="J28">
         <v>1728210</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="2">
         <f t="shared" si="4"/>
-        <v>1753845.3333333333</v>
+        <v>1753.8453333333332</v>
       </c>
       <c r="M28">
         <v>90</v>
@@ -8484,9 +8913,9 @@
       <c r="P28">
         <v>116931</v>
       </c>
-      <c r="Q28">
+      <c r="Q28" s="2">
         <f t="shared" si="5"/>
-        <v>128258.33333333333</v>
+        <v>128.25833333333333</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -8502,9 +8931,9 @@
       <c r="D29">
         <v>122932</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
         <f t="shared" si="3"/>
-        <v>131501</v>
+        <v>131.501</v>
       </c>
       <c r="G29">
         <v>1000</v>
@@ -8518,9 +8947,9 @@
       <c r="J29">
         <v>1944963</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="2">
         <f t="shared" si="4"/>
-        <v>1956096.3333333333</v>
+        <v>1956.0963333333334</v>
       </c>
       <c r="M29">
         <v>100</v>
@@ -8534,9 +8963,9 @@
       <c r="P29">
         <v>137922</v>
       </c>
-      <c r="Q29">
+      <c r="Q29" s="2">
         <f t="shared" si="5"/>
-        <v>136706.33333333334</v>
+        <v>136.70633333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comparison of runtime via graphs added in report
</commit_message>
<xml_diff>
--- a/Documentation/Graphs.xlsx
+++ b/Documentation/Graphs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shalin\Desktop\project-pyteam\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\dsa project\project-pyteam\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="sphere" sheetId="1" r:id="rId1"/>
     <sheet name="rastrigin" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -187,7 +187,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="FF6600"/>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -275,7 +275,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-A408-42EC-ABB5-BED3ED326330}"/>
             </c:ext>
@@ -290,7 +290,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0070C0"/>
+                <a:srgbClr val="FF6600"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -339,7 +339,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-A408-42EC-ABB5-BED3ED326330}"/>
             </c:ext>
@@ -542,7 +542,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -658,7 +658,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-232C-407E-B5B4-E4B6B5F1FCF8}"/>
             </c:ext>
@@ -722,7 +722,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-232C-407E-B5B4-E4B6B5F1FCF8}"/>
             </c:ext>
@@ -925,7 +925,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1041,7 +1041,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-F513-46A0-B3A6-FA237D53372E}"/>
             </c:ext>
@@ -1105,7 +1105,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-F513-46A0-B3A6-FA237D53372E}"/>
             </c:ext>
@@ -1308,7 +1308,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1424,7 +1424,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C4E8-4CD1-8088-5EC56B161007}"/>
             </c:ext>
@@ -1488,7 +1488,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C4E8-4CD1-8088-5EC56B161007}"/>
             </c:ext>
@@ -1544,7 +1544,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1656,7 +1655,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1731,7 +1729,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1799,7 +1796,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1915,7 +1912,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FD71-45DE-A95F-3F39F3CB0F11}"/>
             </c:ext>
@@ -1979,7 +1976,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FD71-45DE-A95F-3F39F3CB0F11}"/>
             </c:ext>
@@ -2035,7 +2032,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2147,7 +2143,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2222,7 +2217,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2290,7 +2284,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2406,7 +2400,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-283A-41CF-863C-842CB246F13C}"/>
             </c:ext>
@@ -2470,7 +2464,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-283A-41CF-863C-842CB246F13C}"/>
             </c:ext>
@@ -2526,7 +2520,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2638,7 +2631,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2713,7 +2705,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6571,8 +6562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" topLeftCell="H26" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
All values for PSO_rastrigin (Graphs)
</commit_message>
<xml_diff>
--- a/Documentation/Graphs.xlsx
+++ b/Documentation/Graphs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="28">
   <si>
     <t>T1 (ms)</t>
   </si>
@@ -97,22 +97,13 @@
     <t>T7(ms)</t>
   </si>
   <si>
-    <t>T38(ms)</t>
-  </si>
-  <si>
     <t>T9(ms)</t>
   </si>
   <si>
     <t>T8(ms)</t>
   </si>
   <si>
-    <t>T39(ms)</t>
-  </si>
-  <si>
-    <t>T310(ms)</t>
-  </si>
-  <si>
-    <t>T35(ms)</t>
+    <t>T5(ms)</t>
   </si>
 </sst>
 </file>
@@ -161,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,6 +173,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,11 +393,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189387136"/>
-        <c:axId val="189388672"/>
+        <c:axId val="199802880"/>
+        <c:axId val="199804416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189387136"/>
+        <c:axId val="199802880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -448,7 +440,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189388672"/>
+        <c:crossAx val="199804416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -456,7 +448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189388672"/>
+        <c:axId val="199804416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -507,7 +499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189387136"/>
+        <c:crossAx val="199802880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -784,11 +776,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189668352"/>
-        <c:axId val="189694720"/>
+        <c:axId val="200354432"/>
+        <c:axId val="200372608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189668352"/>
+        <c:axId val="200354432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -831,7 +823,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189694720"/>
+        <c:crossAx val="200372608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -839,7 +831,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189694720"/>
+        <c:axId val="200372608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -890,7 +882,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189668352"/>
+        <c:crossAx val="200354432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1167,11 +1159,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189716352"/>
-        <c:axId val="189717888"/>
+        <c:axId val="200402432"/>
+        <c:axId val="200403968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189716352"/>
+        <c:axId val="200402432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1214,7 +1206,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189717888"/>
+        <c:crossAx val="200403968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1222,7 +1214,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189717888"/>
+        <c:axId val="200403968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1273,7 +1265,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189716352"/>
+        <c:crossAx val="200402432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1437,34 +1429,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>33.701666666666668</c:v>
+                  <c:v>11.601000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54.657666666666664</c:v>
+                  <c:v>13.523100000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57.314666666666668</c:v>
+                  <c:v>12.815200000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>73.317000000000007</c:v>
+                  <c:v>22.691299999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>78.643333333333331</c:v>
+                  <c:v>21.6022</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89.463666666666668</c:v>
+                  <c:v>23.1996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>136.65700000000001</c:v>
+                  <c:v>27.995100000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>155.21199999999999</c:v>
+                  <c:v>27.611599999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>122.65533333333333</c:v>
+                  <c:v>31.168299999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>188.50366666666667</c:v>
+                  <c:v>34.7742</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1550,11 +1542,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190067840"/>
-        <c:axId val="190069760"/>
+        <c:axId val="200155904"/>
+        <c:axId val="200157824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190067840"/>
+        <c:axId val="200155904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1638,7 +1630,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190069760"/>
+        <c:crossAx val="200157824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1646,7 +1638,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190069760"/>
+        <c:axId val="200157824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1724,7 +1716,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190067840"/>
+        <c:crossAx val="200155904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2012,11 +2004,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190110336"/>
-        <c:axId val="189862656"/>
+        <c:axId val="200205056"/>
+        <c:axId val="200206976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190110336"/>
+        <c:axId val="200205056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2100,7 +2092,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189862656"/>
+        <c:crossAx val="200206976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2108,7 +2100,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189862656"/>
+        <c:axId val="200206976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2186,7 +2178,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190110336"/>
+        <c:crossAx val="200205056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2351,34 +2343,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>26.661000000000001</c:v>
+                  <c:v>2.1048</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59.987333333333339</c:v>
+                  <c:v>4.5905000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99.975000000000009</c:v>
+                  <c:v>6.4826000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>89.202666666666673</c:v>
+                  <c:v>8.8872999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>82.583666666666673</c:v>
+                  <c:v>10.463000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>111.35833333333333</c:v>
+                  <c:v>14.181799999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>113.029</c:v>
+                  <c:v>15.068100000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>115.92033333333333</c:v>
+                  <c:v>16.454000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>147.50399999999999</c:v>
+                  <c:v>21.7515</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>162.11533333333335</c:v>
+                  <c:v>20.684099999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2464,11 +2456,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189901056"/>
-        <c:axId val="189907328"/>
+        <c:axId val="200310784"/>
+        <c:axId val="200312704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189901056"/>
+        <c:axId val="200310784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2552,7 +2544,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189907328"/>
+        <c:crossAx val="200312704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2560,7 +2552,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189907328"/>
+        <c:axId val="200312704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2652,7 +2644,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189901056"/>
+        <c:crossAx val="200310784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3178,7 +3170,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4401,8 +4393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AM11" sqref="AM11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4513,7 +4505,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
@@ -4527,6 +4519,9 @@
       <c r="J3" t="s">
         <v>21</v>
       </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
       <c r="L3" t="s">
         <v>14</v>
       </c>
@@ -4555,10 +4550,10 @@
         <v>24</v>
       </c>
       <c r="V3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="X3" t="s">
         <v>23</v>
@@ -4591,13 +4586,13 @@
         <v>18</v>
       </c>
       <c r="AI3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ3" t="s">
         <v>25</v>
       </c>
-      <c r="AJ3" t="s">
-        <v>28</v>
-      </c>
       <c r="AK3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="AL3" t="s">
         <v>14</v>
@@ -4608,17 +4603,38 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>28536</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>40109</v>
+        <v>7977</v>
       </c>
       <c r="D4">
-        <v>32460</v>
+        <v>20001</v>
+      </c>
+      <c r="E4">
+        <v>8000</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>7998</v>
+      </c>
+      <c r="H4">
+        <v>8000</v>
+      </c>
+      <c r="I4">
+        <v>48002</v>
+      </c>
+      <c r="J4">
+        <v>8033</v>
+      </c>
+      <c r="K4">
+        <v>7999</v>
       </c>
       <c r="L4" s="2">
-        <f t="shared" ref="L4:L13" si="0">AVERAGE(B4:D4) * 0.001</f>
-        <v>33.701666666666668</v>
+        <f>AVERAGE(B4:K4) * 0.001</f>
+        <v>11.601000000000001</v>
       </c>
       <c r="N4">
         <v>100</v>
@@ -4654,24 +4670,45 @@
         <v>7987</v>
       </c>
       <c r="Y4" s="2">
-        <f>AVERAGE(O4:X4)*0.001</f>
+        <f t="shared" ref="Y4:Y13" si="0">AVERAGE(O4:X4)*0.001</f>
         <v>8.6262999999999987</v>
       </c>
       <c r="AA4">
         <v>10</v>
       </c>
-      <c r="AB4">
-        <v>43990</v>
+      <c r="AB4" s="8">
+        <v>2046</v>
       </c>
       <c r="AC4">
-        <v>19993</v>
+        <v>2047</v>
       </c>
       <c r="AD4">
-        <v>16000</v>
+        <v>2056</v>
+      </c>
+      <c r="AE4">
+        <v>1961</v>
+      </c>
+      <c r="AF4">
+        <v>2004</v>
+      </c>
+      <c r="AG4">
+        <v>1995</v>
+      </c>
+      <c r="AH4">
+        <v>2992</v>
+      </c>
+      <c r="AI4">
+        <v>1955</v>
+      </c>
+      <c r="AJ4">
+        <v>1998</v>
+      </c>
+      <c r="AK4">
+        <v>1994</v>
       </c>
       <c r="AL4" s="2">
-        <f>AVERAGE(AB4:AD4)*0.001</f>
-        <v>26.661000000000001</v>
+        <f>AVERAGE(AB4:AK4)*0.001</f>
+        <v>2.1048</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
@@ -4679,17 +4716,38 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>55984</v>
+        <v>15625</v>
       </c>
       <c r="C5">
-        <v>55986</v>
+        <v>8001</v>
       </c>
       <c r="D5">
-        <v>52003</v>
+        <v>24000</v>
+      </c>
+      <c r="E5">
+        <v>7999</v>
+      </c>
+      <c r="F5">
+        <v>15621</v>
+      </c>
+      <c r="G5">
+        <v>12003</v>
+      </c>
+      <c r="H5">
+        <v>8001</v>
+      </c>
+      <c r="I5">
+        <v>16012</v>
+      </c>
+      <c r="J5">
+        <v>11967</v>
+      </c>
+      <c r="K5">
+        <v>16002</v>
       </c>
       <c r="L5" s="2">
-        <f t="shared" si="0"/>
-        <v>54.657666666666664</v>
+        <f>AVERAGE(B5:K5) * 0.001</f>
+        <v>13.523100000000001</v>
       </c>
       <c r="N5">
         <v>200</v>
@@ -4725,24 +4783,45 @@
         <v>17955</v>
       </c>
       <c r="Y5" s="2">
-        <f>AVERAGE(O5:X5)*0.001</f>
+        <f t="shared" si="0"/>
         <v>17.8095</v>
       </c>
       <c r="AA5">
         <v>20</v>
       </c>
-      <c r="AB5">
-        <v>95983</v>
+      <c r="AB5" s="8">
+        <v>4989</v>
       </c>
       <c r="AC5">
-        <v>39994</v>
+        <v>4934</v>
       </c>
       <c r="AD5">
-        <v>43985</v>
+        <v>4957</v>
+      </c>
+      <c r="AE5">
+        <v>4986</v>
+      </c>
+      <c r="AF5">
+        <v>3992</v>
+      </c>
+      <c r="AG5">
+        <v>4040</v>
+      </c>
+      <c r="AH5">
+        <v>3989</v>
+      </c>
+      <c r="AI5">
+        <v>4041</v>
+      </c>
+      <c r="AJ5">
+        <v>4991</v>
+      </c>
+      <c r="AK5">
+        <v>4986</v>
       </c>
       <c r="AL5" s="2">
-        <f t="shared" ref="AL5:AL13" si="1">AVERAGE(AB5:AD5)*0.001</f>
-        <v>59.987333333333339</v>
+        <f t="shared" ref="AL5:AL23" si="1">AVERAGE(AB5:AK5)*0.001</f>
+        <v>4.5905000000000005</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
@@ -4750,17 +4829,38 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>55988</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>59986</v>
+        <v>11999</v>
       </c>
       <c r="D6">
-        <v>55970</v>
+        <v>24003</v>
+      </c>
+      <c r="E6">
+        <v>12000</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>12001</v>
+      </c>
+      <c r="H6">
+        <v>11999</v>
+      </c>
+      <c r="I6">
+        <v>19987</v>
+      </c>
+      <c r="J6">
+        <v>20133</v>
+      </c>
+      <c r="K6">
+        <v>16030</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" si="0"/>
-        <v>57.314666666666668</v>
+        <f t="shared" ref="L6:L23" si="2">AVERAGE(B6:K6) * 0.001</f>
+        <v>12.815200000000001</v>
       </c>
       <c r="N6">
         <v>300</v>
@@ -4796,24 +4896,45 @@
         <v>24930</v>
       </c>
       <c r="Y6" s="2">
-        <f>AVERAGE(O6:X6)*0.001</f>
+        <f t="shared" si="0"/>
         <v>28.3626</v>
       </c>
       <c r="AA6">
         <v>30</v>
       </c>
-      <c r="AB6">
-        <v>123960</v>
+      <c r="AB6" s="8">
+        <v>5985</v>
       </c>
       <c r="AC6">
-        <v>111977</v>
+        <v>6030</v>
       </c>
       <c r="AD6">
-        <v>63988</v>
+        <v>5988</v>
+      </c>
+      <c r="AE6">
+        <v>5984</v>
+      </c>
+      <c r="AF6">
+        <v>6984</v>
+      </c>
+      <c r="AG6">
+        <v>5986</v>
+      </c>
+      <c r="AH6">
+        <v>6020</v>
+      </c>
+      <c r="AI6">
+        <v>5931</v>
+      </c>
+      <c r="AJ6">
+        <v>5944</v>
+      </c>
+      <c r="AK6">
+        <v>9974</v>
       </c>
       <c r="AL6" s="2">
         <f t="shared" si="1"/>
-        <v>99.975000000000009</v>
+        <v>6.4826000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
@@ -4821,17 +4942,38 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>67981</v>
+        <v>25336</v>
       </c>
       <c r="C7">
-        <v>79979</v>
+        <v>24001</v>
       </c>
       <c r="D7">
-        <v>71991</v>
+        <v>28029</v>
+      </c>
+      <c r="E7">
+        <v>28000</v>
+      </c>
+      <c r="F7">
+        <v>17543</v>
+      </c>
+      <c r="G7">
+        <v>19997</v>
+      </c>
+      <c r="H7">
+        <v>24000</v>
+      </c>
+      <c r="I7">
+        <v>27999</v>
+      </c>
+      <c r="J7">
+        <v>15997</v>
+      </c>
+      <c r="K7">
+        <v>16011</v>
       </c>
       <c r="L7" s="2">
-        <f t="shared" si="0"/>
-        <v>73.317000000000007</v>
+        <f t="shared" si="2"/>
+        <v>22.691299999999998</v>
       </c>
       <c r="N7">
         <v>400</v>
@@ -4867,24 +5009,45 @@
         <v>33914</v>
       </c>
       <c r="Y7" s="2">
-        <f>AVERAGE(O7:X7)*0.001</f>
+        <f t="shared" si="0"/>
         <v>32.864699999999999</v>
       </c>
       <c r="AA7">
         <v>40</v>
       </c>
-      <c r="AB7">
-        <v>75671</v>
+      <c r="AB7" s="8">
+        <v>7977</v>
       </c>
       <c r="AC7">
-        <v>75972</v>
+        <v>8930</v>
       </c>
       <c r="AD7">
-        <v>115965</v>
+        <v>8979</v>
+      </c>
+      <c r="AE7">
+        <v>7979</v>
+      </c>
+      <c r="AF7">
+        <v>7977</v>
+      </c>
+      <c r="AG7">
+        <v>7097</v>
+      </c>
+      <c r="AH7">
+        <v>7979</v>
+      </c>
+      <c r="AI7">
+        <v>10972</v>
+      </c>
+      <c r="AJ7">
+        <v>8016</v>
+      </c>
+      <c r="AK7">
+        <v>12967</v>
       </c>
       <c r="AL7" s="2">
         <f t="shared" si="1"/>
-        <v>89.202666666666673</v>
+        <v>8.8872999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
@@ -4892,17 +5055,38 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>79982</v>
+        <v>19998</v>
       </c>
       <c r="C8">
-        <v>79980</v>
+        <v>19998</v>
       </c>
       <c r="D8">
-        <v>75968</v>
+        <v>27964</v>
+      </c>
+      <c r="E8">
+        <v>28000</v>
+      </c>
+      <c r="F8">
+        <v>16099</v>
+      </c>
+      <c r="G8">
+        <v>16001</v>
+      </c>
+      <c r="H8">
+        <v>19999</v>
+      </c>
+      <c r="I8">
+        <v>28000</v>
+      </c>
+      <c r="J8">
+        <v>20003</v>
+      </c>
+      <c r="K8">
+        <v>19960</v>
       </c>
       <c r="L8" s="2">
-        <f t="shared" si="0"/>
-        <v>78.643333333333331</v>
+        <f t="shared" si="2"/>
+        <v>21.6022</v>
       </c>
       <c r="N8">
         <v>500</v>
@@ -4938,24 +5122,45 @@
         <v>40966</v>
       </c>
       <c r="Y8" s="2">
-        <f>AVERAGE(O8:X8)*0.001</f>
+        <f t="shared" si="0"/>
         <v>42.054400000000001</v>
       </c>
       <c r="AA8">
         <v>50</v>
       </c>
-      <c r="AB8">
-        <v>99769</v>
+      <c r="AB8" s="8">
+        <v>10918</v>
       </c>
       <c r="AC8">
-        <v>71980</v>
+        <v>11021</v>
       </c>
       <c r="AD8">
-        <v>76002</v>
+        <v>9932</v>
+      </c>
+      <c r="AE8">
+        <v>11971</v>
+      </c>
+      <c r="AF8">
+        <v>10920</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>10976</v>
+      </c>
+      <c r="AI8">
+        <v>9974</v>
+      </c>
+      <c r="AJ8">
+        <v>10966</v>
+      </c>
+      <c r="AK8">
+        <v>17952</v>
       </c>
       <c r="AL8" s="2">
         <f t="shared" si="1"/>
-        <v>82.583666666666673</v>
+        <v>10.463000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
@@ -4963,17 +5168,38 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>87997</v>
+        <v>20029</v>
       </c>
       <c r="C9">
-        <v>88418</v>
+        <v>20001</v>
       </c>
       <c r="D9">
-        <v>91976</v>
+        <v>24000</v>
+      </c>
+      <c r="E9">
+        <v>36000</v>
+      </c>
+      <c r="F9">
+        <v>15939</v>
+      </c>
+      <c r="G9">
+        <v>20029</v>
+      </c>
+      <c r="H9">
+        <v>27998</v>
+      </c>
+      <c r="I9">
+        <v>24000</v>
+      </c>
+      <c r="J9">
+        <v>27999</v>
+      </c>
+      <c r="K9">
+        <v>16001</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" si="0"/>
-        <v>89.463666666666668</v>
+        <f t="shared" si="2"/>
+        <v>23.1996</v>
       </c>
       <c r="N9">
         <v>600</v>
@@ -5009,24 +5235,45 @@
         <v>49870</v>
       </c>
       <c r="Y9" s="2">
-        <f>AVERAGE(O9:X9)*0.001</f>
+        <f t="shared" si="0"/>
         <v>54.9129</v>
       </c>
       <c r="AA9">
         <v>60</v>
       </c>
-      <c r="AB9">
-        <v>178042</v>
+      <c r="AB9" s="8">
+        <v>12965</v>
       </c>
       <c r="AC9">
-        <v>72034</v>
+        <v>12947</v>
       </c>
       <c r="AD9">
-        <v>83999</v>
+        <v>14013</v>
+      </c>
+      <c r="AE9">
+        <v>11965</v>
+      </c>
+      <c r="AF9">
+        <v>12965</v>
+      </c>
+      <c r="AG9">
+        <v>24039</v>
+      </c>
+      <c r="AH9">
+        <v>12969</v>
+      </c>
+      <c r="AI9">
+        <v>13011</v>
+      </c>
+      <c r="AJ9">
+        <v>12932</v>
+      </c>
+      <c r="AK9">
+        <v>14012</v>
       </c>
       <c r="AL9" s="2">
-        <f>AVERAGE(AB9:AD9)*0.001</f>
-        <v>111.35833333333333</v>
+        <f t="shared" si="1"/>
+        <v>14.181799999999999</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
@@ -5034,17 +5281,38 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>210310</v>
+        <v>23970</v>
       </c>
       <c r="C10">
-        <v>103993</v>
+        <v>24003</v>
       </c>
       <c r="D10">
-        <v>95668</v>
+        <v>32041</v>
+      </c>
+      <c r="E10">
+        <v>48001</v>
+      </c>
+      <c r="F10">
+        <v>19962</v>
+      </c>
+      <c r="G10">
+        <v>23971</v>
+      </c>
+      <c r="H10">
+        <v>32002</v>
+      </c>
+      <c r="I10">
+        <v>31999</v>
+      </c>
+      <c r="J10">
+        <v>23995</v>
+      </c>
+      <c r="K10">
+        <v>20007</v>
       </c>
       <c r="L10" s="2">
-        <f t="shared" si="0"/>
-        <v>136.65700000000001</v>
+        <f t="shared" si="2"/>
+        <v>27.995100000000001</v>
       </c>
       <c r="N10">
         <v>700</v>
@@ -5080,24 +5348,45 @@
         <v>58823</v>
       </c>
       <c r="Y10" s="2">
-        <f>AVERAGE(O10:X10)*0.001</f>
+        <f t="shared" si="0"/>
         <v>60.806300000000007</v>
       </c>
       <c r="AA10">
         <v>70</v>
       </c>
-      <c r="AB10">
-        <v>122890</v>
+      <c r="AB10" s="8">
+        <v>14962</v>
       </c>
       <c r="AC10">
-        <v>111396</v>
+        <v>14970</v>
       </c>
       <c r="AD10">
-        <v>104801</v>
+        <v>13962</v>
+      </c>
+      <c r="AE10">
+        <v>14961</v>
+      </c>
+      <c r="AF10">
+        <v>14960</v>
+      </c>
+      <c r="AG10">
+        <v>15011</v>
+      </c>
+      <c r="AH10">
+        <v>14951</v>
+      </c>
+      <c r="AI10">
+        <v>14956</v>
+      </c>
+      <c r="AJ10">
+        <v>15990</v>
+      </c>
+      <c r="AK10">
+        <v>15958</v>
       </c>
       <c r="AL10" s="2">
         <f t="shared" si="1"/>
-        <v>113.029</v>
+        <v>15.068100000000001</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
@@ -5105,17 +5394,38 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>151814</v>
+        <v>24001</v>
       </c>
       <c r="C11">
-        <v>201819</v>
+        <v>23998</v>
       </c>
       <c r="D11">
-        <v>112003</v>
+        <v>35964</v>
+      </c>
+      <c r="E11">
+        <v>24000</v>
+      </c>
+      <c r="F11">
+        <v>16075</v>
+      </c>
+      <c r="G11">
+        <v>24040</v>
+      </c>
+      <c r="H11">
+        <v>59998</v>
+      </c>
+      <c r="I11">
+        <v>24003</v>
+      </c>
+      <c r="J11">
+        <v>24002</v>
+      </c>
+      <c r="K11">
+        <v>20035</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" si="0"/>
-        <v>155.21199999999999</v>
+        <f t="shared" si="2"/>
+        <v>27.611599999999999</v>
       </c>
       <c r="N11">
         <v>800</v>
@@ -5151,24 +5461,45 @@
         <v>66832</v>
       </c>
       <c r="Y11" s="2">
-        <f>AVERAGE(O11:X11)*0.001</f>
+        <f t="shared" si="0"/>
         <v>68.180499999999995</v>
       </c>
       <c r="AA11">
         <v>80</v>
       </c>
-      <c r="AB11">
-        <v>132054</v>
+      <c r="AB11" s="8">
+        <v>16009</v>
       </c>
       <c r="AC11">
-        <v>104402</v>
+        <v>15914</v>
       </c>
       <c r="AD11">
-        <v>111305</v>
+        <v>16956</v>
+      </c>
+      <c r="AE11">
+        <v>15957</v>
+      </c>
+      <c r="AF11">
+        <v>16013</v>
+      </c>
+      <c r="AG11">
+        <v>16951</v>
+      </c>
+      <c r="AH11">
+        <v>16918</v>
+      </c>
+      <c r="AI11">
+        <v>15915</v>
+      </c>
+      <c r="AJ11">
+        <v>16955</v>
+      </c>
+      <c r="AK11">
+        <v>16952</v>
       </c>
       <c r="AL11" s="2">
         <f t="shared" si="1"/>
-        <v>115.92033333333333</v>
+        <v>16.454000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
@@ -5176,17 +5507,38 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>111669</v>
+        <v>24000</v>
       </c>
       <c r="C12">
-        <v>104445</v>
+        <v>32002</v>
       </c>
       <c r="D12">
-        <v>151852</v>
+        <v>40061</v>
+      </c>
+      <c r="E12">
+        <v>36009</v>
+      </c>
+      <c r="F12">
+        <v>15657</v>
+      </c>
+      <c r="G12">
+        <v>28000</v>
+      </c>
+      <c r="H12">
+        <v>48000</v>
+      </c>
+      <c r="I12">
+        <v>27998</v>
+      </c>
+      <c r="J12">
+        <v>32000</v>
+      </c>
+      <c r="K12">
+        <v>27956</v>
       </c>
       <c r="L12" s="2">
-        <f t="shared" si="0"/>
-        <v>122.65533333333333</v>
+        <f t="shared" si="2"/>
+        <v>31.168299999999999</v>
       </c>
       <c r="N12">
         <v>900</v>
@@ -5222,24 +5574,45 @@
         <v>74803</v>
       </c>
       <c r="Y12" s="2">
-        <f>AVERAGE(O12:X12)*0.001</f>
+        <f t="shared" si="0"/>
         <v>73.411000000000001</v>
       </c>
       <c r="AA12">
         <v>90</v>
       </c>
-      <c r="AB12">
-        <v>151312</v>
+      <c r="AB12" s="8">
+        <v>18897</v>
       </c>
       <c r="AC12">
-        <v>175861</v>
+        <v>19948</v>
       </c>
       <c r="AD12">
-        <v>115339</v>
+        <v>18947</v>
+      </c>
+      <c r="AE12">
+        <v>44880</v>
+      </c>
+      <c r="AF12">
+        <v>18943</v>
+      </c>
+      <c r="AG12">
+        <v>17956</v>
+      </c>
+      <c r="AH12">
+        <v>18998</v>
+      </c>
+      <c r="AI12">
+        <v>19007</v>
+      </c>
+      <c r="AJ12">
+        <v>18949</v>
+      </c>
+      <c r="AK12">
+        <v>20990</v>
       </c>
       <c r="AL12" s="2">
         <f t="shared" si="1"/>
-        <v>147.50399999999999</v>
+        <v>21.7515</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
@@ -5247,17 +5620,38 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>135701</v>
+        <v>27999</v>
       </c>
       <c r="C13">
-        <v>198926</v>
+        <v>36006</v>
       </c>
       <c r="D13">
-        <v>230884</v>
+        <v>39934</v>
+      </c>
+      <c r="E13">
+        <v>28001</v>
+      </c>
+      <c r="F13">
+        <v>15682</v>
+      </c>
+      <c r="G13">
+        <v>67959</v>
+      </c>
+      <c r="H13">
+        <v>39998</v>
+      </c>
+      <c r="I13">
+        <v>36163</v>
+      </c>
+      <c r="J13">
+        <v>32001</v>
+      </c>
+      <c r="K13">
+        <v>23999</v>
       </c>
       <c r="L13" s="2">
-        <f t="shared" si="0"/>
-        <v>188.50366666666667</v>
+        <f t="shared" si="2"/>
+        <v>34.7742</v>
       </c>
       <c r="N13">
         <v>1000</v>
@@ -5293,27 +5687,85 @@
         <v>84722</v>
       </c>
       <c r="Y13" s="2">
-        <f>AVERAGE(O13:X13)*0.001</f>
+        <f t="shared" si="0"/>
         <v>81.04610000000001</v>
       </c>
       <c r="AA13">
         <v>100</v>
       </c>
-      <c r="AB13">
-        <v>184343</v>
+      <c r="AB13" s="8">
+        <v>19990</v>
       </c>
       <c r="AC13">
-        <v>155428</v>
+        <v>20990</v>
       </c>
       <c r="AD13">
-        <v>146575</v>
+        <v>20898</v>
+      </c>
+      <c r="AE13">
+        <v>23936</v>
+      </c>
+      <c r="AF13">
+        <v>19950</v>
+      </c>
+      <c r="AG13">
+        <v>15360</v>
+      </c>
+      <c r="AH13">
+        <v>21892</v>
+      </c>
+      <c r="AI13">
+        <v>20932</v>
+      </c>
+      <c r="AJ13">
+        <v>19947</v>
+      </c>
+      <c r="AK13">
+        <v>22946</v>
       </c>
       <c r="AL13" s="2">
         <f t="shared" si="1"/>
-        <v>162.11533333333335</v>
+        <v>20.684099999999997</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>40010</v>
+      </c>
+      <c r="C14">
+        <v>59999</v>
+      </c>
+      <c r="D14">
+        <v>40000</v>
+      </c>
+      <c r="E14">
+        <v>44005</v>
+      </c>
+      <c r="F14">
+        <v>28617</v>
+      </c>
+      <c r="G14">
+        <v>32037</v>
+      </c>
+      <c r="H14">
+        <v>36005</v>
+      </c>
+      <c r="I14">
+        <v>36001</v>
+      </c>
+      <c r="J14">
+        <v>27999</v>
+      </c>
+      <c r="K14">
+        <v>28038</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="2"/>
+        <v>37.271099999999997</v>
+      </c>
       <c r="N14">
         <v>1100</v>
       </c>
@@ -5348,11 +5800,85 @@
         <v>92752</v>
       </c>
       <c r="Y14" s="2">
-        <f t="shared" ref="Y14:Y23" si="2">AVERAGE(O14:X14)*0.001</f>
+        <f t="shared" ref="Y14:Y23" si="3">AVERAGE(O14:X14)*0.001</f>
         <v>95.047800000000009</v>
+      </c>
+      <c r="AA14">
+        <v>110</v>
+      </c>
+      <c r="AB14" s="8">
+        <v>22934</v>
+      </c>
+      <c r="AC14">
+        <v>22890</v>
+      </c>
+      <c r="AD14">
+        <v>22986</v>
+      </c>
+      <c r="AE14">
+        <v>22971</v>
+      </c>
+      <c r="AF14">
+        <v>22937</v>
+      </c>
+      <c r="AG14">
+        <v>30794</v>
+      </c>
+      <c r="AH14">
+        <v>29969</v>
+      </c>
+      <c r="AI14">
+        <v>22924</v>
+      </c>
+      <c r="AJ14">
+        <v>22945</v>
+      </c>
+      <c r="AK14">
+        <v>23936</v>
+      </c>
+      <c r="AL14" s="2">
+        <f t="shared" si="1"/>
+        <v>24.528599999999997</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>35993</v>
+      </c>
+      <c r="C15">
+        <v>47997</v>
+      </c>
+      <c r="D15">
+        <v>60002</v>
+      </c>
+      <c r="E15">
+        <v>55999</v>
+      </c>
+      <c r="F15">
+        <v>15660</v>
+      </c>
+      <c r="G15">
+        <v>27999</v>
+      </c>
+      <c r="H15">
+        <v>44031</v>
+      </c>
+      <c r="I15">
+        <v>60000</v>
+      </c>
+      <c r="J15">
+        <v>35999</v>
+      </c>
+      <c r="K15">
+        <v>83996</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="2"/>
+        <v>46.767600000000002</v>
+      </c>
       <c r="N15">
         <v>1200</v>
       </c>
@@ -5387,11 +5913,85 @@
         <v>101728</v>
       </c>
       <c r="Y15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>101.28760000000001</v>
+      </c>
+      <c r="AA15">
+        <v>120</v>
+      </c>
+      <c r="AB15" s="8">
+        <v>23952</v>
+      </c>
+      <c r="AC15">
+        <v>24934</v>
+      </c>
+      <c r="AD15">
+        <v>24936</v>
+      </c>
+      <c r="AE15">
+        <v>25935</v>
+      </c>
+      <c r="AF15">
+        <v>24934</v>
+      </c>
+      <c r="AG15">
+        <v>20555</v>
+      </c>
+      <c r="AH15">
+        <v>24926</v>
+      </c>
+      <c r="AI15">
+        <v>50833</v>
+      </c>
+      <c r="AJ15">
+        <v>24939</v>
+      </c>
+      <c r="AK15">
+        <v>26926</v>
+      </c>
+      <c r="AL15" s="2">
+        <f t="shared" si="1"/>
+        <v>27.286999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>44000</v>
+      </c>
+      <c r="C16">
+        <v>40006</v>
+      </c>
+      <c r="D16">
+        <v>51999</v>
+      </c>
+      <c r="E16">
+        <v>58924</v>
+      </c>
+      <c r="F16">
+        <v>31243</v>
+      </c>
+      <c r="G16">
+        <v>32004</v>
+      </c>
+      <c r="H16">
+        <v>44031</v>
+      </c>
+      <c r="I16">
+        <v>60004</v>
+      </c>
+      <c r="J16">
+        <v>40001</v>
+      </c>
+      <c r="K16">
+        <v>64000</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="2"/>
+        <v>46.621199999999995</v>
+      </c>
       <c r="N16">
         <v>1300</v>
       </c>
@@ -5426,11 +6026,85 @@
         <v>3331750</v>
       </c>
       <c r="Y16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>432.28730000000002</v>
+      </c>
+      <c r="AA16">
+        <v>130</v>
+      </c>
+      <c r="AB16" s="8">
+        <v>51805</v>
+      </c>
+      <c r="AC16">
+        <v>45880</v>
+      </c>
+      <c r="AD16">
+        <v>49815</v>
+      </c>
+      <c r="AE16">
+        <v>26946</v>
+      </c>
+      <c r="AF16">
+        <v>41871</v>
+      </c>
+      <c r="AG16">
+        <v>30659</v>
+      </c>
+      <c r="AH16">
+        <v>31873</v>
+      </c>
+      <c r="AI16">
+        <v>33954</v>
+      </c>
+      <c r="AJ16">
+        <v>43838</v>
+      </c>
+      <c r="AK16">
+        <v>28920</v>
+      </c>
+      <c r="AL16" s="2">
+        <f t="shared" si="1"/>
+        <v>38.556100000000001</v>
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>40002</v>
+      </c>
+      <c r="C17">
+        <v>43991</v>
+      </c>
+      <c r="D17">
+        <v>44056</v>
+      </c>
+      <c r="E17">
+        <v>63816</v>
+      </c>
+      <c r="F17">
+        <v>15621</v>
+      </c>
+      <c r="G17">
+        <v>35961</v>
+      </c>
+      <c r="H17">
+        <v>59934</v>
+      </c>
+      <c r="I17">
+        <v>55997</v>
+      </c>
+      <c r="J17">
+        <v>32001</v>
+      </c>
+      <c r="K17">
+        <v>56997</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="2"/>
+        <v>44.837600000000002</v>
+      </c>
       <c r="N17">
         <v>1400</v>
       </c>
@@ -5465,11 +6139,85 @@
         <v>119678</v>
       </c>
       <c r="Y17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>115.3154</v>
+      </c>
+      <c r="AA17">
+        <v>140</v>
+      </c>
+      <c r="AB17" s="8">
+        <v>29922</v>
+      </c>
+      <c r="AC17">
+        <v>29971</v>
+      </c>
+      <c r="AD17">
+        <v>30918</v>
+      </c>
+      <c r="AE17">
+        <v>29921</v>
+      </c>
+      <c r="AF17">
+        <v>31879</v>
+      </c>
+      <c r="AG17">
+        <v>30278</v>
+      </c>
+      <c r="AH17">
+        <v>29969</v>
+      </c>
+      <c r="AI17">
+        <v>28928</v>
+      </c>
+      <c r="AJ17">
+        <v>38944</v>
+      </c>
+      <c r="AK17">
+        <v>30921</v>
+      </c>
+      <c r="AL17" s="2">
+        <f t="shared" si="1"/>
+        <v>31.165099999999999</v>
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>44028</v>
+      </c>
+      <c r="C18">
+        <v>44003</v>
+      </c>
+      <c r="D18">
+        <v>72000</v>
+      </c>
+      <c r="E18">
+        <v>36081</v>
+      </c>
+      <c r="F18">
+        <v>39852</v>
+      </c>
+      <c r="G18">
+        <v>44004</v>
+      </c>
+      <c r="H18">
+        <v>56002</v>
+      </c>
+      <c r="I18">
+        <v>64001</v>
+      </c>
+      <c r="J18">
+        <v>9999</v>
+      </c>
+      <c r="K18">
+        <v>58002</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="2"/>
+        <v>46.797199999999997</v>
+      </c>
       <c r="N18">
         <v>1500</v>
       </c>
@@ -5504,11 +6252,85 @@
         <v>128610</v>
       </c>
       <c r="Y18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>135.67929999999998</v>
+      </c>
+      <c r="AA18">
+        <v>150</v>
+      </c>
+      <c r="AB18" s="8">
+        <v>30974</v>
+      </c>
+      <c r="AC18">
+        <v>30915</v>
+      </c>
+      <c r="AD18">
+        <v>30917</v>
+      </c>
+      <c r="AE18">
+        <v>30909</v>
+      </c>
+      <c r="AF18">
+        <v>30917</v>
+      </c>
+      <c r="AG18">
+        <v>28397</v>
+      </c>
+      <c r="AH18">
+        <v>30923</v>
+      </c>
+      <c r="AI18">
+        <v>30919</v>
+      </c>
+      <c r="AJ18">
+        <v>30918</v>
+      </c>
+      <c r="AK18">
+        <v>32908</v>
+      </c>
+      <c r="AL18" s="2">
+        <f t="shared" si="1"/>
+        <v>30.869700000000002</v>
       </c>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>35967</v>
+      </c>
+      <c r="C19">
+        <v>63997</v>
+      </c>
+      <c r="D19">
+        <v>83344</v>
+      </c>
+      <c r="E19">
+        <v>46868</v>
+      </c>
+      <c r="F19">
+        <v>28395</v>
+      </c>
+      <c r="G19">
+        <v>60381</v>
+      </c>
+      <c r="H19">
+        <v>55997</v>
+      </c>
+      <c r="I19">
+        <v>51998</v>
+      </c>
+      <c r="J19">
+        <v>49065</v>
+      </c>
+      <c r="K19">
+        <v>55897</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="2"/>
+        <v>53.190899999999999</v>
+      </c>
       <c r="N19">
         <v>1600</v>
       </c>
@@ -5543,11 +6365,85 @@
         <v>135690</v>
       </c>
       <c r="Y19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>132.42620000000002</v>
+      </c>
+      <c r="AA19">
+        <v>160</v>
+      </c>
+      <c r="AB19" s="8">
+        <v>32908</v>
+      </c>
+      <c r="AC19">
+        <v>32914</v>
+      </c>
+      <c r="AD19">
+        <v>32912</v>
+      </c>
+      <c r="AE19">
+        <v>33916</v>
+      </c>
+      <c r="AF19">
+        <v>32912</v>
+      </c>
+      <c r="AG19">
+        <v>32362</v>
+      </c>
+      <c r="AH19">
+        <v>32911</v>
+      </c>
+      <c r="AI19">
+        <v>32859</v>
+      </c>
+      <c r="AJ19">
+        <v>33892</v>
+      </c>
+      <c r="AK19">
+        <v>34963</v>
+      </c>
+      <c r="AL19" s="2">
+        <f t="shared" si="1"/>
+        <v>33.254899999999999</v>
       </c>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>44033</v>
+      </c>
+      <c r="C20">
+        <v>60032</v>
+      </c>
+      <c r="D20">
+        <v>74000</v>
+      </c>
+      <c r="E20">
+        <v>45258</v>
+      </c>
+      <c r="F20">
+        <v>46321</v>
+      </c>
+      <c r="G20">
+        <v>72032</v>
+      </c>
+      <c r="H20">
+        <v>56000</v>
+      </c>
+      <c r="I20">
+        <v>44000</v>
+      </c>
+      <c r="J20">
+        <v>56643</v>
+      </c>
+      <c r="K20">
+        <v>56000</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="2"/>
+        <v>55.431900000000006</v>
+      </c>
       <c r="N20">
         <v>1700</v>
       </c>
@@ -5582,11 +6478,85 @@
         <v>145558</v>
       </c>
       <c r="Y20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>143.2165</v>
+      </c>
+      <c r="AA20">
+        <v>170</v>
+      </c>
+      <c r="AB20" s="8">
+        <v>34904</v>
+      </c>
+      <c r="AC20">
+        <v>34908</v>
+      </c>
+      <c r="AD20">
+        <v>34906</v>
+      </c>
+      <c r="AE20">
+        <v>34906</v>
+      </c>
+      <c r="AF20">
+        <v>34907</v>
+      </c>
+      <c r="AG20">
+        <v>30828</v>
+      </c>
+      <c r="AH20">
+        <v>33910</v>
+      </c>
+      <c r="AI20">
+        <v>38952</v>
+      </c>
+      <c r="AJ20">
+        <v>34915</v>
+      </c>
+      <c r="AK20">
+        <v>30769</v>
+      </c>
+      <c r="AL20" s="2">
+        <f t="shared" si="1"/>
+        <v>34.390500000000003</v>
       </c>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>51969</v>
+      </c>
+      <c r="C21">
+        <v>51970</v>
+      </c>
+      <c r="D21">
+        <v>67999</v>
+      </c>
+      <c r="E21">
+        <v>46873</v>
+      </c>
+      <c r="F21">
+        <v>38443</v>
+      </c>
+      <c r="G21">
+        <v>63970</v>
+      </c>
+      <c r="H21">
+        <v>56020</v>
+      </c>
+      <c r="I21">
+        <v>67999</v>
+      </c>
+      <c r="J21">
+        <v>56431</v>
+      </c>
+      <c r="K21">
+        <v>56020</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="2"/>
+        <v>55.769400000000005</v>
+      </c>
       <c r="N21">
         <v>1800</v>
       </c>
@@ -5621,11 +6591,85 @@
         <v>151553</v>
       </c>
       <c r="Y21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>154.12810000000002</v>
+      </c>
+      <c r="AA21">
+        <v>180</v>
+      </c>
+      <c r="AB21" s="8">
+        <v>38933</v>
+      </c>
+      <c r="AC21">
+        <v>35850</v>
+      </c>
+      <c r="AD21">
+        <v>36902</v>
+      </c>
+      <c r="AE21">
+        <v>36846</v>
+      </c>
+      <c r="AF21">
+        <v>36901</v>
+      </c>
+      <c r="AG21">
+        <v>40448</v>
+      </c>
+      <c r="AH21">
+        <v>37893</v>
+      </c>
+      <c r="AI21">
+        <v>36897</v>
+      </c>
+      <c r="AJ21">
+        <v>37896</v>
+      </c>
+      <c r="AK21">
+        <v>41115</v>
+      </c>
+      <c r="AL21" s="2">
+        <f t="shared" si="1"/>
+        <v>37.9681</v>
       </c>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>43997</v>
+      </c>
+      <c r="C22">
+        <v>71999</v>
+      </c>
+      <c r="D22">
+        <v>76000</v>
+      </c>
+      <c r="E22">
+        <v>53375</v>
+      </c>
+      <c r="F22">
+        <v>41006</v>
+      </c>
+      <c r="G22">
+        <v>72036</v>
+      </c>
+      <c r="H22">
+        <v>43997</v>
+      </c>
+      <c r="I22">
+        <v>56000</v>
+      </c>
+      <c r="J22">
+        <v>48240</v>
+      </c>
+      <c r="K22">
+        <v>43997</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="2"/>
+        <v>55.064699999999995</v>
+      </c>
       <c r="N22">
         <v>1900</v>
       </c>
@@ -5660,11 +6704,85 @@
         <v>153591</v>
       </c>
       <c r="Y22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>159.2218</v>
+      </c>
+      <c r="AA22">
+        <v>190</v>
+      </c>
+      <c r="AB22" s="8">
+        <v>41903</v>
+      </c>
+      <c r="AC22">
+        <v>39894</v>
+      </c>
+      <c r="AD22">
+        <v>39893</v>
+      </c>
+      <c r="AE22">
+        <v>38897</v>
+      </c>
+      <c r="AF22">
+        <v>38902</v>
+      </c>
+      <c r="AG22">
+        <v>38893</v>
+      </c>
+      <c r="AH22">
+        <v>38902</v>
+      </c>
+      <c r="AI22">
+        <v>37900</v>
+      </c>
+      <c r="AJ22">
+        <v>39857</v>
+      </c>
+      <c r="AK22">
+        <v>44337</v>
+      </c>
+      <c r="AL22" s="2">
+        <f t="shared" si="1"/>
+        <v>39.937800000000003</v>
       </c>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>52034</v>
+      </c>
+      <c r="C23">
+        <v>61534</v>
+      </c>
+      <c r="D23">
+        <v>64000</v>
+      </c>
+      <c r="E23">
+        <v>65100</v>
+      </c>
+      <c r="F23">
+        <v>34120</v>
+      </c>
+      <c r="G23">
+        <v>75976</v>
+      </c>
+      <c r="H23">
+        <v>52034</v>
+      </c>
+      <c r="I23">
+        <v>84000</v>
+      </c>
+      <c r="J23">
+        <v>60454</v>
+      </c>
+      <c r="K23">
+        <v>62034</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" si="2"/>
+        <v>61.128599999999999</v>
+      </c>
       <c r="N23">
         <v>2000</v>
       </c>
@@ -5699,8 +6817,45 @@
         <v>161889</v>
       </c>
       <c r="Y23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>166.41410000000002</v>
+      </c>
+      <c r="AA23">
+        <v>200</v>
+      </c>
+      <c r="AB23" s="8">
+        <v>42803</v>
+      </c>
+      <c r="AC23">
+        <v>40891</v>
+      </c>
+      <c r="AD23">
+        <v>41888</v>
+      </c>
+      <c r="AE23">
+        <v>40890</v>
+      </c>
+      <c r="AF23">
+        <v>41882</v>
+      </c>
+      <c r="AG23">
+        <v>40907</v>
+      </c>
+      <c r="AH23">
+        <v>39185</v>
+      </c>
+      <c r="AI23">
+        <v>41882</v>
+      </c>
+      <c r="AJ23">
+        <v>41921</v>
+      </c>
+      <c r="AK23">
+        <v>45347</v>
+      </c>
+      <c r="AL23" s="2">
+        <f t="shared" si="1"/>
+        <v>41.759599999999999</v>
       </c>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.25">
@@ -5904,7 +7059,7 @@
         <v>125751</v>
       </c>
       <c r="L28" s="2">
-        <f t="shared" ref="L28:L37" si="3">AVERAGE(B28:D28)*0.001</f>
+        <f t="shared" ref="L28:L37" si="4">AVERAGE(B28:D28)*0.001</f>
         <v>134.86266666666666</v>
       </c>
       <c r="N28">
@@ -5920,7 +7075,7 @@
         <v>233865</v>
       </c>
       <c r="Y28" s="2">
-        <f>AVERAGE(O28:Q28)*0.001</f>
+        <f t="shared" ref="Y28:Y37" si="5">AVERAGE(O28:Q28)*0.001</f>
         <v>234.39099999999999</v>
       </c>
       <c r="AA28">
@@ -5954,7 +7109,7 @@
         <v>132925</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>125.26166666666667</v>
       </c>
       <c r="N29">
@@ -5970,7 +7125,7 @@
         <v>423914</v>
       </c>
       <c r="Y29" s="2">
-        <f>AVERAGE(O29:Q29)*0.001</f>
+        <f t="shared" si="5"/>
         <v>424.8896666666667</v>
       </c>
       <c r="AA29">
@@ -5986,7 +7141,7 @@
         <v>136593</v>
       </c>
       <c r="AL29" s="2">
-        <f t="shared" ref="AL29:AL37" si="4">AVERAGE(AB29:AD29)*0.001</f>
+        <f t="shared" ref="AL29:AL37" si="6">AVERAGE(AB29:AD29)*0.001</f>
         <v>145.03633333333335</v>
       </c>
     </row>
@@ -6004,7 +7159,7 @@
         <v>122929</v>
       </c>
       <c r="L30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>124.26833333333333</v>
       </c>
       <c r="N30">
@@ -6020,7 +7175,7 @@
         <v>613485</v>
       </c>
       <c r="Y30" s="2">
-        <f>AVERAGE(O30:Q30)*0.001</f>
+        <f t="shared" si="5"/>
         <v>611.08666666666659</v>
       </c>
       <c r="AA30">
@@ -6036,7 +7191,7 @@
         <v>167517</v>
       </c>
       <c r="AL30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>150.358</v>
       </c>
     </row>
@@ -6054,7 +7209,7 @@
         <v>124692</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>129.18133333333333</v>
       </c>
       <c r="N31">
@@ -6070,7 +7225,7 @@
         <v>812709</v>
       </c>
       <c r="Y31" s="2">
-        <f>AVERAGE(O31:Q31)*0.001</f>
+        <f t="shared" si="5"/>
         <v>805.37800000000004</v>
       </c>
       <c r="AA31">
@@ -6086,7 +7241,7 @@
         <v>173899</v>
       </c>
       <c r="AL31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>160.57566666666665</v>
       </c>
     </row>
@@ -6104,7 +7259,7 @@
         <v>117933</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>122.92933333333333</v>
       </c>
       <c r="N32">
@@ -6120,7 +7275,7 @@
         <v>131466</v>
       </c>
       <c r="Y32" s="2">
-        <f>AVERAGE(O32:Q32)*0.001</f>
+        <f t="shared" si="5"/>
         <v>434.23633333333333</v>
       </c>
       <c r="AA32">
@@ -6136,7 +7291,7 @@
         <v>163908</v>
       </c>
       <c r="AL32" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>140.95233333333334</v>
       </c>
     </row>
@@ -6154,7 +7309,7 @@
         <v>151912</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>174.56766666666667</v>
       </c>
       <c r="N33">
@@ -6170,7 +7325,7 @@
         <v>1263482</v>
       </c>
       <c r="Y33" s="2">
-        <f>AVERAGE(O33:Q33)*0.001</f>
+        <f t="shared" si="5"/>
         <v>1226.0323333333333</v>
       </c>
       <c r="AA33">
@@ -6186,7 +7341,7 @@
         <v>167902</v>
       </c>
       <c r="AL33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>136.45833333333334</v>
       </c>
     </row>
@@ -6204,7 +7359,7 @@
         <v>131925</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>136.91533333333334</v>
       </c>
       <c r="N34">
@@ -6220,7 +7375,7 @@
         <v>1374165</v>
       </c>
       <c r="Y34" s="2">
-        <f>AVERAGE(O34:Q34)*0.001</f>
+        <f t="shared" si="5"/>
         <v>1360.6426666666669</v>
       </c>
       <c r="AA34">
@@ -6236,7 +7391,7 @@
         <v>150912</v>
       </c>
       <c r="AL34" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>136.88466666666665</v>
       </c>
     </row>
@@ -6254,7 +7409,7 @@
         <v>118932</v>
       </c>
       <c r="L35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>131.59133333333335</v>
       </c>
       <c r="N35">
@@ -6270,7 +7425,7 @@
         <v>1535428</v>
       </c>
       <c r="Y35" s="2">
-        <f>AVERAGE(O35:Q35)*0.001</f>
+        <f t="shared" si="5"/>
         <v>1547.5319999999999</v>
       </c>
       <c r="AA35">
@@ -6286,7 +7441,7 @@
         <v>158343</v>
       </c>
       <c r="AL35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>171.71299999999999</v>
       </c>
     </row>
@@ -6304,7 +7459,7 @@
         <v>147916</v>
       </c>
       <c r="L36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>130.31100000000001</v>
       </c>
       <c r="N36">
@@ -6320,7 +7475,7 @@
         <v>1728210</v>
       </c>
       <c r="Y36" s="2">
-        <f>AVERAGE(O36:Q36)*0.001</f>
+        <f t="shared" si="5"/>
         <v>1753.8453333333332</v>
       </c>
       <c r="AA36">
@@ -6336,7 +7491,7 @@
         <v>170901</v>
       </c>
       <c r="AL36" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>141.53033333333335</v>
       </c>
     </row>
@@ -6354,7 +7509,7 @@
         <v>122932</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>131.501</v>
       </c>
       <c r="N37">
@@ -6370,7 +7525,7 @@
         <v>1944963</v>
       </c>
       <c r="Y37" s="2">
-        <f>AVERAGE(O37:Q37)*0.001</f>
+        <f t="shared" si="5"/>
         <v>1956.0963333333334</v>
       </c>
       <c r="AA37">
@@ -6386,7 +7541,7 @@
         <v>173900</v>
       </c>
       <c r="AL37" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>138.25300000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
All values for PSO_rastrigin added (Graphs)
</commit_message>
<xml_diff>
--- a/Documentation/Graphs.xlsx
+++ b/Documentation/Graphs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="28">
   <si>
     <t>T1 (ms)</t>
   </si>
@@ -97,22 +97,13 @@
     <t>T7(ms)</t>
   </si>
   <si>
-    <t>T38(ms)</t>
-  </si>
-  <si>
     <t>T9(ms)</t>
   </si>
   <si>
     <t>T8(ms)</t>
   </si>
   <si>
-    <t>T39(ms)</t>
-  </si>
-  <si>
-    <t>T310(ms)</t>
-  </si>
-  <si>
-    <t>T35(ms)</t>
+    <t>T5(ms)</t>
   </si>
 </sst>
 </file>
@@ -161,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -173,6 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -401,11 +393,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189387136"/>
-        <c:axId val="189388672"/>
+        <c:axId val="190169472"/>
+        <c:axId val="190171008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189387136"/>
+        <c:axId val="190169472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -448,7 +440,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189388672"/>
+        <c:crossAx val="190171008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -456,7 +448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189388672"/>
+        <c:axId val="190171008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -507,7 +499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189387136"/>
+        <c:crossAx val="190169472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -784,11 +776,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189668352"/>
-        <c:axId val="189694720"/>
+        <c:axId val="190450688"/>
+        <c:axId val="190477056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189668352"/>
+        <c:axId val="190450688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -831,7 +823,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189694720"/>
+        <c:crossAx val="190477056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -839,7 +831,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189694720"/>
+        <c:axId val="190477056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -890,7 +882,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189668352"/>
+        <c:crossAx val="190450688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1167,11 +1159,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189716352"/>
-        <c:axId val="189717888"/>
+        <c:axId val="190506880"/>
+        <c:axId val="190508416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189716352"/>
+        <c:axId val="190506880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1214,7 +1206,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189717888"/>
+        <c:crossAx val="190508416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1222,7 +1214,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189717888"/>
+        <c:axId val="190508416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1273,7 +1265,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189716352"/>
+        <c:crossAx val="190506880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1437,34 +1429,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>33.701666666666668</c:v>
+                  <c:v>11.601000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54.657666666666664</c:v>
+                  <c:v>13.523100000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57.314666666666668</c:v>
+                  <c:v>12.815200000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>73.317000000000007</c:v>
+                  <c:v>22.691299999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>78.643333333333331</c:v>
+                  <c:v>21.6022</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89.463666666666668</c:v>
+                  <c:v>23.1996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>136.65700000000001</c:v>
+                  <c:v>27.995100000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>155.21199999999999</c:v>
+                  <c:v>27.611599999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>122.65533333333333</c:v>
+                  <c:v>31.168299999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>188.50366666666667</c:v>
+                  <c:v>34.7742</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1550,11 +1542,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190067840"/>
-        <c:axId val="190069760"/>
+        <c:axId val="190854272"/>
+        <c:axId val="190856192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190067840"/>
+        <c:axId val="190854272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,7 +1583,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1638,7 +1629,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190069760"/>
+        <c:crossAx val="190856192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1646,7 +1637,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190069760"/>
+        <c:axId val="190856192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1683,7 +1674,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1724,7 +1714,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190067840"/>
+        <c:crossAx val="190854272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1738,7 +1728,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2012,11 +2001,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190110336"/>
-        <c:axId val="189862656"/>
+        <c:axId val="190894848"/>
+        <c:axId val="190896768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190110336"/>
+        <c:axId val="190894848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2053,7 +2042,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2100,7 +2088,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189862656"/>
+        <c:crossAx val="190896768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2108,7 +2096,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189862656"/>
+        <c:axId val="190896768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2145,7 +2133,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2186,7 +2173,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190110336"/>
+        <c:crossAx val="190894848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2200,7 +2187,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2351,34 +2337,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>26.661000000000001</c:v>
+                  <c:v>2.1048</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59.987333333333339</c:v>
+                  <c:v>4.5905000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99.975000000000009</c:v>
+                  <c:v>6.4826000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>89.202666666666673</c:v>
+                  <c:v>8.8872999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>82.583666666666673</c:v>
+                  <c:v>10.463000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>111.35833333333333</c:v>
+                  <c:v>14.181799999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>113.029</c:v>
+                  <c:v>15.068100000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>115.92033333333333</c:v>
+                  <c:v>16.454000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>147.50399999999999</c:v>
+                  <c:v>21.7515</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>162.11533333333335</c:v>
+                  <c:v>20.684099999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2464,11 +2450,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189901056"/>
-        <c:axId val="189907328"/>
+        <c:axId val="190677376"/>
+        <c:axId val="190679296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="189901056"/>
+        <c:axId val="190677376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2505,7 +2491,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2552,7 +2537,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189907328"/>
+        <c:crossAx val="190679296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2560,7 +2545,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189907328"/>
+        <c:axId val="190679296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2611,7 +2596,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2652,7 +2636,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189901056"/>
+        <c:crossAx val="190677376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2666,7 +2650,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3178,7 +3161,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3200,42 +3183,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="H3" s="7" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="H3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="N3" s="7" t="s">
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="N3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -3785,42 +3768,42 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="H19" s="7" t="s">
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="H19" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="N19" s="7" t="s">
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="N19" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -4401,8 +4384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4418,64 +4401,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="6"/>
+      <c r="AJ1" s="6"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
@@ -4483,11 +4466,11 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
       <c r="X2" s="4"/>
-      <c r="AB2" s="7" t="s">
+      <c r="AB2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
       <c r="AE2" s="3"/>
       <c r="AF2" s="3"/>
       <c r="AG2" s="3"/>
@@ -4513,7 +4496,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
@@ -4527,6 +4510,9 @@
       <c r="J3" t="s">
         <v>21</v>
       </c>
+      <c r="K3" t="s">
+        <v>23</v>
+      </c>
       <c r="L3" t="s">
         <v>14</v>
       </c>
@@ -4555,10 +4541,10 @@
         <v>24</v>
       </c>
       <c r="V3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="X3" t="s">
         <v>23</v>
@@ -4591,13 +4577,13 @@
         <v>18</v>
       </c>
       <c r="AI3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ3" t="s">
         <v>25</v>
       </c>
-      <c r="AJ3" t="s">
-        <v>28</v>
-      </c>
       <c r="AK3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="AL3" t="s">
         <v>14</v>
@@ -4608,17 +4594,38 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>28536</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>40109</v>
+        <v>7977</v>
       </c>
       <c r="D4">
-        <v>32460</v>
+        <v>20001</v>
+      </c>
+      <c r="E4">
+        <v>8000</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>7998</v>
+      </c>
+      <c r="H4">
+        <v>8000</v>
+      </c>
+      <c r="I4">
+        <v>48002</v>
+      </c>
+      <c r="J4">
+        <v>8033</v>
+      </c>
+      <c r="K4">
+        <v>7999</v>
       </c>
       <c r="L4" s="2">
-        <f t="shared" ref="L4:L13" si="0">AVERAGE(B4:D4) * 0.001</f>
-        <v>33.701666666666668</v>
+        <f>AVERAGE(B4:K4) * 0.001</f>
+        <v>11.601000000000001</v>
       </c>
       <c r="N4">
         <v>100</v>
@@ -4654,24 +4661,45 @@
         <v>7987</v>
       </c>
       <c r="Y4" s="2">
-        <f>AVERAGE(O4:X4)*0.001</f>
+        <f t="shared" ref="Y4:Y13" si="0">AVERAGE(O4:X4)*0.001</f>
         <v>8.6262999999999987</v>
       </c>
       <c r="AA4">
         <v>10</v>
       </c>
-      <c r="AB4">
-        <v>43990</v>
+      <c r="AB4" s="5">
+        <v>2046</v>
       </c>
       <c r="AC4">
-        <v>19993</v>
+        <v>2047</v>
       </c>
       <c r="AD4">
-        <v>16000</v>
+        <v>2056</v>
+      </c>
+      <c r="AE4">
+        <v>1961</v>
+      </c>
+      <c r="AF4">
+        <v>2004</v>
+      </c>
+      <c r="AG4">
+        <v>1995</v>
+      </c>
+      <c r="AH4">
+        <v>2992</v>
+      </c>
+      <c r="AI4">
+        <v>1955</v>
+      </c>
+      <c r="AJ4">
+        <v>1998</v>
+      </c>
+      <c r="AK4">
+        <v>1994</v>
       </c>
       <c r="AL4" s="2">
-        <f>AVERAGE(AB4:AD4)*0.001</f>
-        <v>26.661000000000001</v>
+        <f>AVERAGE(AB4:AK4)*0.001</f>
+        <v>2.1048</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
@@ -4679,17 +4707,38 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>55984</v>
+        <v>15625</v>
       </c>
       <c r="C5">
-        <v>55986</v>
+        <v>8001</v>
       </c>
       <c r="D5">
-        <v>52003</v>
+        <v>24000</v>
+      </c>
+      <c r="E5">
+        <v>7999</v>
+      </c>
+      <c r="F5">
+        <v>15621</v>
+      </c>
+      <c r="G5">
+        <v>12003</v>
+      </c>
+      <c r="H5">
+        <v>8001</v>
+      </c>
+      <c r="I5">
+        <v>16012</v>
+      </c>
+      <c r="J5">
+        <v>11967</v>
+      </c>
+      <c r="K5">
+        <v>16002</v>
       </c>
       <c r="L5" s="2">
-        <f t="shared" si="0"/>
-        <v>54.657666666666664</v>
+        <f>AVERAGE(B5:K5) * 0.001</f>
+        <v>13.523100000000001</v>
       </c>
       <c r="N5">
         <v>200</v>
@@ -4725,24 +4774,45 @@
         <v>17955</v>
       </c>
       <c r="Y5" s="2">
-        <f>AVERAGE(O5:X5)*0.001</f>
+        <f t="shared" si="0"/>
         <v>17.8095</v>
       </c>
       <c r="AA5">
         <v>20</v>
       </c>
-      <c r="AB5">
-        <v>95983</v>
+      <c r="AB5" s="5">
+        <v>4989</v>
       </c>
       <c r="AC5">
-        <v>39994</v>
+        <v>4934</v>
       </c>
       <c r="AD5">
-        <v>43985</v>
+        <v>4957</v>
+      </c>
+      <c r="AE5">
+        <v>4986</v>
+      </c>
+      <c r="AF5">
+        <v>3992</v>
+      </c>
+      <c r="AG5">
+        <v>4040</v>
+      </c>
+      <c r="AH5">
+        <v>3989</v>
+      </c>
+      <c r="AI5">
+        <v>4041</v>
+      </c>
+      <c r="AJ5">
+        <v>4991</v>
+      </c>
+      <c r="AK5">
+        <v>4986</v>
       </c>
       <c r="AL5" s="2">
-        <f t="shared" ref="AL5:AL13" si="1">AVERAGE(AB5:AD5)*0.001</f>
-        <v>59.987333333333339</v>
+        <f t="shared" ref="AL5:AL23" si="1">AVERAGE(AB5:AK5)*0.001</f>
+        <v>4.5905000000000005</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
@@ -4750,17 +4820,38 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>55988</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>59986</v>
+        <v>11999</v>
       </c>
       <c r="D6">
-        <v>55970</v>
+        <v>24003</v>
+      </c>
+      <c r="E6">
+        <v>12000</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>12001</v>
+      </c>
+      <c r="H6">
+        <v>11999</v>
+      </c>
+      <c r="I6">
+        <v>19987</v>
+      </c>
+      <c r="J6">
+        <v>20133</v>
+      </c>
+      <c r="K6">
+        <v>16030</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" si="0"/>
-        <v>57.314666666666668</v>
+        <f t="shared" ref="L6:L23" si="2">AVERAGE(B6:K6) * 0.001</f>
+        <v>12.815200000000001</v>
       </c>
       <c r="N6">
         <v>300</v>
@@ -4796,24 +4887,45 @@
         <v>24930</v>
       </c>
       <c r="Y6" s="2">
-        <f>AVERAGE(O6:X6)*0.001</f>
+        <f t="shared" si="0"/>
         <v>28.3626</v>
       </c>
       <c r="AA6">
         <v>30</v>
       </c>
-      <c r="AB6">
-        <v>123960</v>
+      <c r="AB6" s="5">
+        <v>5985</v>
       </c>
       <c r="AC6">
-        <v>111977</v>
+        <v>6030</v>
       </c>
       <c r="AD6">
-        <v>63988</v>
+        <v>5988</v>
+      </c>
+      <c r="AE6">
+        <v>5984</v>
+      </c>
+      <c r="AF6">
+        <v>6984</v>
+      </c>
+      <c r="AG6">
+        <v>5986</v>
+      </c>
+      <c r="AH6">
+        <v>6020</v>
+      </c>
+      <c r="AI6">
+        <v>5931</v>
+      </c>
+      <c r="AJ6">
+        <v>5944</v>
+      </c>
+      <c r="AK6">
+        <v>9974</v>
       </c>
       <c r="AL6" s="2">
         <f t="shared" si="1"/>
-        <v>99.975000000000009</v>
+        <v>6.4826000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
@@ -4821,17 +4933,38 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>67981</v>
+        <v>25336</v>
       </c>
       <c r="C7">
-        <v>79979</v>
+        <v>24001</v>
       </c>
       <c r="D7">
-        <v>71991</v>
+        <v>28029</v>
+      </c>
+      <c r="E7">
+        <v>28000</v>
+      </c>
+      <c r="F7">
+        <v>17543</v>
+      </c>
+      <c r="G7">
+        <v>19997</v>
+      </c>
+      <c r="H7">
+        <v>24000</v>
+      </c>
+      <c r="I7">
+        <v>27999</v>
+      </c>
+      <c r="J7">
+        <v>15997</v>
+      </c>
+      <c r="K7">
+        <v>16011</v>
       </c>
       <c r="L7" s="2">
-        <f t="shared" si="0"/>
-        <v>73.317000000000007</v>
+        <f t="shared" si="2"/>
+        <v>22.691299999999998</v>
       </c>
       <c r="N7">
         <v>400</v>
@@ -4867,24 +5000,45 @@
         <v>33914</v>
       </c>
       <c r="Y7" s="2">
-        <f>AVERAGE(O7:X7)*0.001</f>
+        <f t="shared" si="0"/>
         <v>32.864699999999999</v>
       </c>
       <c r="AA7">
         <v>40</v>
       </c>
-      <c r="AB7">
-        <v>75671</v>
+      <c r="AB7" s="5">
+        <v>7977</v>
       </c>
       <c r="AC7">
-        <v>75972</v>
+        <v>8930</v>
       </c>
       <c r="AD7">
-        <v>115965</v>
+        <v>8979</v>
+      </c>
+      <c r="AE7">
+        <v>7979</v>
+      </c>
+      <c r="AF7">
+        <v>7977</v>
+      </c>
+      <c r="AG7">
+        <v>7097</v>
+      </c>
+      <c r="AH7">
+        <v>7979</v>
+      </c>
+      <c r="AI7">
+        <v>10972</v>
+      </c>
+      <c r="AJ7">
+        <v>8016</v>
+      </c>
+      <c r="AK7">
+        <v>12967</v>
       </c>
       <c r="AL7" s="2">
         <f t="shared" si="1"/>
-        <v>89.202666666666673</v>
+        <v>8.8872999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
@@ -4892,17 +5046,38 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>79982</v>
+        <v>19998</v>
       </c>
       <c r="C8">
-        <v>79980</v>
+        <v>19998</v>
       </c>
       <c r="D8">
-        <v>75968</v>
+        <v>27964</v>
+      </c>
+      <c r="E8">
+        <v>28000</v>
+      </c>
+      <c r="F8">
+        <v>16099</v>
+      </c>
+      <c r="G8">
+        <v>16001</v>
+      </c>
+      <c r="H8">
+        <v>19999</v>
+      </c>
+      <c r="I8">
+        <v>28000</v>
+      </c>
+      <c r="J8">
+        <v>20003</v>
+      </c>
+      <c r="K8">
+        <v>19960</v>
       </c>
       <c r="L8" s="2">
-        <f t="shared" si="0"/>
-        <v>78.643333333333331</v>
+        <f t="shared" si="2"/>
+        <v>21.6022</v>
       </c>
       <c r="N8">
         <v>500</v>
@@ -4938,24 +5113,45 @@
         <v>40966</v>
       </c>
       <c r="Y8" s="2">
-        <f>AVERAGE(O8:X8)*0.001</f>
+        <f t="shared" si="0"/>
         <v>42.054400000000001</v>
       </c>
       <c r="AA8">
         <v>50</v>
       </c>
-      <c r="AB8">
-        <v>99769</v>
+      <c r="AB8" s="5">
+        <v>10918</v>
       </c>
       <c r="AC8">
-        <v>71980</v>
+        <v>11021</v>
       </c>
       <c r="AD8">
-        <v>76002</v>
+        <v>9932</v>
+      </c>
+      <c r="AE8">
+        <v>11971</v>
+      </c>
+      <c r="AF8">
+        <v>10920</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>10976</v>
+      </c>
+      <c r="AI8">
+        <v>9974</v>
+      </c>
+      <c r="AJ8">
+        <v>10966</v>
+      </c>
+      <c r="AK8">
+        <v>17952</v>
       </c>
       <c r="AL8" s="2">
         <f t="shared" si="1"/>
-        <v>82.583666666666673</v>
+        <v>10.463000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
@@ -4963,17 +5159,38 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>87997</v>
+        <v>20029</v>
       </c>
       <c r="C9">
-        <v>88418</v>
+        <v>20001</v>
       </c>
       <c r="D9">
-        <v>91976</v>
+        <v>24000</v>
+      </c>
+      <c r="E9">
+        <v>36000</v>
+      </c>
+      <c r="F9">
+        <v>15939</v>
+      </c>
+      <c r="G9">
+        <v>20029</v>
+      </c>
+      <c r="H9">
+        <v>27998</v>
+      </c>
+      <c r="I9">
+        <v>24000</v>
+      </c>
+      <c r="J9">
+        <v>27999</v>
+      </c>
+      <c r="K9">
+        <v>16001</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" si="0"/>
-        <v>89.463666666666668</v>
+        <f t="shared" si="2"/>
+        <v>23.1996</v>
       </c>
       <c r="N9">
         <v>600</v>
@@ -5009,24 +5226,45 @@
         <v>49870</v>
       </c>
       <c r="Y9" s="2">
-        <f>AVERAGE(O9:X9)*0.001</f>
+        <f t="shared" si="0"/>
         <v>54.9129</v>
       </c>
       <c r="AA9">
         <v>60</v>
       </c>
-      <c r="AB9">
-        <v>178042</v>
+      <c r="AB9" s="5">
+        <v>12965</v>
       </c>
       <c r="AC9">
-        <v>72034</v>
+        <v>12947</v>
       </c>
       <c r="AD9">
-        <v>83999</v>
+        <v>14013</v>
+      </c>
+      <c r="AE9">
+        <v>11965</v>
+      </c>
+      <c r="AF9">
+        <v>12965</v>
+      </c>
+      <c r="AG9">
+        <v>24039</v>
+      </c>
+      <c r="AH9">
+        <v>12969</v>
+      </c>
+      <c r="AI9">
+        <v>13011</v>
+      </c>
+      <c r="AJ9">
+        <v>12932</v>
+      </c>
+      <c r="AK9">
+        <v>14012</v>
       </c>
       <c r="AL9" s="2">
-        <f>AVERAGE(AB9:AD9)*0.001</f>
-        <v>111.35833333333333</v>
+        <f t="shared" si="1"/>
+        <v>14.181799999999999</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
@@ -5034,17 +5272,38 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>210310</v>
+        <v>23970</v>
       </c>
       <c r="C10">
-        <v>103993</v>
+        <v>24003</v>
       </c>
       <c r="D10">
-        <v>95668</v>
+        <v>32041</v>
+      </c>
+      <c r="E10">
+        <v>48001</v>
+      </c>
+      <c r="F10">
+        <v>19962</v>
+      </c>
+      <c r="G10">
+        <v>23971</v>
+      </c>
+      <c r="H10">
+        <v>32002</v>
+      </c>
+      <c r="I10">
+        <v>31999</v>
+      </c>
+      <c r="J10">
+        <v>23995</v>
+      </c>
+      <c r="K10">
+        <v>20007</v>
       </c>
       <c r="L10" s="2">
-        <f t="shared" si="0"/>
-        <v>136.65700000000001</v>
+        <f t="shared" si="2"/>
+        <v>27.995100000000001</v>
       </c>
       <c r="N10">
         <v>700</v>
@@ -5080,24 +5339,45 @@
         <v>58823</v>
       </c>
       <c r="Y10" s="2">
-        <f>AVERAGE(O10:X10)*0.001</f>
+        <f t="shared" si="0"/>
         <v>60.806300000000007</v>
       </c>
       <c r="AA10">
         <v>70</v>
       </c>
-      <c r="AB10">
-        <v>122890</v>
+      <c r="AB10" s="5">
+        <v>14962</v>
       </c>
       <c r="AC10">
-        <v>111396</v>
+        <v>14970</v>
       </c>
       <c r="AD10">
-        <v>104801</v>
+        <v>13962</v>
+      </c>
+      <c r="AE10">
+        <v>14961</v>
+      </c>
+      <c r="AF10">
+        <v>14960</v>
+      </c>
+      <c r="AG10">
+        <v>15011</v>
+      </c>
+      <c r="AH10">
+        <v>14951</v>
+      </c>
+      <c r="AI10">
+        <v>14956</v>
+      </c>
+      <c r="AJ10">
+        <v>15990</v>
+      </c>
+      <c r="AK10">
+        <v>15958</v>
       </c>
       <c r="AL10" s="2">
         <f t="shared" si="1"/>
-        <v>113.029</v>
+        <v>15.068100000000001</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
@@ -5105,17 +5385,38 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>151814</v>
+        <v>24001</v>
       </c>
       <c r="C11">
-        <v>201819</v>
+        <v>23998</v>
       </c>
       <c r="D11">
-        <v>112003</v>
+        <v>35964</v>
+      </c>
+      <c r="E11">
+        <v>24000</v>
+      </c>
+      <c r="F11">
+        <v>16075</v>
+      </c>
+      <c r="G11">
+        <v>24040</v>
+      </c>
+      <c r="H11">
+        <v>59998</v>
+      </c>
+      <c r="I11">
+        <v>24003</v>
+      </c>
+      <c r="J11">
+        <v>24002</v>
+      </c>
+      <c r="K11">
+        <v>20035</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" si="0"/>
-        <v>155.21199999999999</v>
+        <f t="shared" si="2"/>
+        <v>27.611599999999999</v>
       </c>
       <c r="N11">
         <v>800</v>
@@ -5151,24 +5452,45 @@
         <v>66832</v>
       </c>
       <c r="Y11" s="2">
-        <f>AVERAGE(O11:X11)*0.001</f>
+        <f t="shared" si="0"/>
         <v>68.180499999999995</v>
       </c>
       <c r="AA11">
         <v>80</v>
       </c>
-      <c r="AB11">
-        <v>132054</v>
+      <c r="AB11" s="5">
+        <v>16009</v>
       </c>
       <c r="AC11">
-        <v>104402</v>
+        <v>15914</v>
       </c>
       <c r="AD11">
-        <v>111305</v>
+        <v>16956</v>
+      </c>
+      <c r="AE11">
+        <v>15957</v>
+      </c>
+      <c r="AF11">
+        <v>16013</v>
+      </c>
+      <c r="AG11">
+        <v>16951</v>
+      </c>
+      <c r="AH11">
+        <v>16918</v>
+      </c>
+      <c r="AI11">
+        <v>15915</v>
+      </c>
+      <c r="AJ11">
+        <v>16955</v>
+      </c>
+      <c r="AK11">
+        <v>16952</v>
       </c>
       <c r="AL11" s="2">
         <f t="shared" si="1"/>
-        <v>115.92033333333333</v>
+        <v>16.454000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
@@ -5176,17 +5498,38 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>111669</v>
+        <v>24000</v>
       </c>
       <c r="C12">
-        <v>104445</v>
+        <v>32002</v>
       </c>
       <c r="D12">
-        <v>151852</v>
+        <v>40061</v>
+      </c>
+      <c r="E12">
+        <v>36009</v>
+      </c>
+      <c r="F12">
+        <v>15657</v>
+      </c>
+      <c r="G12">
+        <v>28000</v>
+      </c>
+      <c r="H12">
+        <v>48000</v>
+      </c>
+      <c r="I12">
+        <v>27998</v>
+      </c>
+      <c r="J12">
+        <v>32000</v>
+      </c>
+      <c r="K12">
+        <v>27956</v>
       </c>
       <c r="L12" s="2">
-        <f t="shared" si="0"/>
-        <v>122.65533333333333</v>
+        <f t="shared" si="2"/>
+        <v>31.168299999999999</v>
       </c>
       <c r="N12">
         <v>900</v>
@@ -5222,24 +5565,45 @@
         <v>74803</v>
       </c>
       <c r="Y12" s="2">
-        <f>AVERAGE(O12:X12)*0.001</f>
+        <f t="shared" si="0"/>
         <v>73.411000000000001</v>
       </c>
       <c r="AA12">
         <v>90</v>
       </c>
-      <c r="AB12">
-        <v>151312</v>
+      <c r="AB12" s="5">
+        <v>18897</v>
       </c>
       <c r="AC12">
-        <v>175861</v>
+        <v>19948</v>
       </c>
       <c r="AD12">
-        <v>115339</v>
+        <v>18947</v>
+      </c>
+      <c r="AE12">
+        <v>44880</v>
+      </c>
+      <c r="AF12">
+        <v>18943</v>
+      </c>
+      <c r="AG12">
+        <v>17956</v>
+      </c>
+      <c r="AH12">
+        <v>18998</v>
+      </c>
+      <c r="AI12">
+        <v>19007</v>
+      </c>
+      <c r="AJ12">
+        <v>18949</v>
+      </c>
+      <c r="AK12">
+        <v>20990</v>
       </c>
       <c r="AL12" s="2">
         <f t="shared" si="1"/>
-        <v>147.50399999999999</v>
+        <v>21.7515</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
@@ -5247,17 +5611,38 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>135701</v>
+        <v>27999</v>
       </c>
       <c r="C13">
-        <v>198926</v>
+        <v>36006</v>
       </c>
       <c r="D13">
-        <v>230884</v>
+        <v>39934</v>
+      </c>
+      <c r="E13">
+        <v>28001</v>
+      </c>
+      <c r="F13">
+        <v>15682</v>
+      </c>
+      <c r="G13">
+        <v>67959</v>
+      </c>
+      <c r="H13">
+        <v>39998</v>
+      </c>
+      <c r="I13">
+        <v>36163</v>
+      </c>
+      <c r="J13">
+        <v>32001</v>
+      </c>
+      <c r="K13">
+        <v>23999</v>
       </c>
       <c r="L13" s="2">
-        <f t="shared" si="0"/>
-        <v>188.50366666666667</v>
+        <f t="shared" si="2"/>
+        <v>34.7742</v>
       </c>
       <c r="N13">
         <v>1000</v>
@@ -5293,27 +5678,85 @@
         <v>84722</v>
       </c>
       <c r="Y13" s="2">
-        <f>AVERAGE(O13:X13)*0.001</f>
+        <f t="shared" si="0"/>
         <v>81.04610000000001</v>
       </c>
       <c r="AA13">
         <v>100</v>
       </c>
-      <c r="AB13">
-        <v>184343</v>
+      <c r="AB13" s="5">
+        <v>19990</v>
       </c>
       <c r="AC13">
-        <v>155428</v>
+        <v>20990</v>
       </c>
       <c r="AD13">
-        <v>146575</v>
+        <v>20898</v>
+      </c>
+      <c r="AE13">
+        <v>23936</v>
+      </c>
+      <c r="AF13">
+        <v>19950</v>
+      </c>
+      <c r="AG13">
+        <v>15360</v>
+      </c>
+      <c r="AH13">
+        <v>21892</v>
+      </c>
+      <c r="AI13">
+        <v>20932</v>
+      </c>
+      <c r="AJ13">
+        <v>19947</v>
+      </c>
+      <c r="AK13">
+        <v>22946</v>
       </c>
       <c r="AL13" s="2">
         <f t="shared" si="1"/>
-        <v>162.11533333333335</v>
+        <v>20.684099999999997</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>40010</v>
+      </c>
+      <c r="C14">
+        <v>59999</v>
+      </c>
+      <c r="D14">
+        <v>40000</v>
+      </c>
+      <c r="E14">
+        <v>44005</v>
+      </c>
+      <c r="F14">
+        <v>28617</v>
+      </c>
+      <c r="G14">
+        <v>32037</v>
+      </c>
+      <c r="H14">
+        <v>36005</v>
+      </c>
+      <c r="I14">
+        <v>36001</v>
+      </c>
+      <c r="J14">
+        <v>27999</v>
+      </c>
+      <c r="K14">
+        <v>28038</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="2"/>
+        <v>37.271099999999997</v>
+      </c>
       <c r="N14">
         <v>1100</v>
       </c>
@@ -5348,11 +5791,85 @@
         <v>92752</v>
       </c>
       <c r="Y14" s="2">
-        <f t="shared" ref="Y14:Y23" si="2">AVERAGE(O14:X14)*0.001</f>
+        <f t="shared" ref="Y14:Y23" si="3">AVERAGE(O14:X14)*0.001</f>
         <v>95.047800000000009</v>
+      </c>
+      <c r="AA14">
+        <v>110</v>
+      </c>
+      <c r="AB14" s="5">
+        <v>22934</v>
+      </c>
+      <c r="AC14">
+        <v>22890</v>
+      </c>
+      <c r="AD14">
+        <v>22986</v>
+      </c>
+      <c r="AE14">
+        <v>22971</v>
+      </c>
+      <c r="AF14">
+        <v>22937</v>
+      </c>
+      <c r="AG14">
+        <v>30794</v>
+      </c>
+      <c r="AH14">
+        <v>29969</v>
+      </c>
+      <c r="AI14">
+        <v>22924</v>
+      </c>
+      <c r="AJ14">
+        <v>22945</v>
+      </c>
+      <c r="AK14">
+        <v>23936</v>
+      </c>
+      <c r="AL14" s="2">
+        <f t="shared" si="1"/>
+        <v>24.528599999999997</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>35993</v>
+      </c>
+      <c r="C15">
+        <v>47997</v>
+      </c>
+      <c r="D15">
+        <v>60002</v>
+      </c>
+      <c r="E15">
+        <v>55999</v>
+      </c>
+      <c r="F15">
+        <v>15660</v>
+      </c>
+      <c r="G15">
+        <v>27999</v>
+      </c>
+      <c r="H15">
+        <v>44031</v>
+      </c>
+      <c r="I15">
+        <v>60000</v>
+      </c>
+      <c r="J15">
+        <v>35999</v>
+      </c>
+      <c r="K15">
+        <v>83996</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="2"/>
+        <v>46.767600000000002</v>
+      </c>
       <c r="N15">
         <v>1200</v>
       </c>
@@ -5387,11 +5904,85 @@
         <v>101728</v>
       </c>
       <c r="Y15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>101.28760000000001</v>
+      </c>
+      <c r="AA15">
+        <v>120</v>
+      </c>
+      <c r="AB15" s="5">
+        <v>23952</v>
+      </c>
+      <c r="AC15">
+        <v>24934</v>
+      </c>
+      <c r="AD15">
+        <v>24936</v>
+      </c>
+      <c r="AE15">
+        <v>25935</v>
+      </c>
+      <c r="AF15">
+        <v>24934</v>
+      </c>
+      <c r="AG15">
+        <v>20555</v>
+      </c>
+      <c r="AH15">
+        <v>24926</v>
+      </c>
+      <c r="AI15">
+        <v>50833</v>
+      </c>
+      <c r="AJ15">
+        <v>24939</v>
+      </c>
+      <c r="AK15">
+        <v>26926</v>
+      </c>
+      <c r="AL15" s="2">
+        <f t="shared" si="1"/>
+        <v>27.286999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>44000</v>
+      </c>
+      <c r="C16">
+        <v>40006</v>
+      </c>
+      <c r="D16">
+        <v>51999</v>
+      </c>
+      <c r="E16">
+        <v>58924</v>
+      </c>
+      <c r="F16">
+        <v>31243</v>
+      </c>
+      <c r="G16">
+        <v>32004</v>
+      </c>
+      <c r="H16">
+        <v>44031</v>
+      </c>
+      <c r="I16">
+        <v>60004</v>
+      </c>
+      <c r="J16">
+        <v>40001</v>
+      </c>
+      <c r="K16">
+        <v>64000</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="2"/>
+        <v>46.621199999999995</v>
+      </c>
       <c r="N16">
         <v>1300</v>
       </c>
@@ -5426,11 +6017,85 @@
         <v>3331750</v>
       </c>
       <c r="Y16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>432.28730000000002</v>
+      </c>
+      <c r="AA16">
+        <v>130</v>
+      </c>
+      <c r="AB16" s="5">
+        <v>51805</v>
+      </c>
+      <c r="AC16">
+        <v>45880</v>
+      </c>
+      <c r="AD16">
+        <v>49815</v>
+      </c>
+      <c r="AE16">
+        <v>26946</v>
+      </c>
+      <c r="AF16">
+        <v>41871</v>
+      </c>
+      <c r="AG16">
+        <v>30659</v>
+      </c>
+      <c r="AH16">
+        <v>31873</v>
+      </c>
+      <c r="AI16">
+        <v>33954</v>
+      </c>
+      <c r="AJ16">
+        <v>43838</v>
+      </c>
+      <c r="AK16">
+        <v>28920</v>
+      </c>
+      <c r="AL16" s="2">
+        <f t="shared" si="1"/>
+        <v>38.556100000000001</v>
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>40002</v>
+      </c>
+      <c r="C17">
+        <v>43991</v>
+      </c>
+      <c r="D17">
+        <v>44056</v>
+      </c>
+      <c r="E17">
+        <v>63816</v>
+      </c>
+      <c r="F17">
+        <v>15621</v>
+      </c>
+      <c r="G17">
+        <v>35961</v>
+      </c>
+      <c r="H17">
+        <v>59934</v>
+      </c>
+      <c r="I17">
+        <v>55997</v>
+      </c>
+      <c r="J17">
+        <v>32001</v>
+      </c>
+      <c r="K17">
+        <v>56997</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="2"/>
+        <v>44.837600000000002</v>
+      </c>
       <c r="N17">
         <v>1400</v>
       </c>
@@ -5465,11 +6130,85 @@
         <v>119678</v>
       </c>
       <c r="Y17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>115.3154</v>
+      </c>
+      <c r="AA17">
+        <v>140</v>
+      </c>
+      <c r="AB17" s="5">
+        <v>29922</v>
+      </c>
+      <c r="AC17">
+        <v>29971</v>
+      </c>
+      <c r="AD17">
+        <v>30918</v>
+      </c>
+      <c r="AE17">
+        <v>29921</v>
+      </c>
+      <c r="AF17">
+        <v>31879</v>
+      </c>
+      <c r="AG17">
+        <v>30278</v>
+      </c>
+      <c r="AH17">
+        <v>29969</v>
+      </c>
+      <c r="AI17">
+        <v>28928</v>
+      </c>
+      <c r="AJ17">
+        <v>38944</v>
+      </c>
+      <c r="AK17">
+        <v>30921</v>
+      </c>
+      <c r="AL17" s="2">
+        <f t="shared" si="1"/>
+        <v>31.165099999999999</v>
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>44028</v>
+      </c>
+      <c r="C18">
+        <v>44003</v>
+      </c>
+      <c r="D18">
+        <v>72000</v>
+      </c>
+      <c r="E18">
+        <v>36081</v>
+      </c>
+      <c r="F18">
+        <v>39852</v>
+      </c>
+      <c r="G18">
+        <v>44004</v>
+      </c>
+      <c r="H18">
+        <v>56002</v>
+      </c>
+      <c r="I18">
+        <v>64001</v>
+      </c>
+      <c r="J18">
+        <v>9999</v>
+      </c>
+      <c r="K18">
+        <v>58002</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="2"/>
+        <v>46.797199999999997</v>
+      </c>
       <c r="N18">
         <v>1500</v>
       </c>
@@ -5504,11 +6243,85 @@
         <v>128610</v>
       </c>
       <c r="Y18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>135.67929999999998</v>
+      </c>
+      <c r="AA18">
+        <v>150</v>
+      </c>
+      <c r="AB18" s="5">
+        <v>30974</v>
+      </c>
+      <c r="AC18">
+        <v>30915</v>
+      </c>
+      <c r="AD18">
+        <v>30917</v>
+      </c>
+      <c r="AE18">
+        <v>30909</v>
+      </c>
+      <c r="AF18">
+        <v>30917</v>
+      </c>
+      <c r="AG18">
+        <v>28397</v>
+      </c>
+      <c r="AH18">
+        <v>30923</v>
+      </c>
+      <c r="AI18">
+        <v>30919</v>
+      </c>
+      <c r="AJ18">
+        <v>30918</v>
+      </c>
+      <c r="AK18">
+        <v>32908</v>
+      </c>
+      <c r="AL18" s="2">
+        <f t="shared" si="1"/>
+        <v>30.869700000000002</v>
       </c>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>35967</v>
+      </c>
+      <c r="C19">
+        <v>63997</v>
+      </c>
+      <c r="D19">
+        <v>83344</v>
+      </c>
+      <c r="E19">
+        <v>46868</v>
+      </c>
+      <c r="F19">
+        <v>28395</v>
+      </c>
+      <c r="G19">
+        <v>60381</v>
+      </c>
+      <c r="H19">
+        <v>55997</v>
+      </c>
+      <c r="I19">
+        <v>51998</v>
+      </c>
+      <c r="J19">
+        <v>49065</v>
+      </c>
+      <c r="K19">
+        <v>55897</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="2"/>
+        <v>53.190899999999999</v>
+      </c>
       <c r="N19">
         <v>1600</v>
       </c>
@@ -5543,11 +6356,85 @@
         <v>135690</v>
       </c>
       <c r="Y19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>132.42620000000002</v>
+      </c>
+      <c r="AA19">
+        <v>160</v>
+      </c>
+      <c r="AB19" s="5">
+        <v>32908</v>
+      </c>
+      <c r="AC19">
+        <v>32914</v>
+      </c>
+      <c r="AD19">
+        <v>32912</v>
+      </c>
+      <c r="AE19">
+        <v>33916</v>
+      </c>
+      <c r="AF19">
+        <v>32912</v>
+      </c>
+      <c r="AG19">
+        <v>32362</v>
+      </c>
+      <c r="AH19">
+        <v>32911</v>
+      </c>
+      <c r="AI19">
+        <v>32859</v>
+      </c>
+      <c r="AJ19">
+        <v>33892</v>
+      </c>
+      <c r="AK19">
+        <v>34963</v>
+      </c>
+      <c r="AL19" s="2">
+        <f t="shared" si="1"/>
+        <v>33.254899999999999</v>
       </c>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>44033</v>
+      </c>
+      <c r="C20">
+        <v>60032</v>
+      </c>
+      <c r="D20">
+        <v>74000</v>
+      </c>
+      <c r="E20">
+        <v>45258</v>
+      </c>
+      <c r="F20">
+        <v>46321</v>
+      </c>
+      <c r="G20">
+        <v>72032</v>
+      </c>
+      <c r="H20">
+        <v>56000</v>
+      </c>
+      <c r="I20">
+        <v>44000</v>
+      </c>
+      <c r="J20">
+        <v>56643</v>
+      </c>
+      <c r="K20">
+        <v>56000</v>
+      </c>
+      <c r="L20" s="2">
+        <f t="shared" si="2"/>
+        <v>55.431900000000006</v>
+      </c>
       <c r="N20">
         <v>1700</v>
       </c>
@@ -5582,11 +6469,85 @@
         <v>145558</v>
       </c>
       <c r="Y20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>143.2165</v>
+      </c>
+      <c r="AA20">
+        <v>170</v>
+      </c>
+      <c r="AB20" s="5">
+        <v>34904</v>
+      </c>
+      <c r="AC20">
+        <v>34908</v>
+      </c>
+      <c r="AD20">
+        <v>34906</v>
+      </c>
+      <c r="AE20">
+        <v>34906</v>
+      </c>
+      <c r="AF20">
+        <v>34907</v>
+      </c>
+      <c r="AG20">
+        <v>30828</v>
+      </c>
+      <c r="AH20">
+        <v>33910</v>
+      </c>
+      <c r="AI20">
+        <v>38952</v>
+      </c>
+      <c r="AJ20">
+        <v>34915</v>
+      </c>
+      <c r="AK20">
+        <v>30769</v>
+      </c>
+      <c r="AL20" s="2">
+        <f t="shared" si="1"/>
+        <v>34.390500000000003</v>
       </c>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>51969</v>
+      </c>
+      <c r="C21">
+        <v>51970</v>
+      </c>
+      <c r="D21">
+        <v>67999</v>
+      </c>
+      <c r="E21">
+        <v>46873</v>
+      </c>
+      <c r="F21">
+        <v>38443</v>
+      </c>
+      <c r="G21">
+        <v>63970</v>
+      </c>
+      <c r="H21">
+        <v>56020</v>
+      </c>
+      <c r="I21">
+        <v>67999</v>
+      </c>
+      <c r="J21">
+        <v>56431</v>
+      </c>
+      <c r="K21">
+        <v>56020</v>
+      </c>
+      <c r="L21" s="2">
+        <f t="shared" si="2"/>
+        <v>55.769400000000005</v>
+      </c>
       <c r="N21">
         <v>1800</v>
       </c>
@@ -5621,11 +6582,85 @@
         <v>151553</v>
       </c>
       <c r="Y21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>154.12810000000002</v>
+      </c>
+      <c r="AA21">
+        <v>180</v>
+      </c>
+      <c r="AB21" s="5">
+        <v>38933</v>
+      </c>
+      <c r="AC21">
+        <v>35850</v>
+      </c>
+      <c r="AD21">
+        <v>36902</v>
+      </c>
+      <c r="AE21">
+        <v>36846</v>
+      </c>
+      <c r="AF21">
+        <v>36901</v>
+      </c>
+      <c r="AG21">
+        <v>40448</v>
+      </c>
+      <c r="AH21">
+        <v>37893</v>
+      </c>
+      <c r="AI21">
+        <v>36897</v>
+      </c>
+      <c r="AJ21">
+        <v>37896</v>
+      </c>
+      <c r="AK21">
+        <v>41115</v>
+      </c>
+      <c r="AL21" s="2">
+        <f t="shared" si="1"/>
+        <v>37.9681</v>
       </c>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>43997</v>
+      </c>
+      <c r="C22">
+        <v>71999</v>
+      </c>
+      <c r="D22">
+        <v>76000</v>
+      </c>
+      <c r="E22">
+        <v>53375</v>
+      </c>
+      <c r="F22">
+        <v>41006</v>
+      </c>
+      <c r="G22">
+        <v>72036</v>
+      </c>
+      <c r="H22">
+        <v>43997</v>
+      </c>
+      <c r="I22">
+        <v>56000</v>
+      </c>
+      <c r="J22">
+        <v>48240</v>
+      </c>
+      <c r="K22">
+        <v>43997</v>
+      </c>
+      <c r="L22" s="2">
+        <f t="shared" si="2"/>
+        <v>55.064699999999995</v>
+      </c>
       <c r="N22">
         <v>1900</v>
       </c>
@@ -5660,11 +6695,85 @@
         <v>153591</v>
       </c>
       <c r="Y22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>159.2218</v>
+      </c>
+      <c r="AA22">
+        <v>190</v>
+      </c>
+      <c r="AB22" s="5">
+        <v>41903</v>
+      </c>
+      <c r="AC22">
+        <v>39894</v>
+      </c>
+      <c r="AD22">
+        <v>39893</v>
+      </c>
+      <c r="AE22">
+        <v>38897</v>
+      </c>
+      <c r="AF22">
+        <v>38902</v>
+      </c>
+      <c r="AG22">
+        <v>38893</v>
+      </c>
+      <c r="AH22">
+        <v>38902</v>
+      </c>
+      <c r="AI22">
+        <v>37900</v>
+      </c>
+      <c r="AJ22">
+        <v>39857</v>
+      </c>
+      <c r="AK22">
+        <v>44337</v>
+      </c>
+      <c r="AL22" s="2">
+        <f t="shared" si="1"/>
+        <v>39.937800000000003</v>
       </c>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>52034</v>
+      </c>
+      <c r="C23">
+        <v>61534</v>
+      </c>
+      <c r="D23">
+        <v>64000</v>
+      </c>
+      <c r="E23">
+        <v>65100</v>
+      </c>
+      <c r="F23">
+        <v>34120</v>
+      </c>
+      <c r="G23">
+        <v>75976</v>
+      </c>
+      <c r="H23">
+        <v>52034</v>
+      </c>
+      <c r="I23">
+        <v>84000</v>
+      </c>
+      <c r="J23">
+        <v>60454</v>
+      </c>
+      <c r="K23">
+        <v>62034</v>
+      </c>
+      <c r="L23" s="2">
+        <f t="shared" si="2"/>
+        <v>61.128599999999999</v>
+      </c>
       <c r="N23">
         <v>2000</v>
       </c>
@@ -5699,58 +6808,95 @@
         <v>161889</v>
       </c>
       <c r="Y23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>166.41410000000002</v>
+      </c>
+      <c r="AA23">
+        <v>200</v>
+      </c>
+      <c r="AB23" s="5">
+        <v>42803</v>
+      </c>
+      <c r="AC23">
+        <v>40891</v>
+      </c>
+      <c r="AD23">
+        <v>41888</v>
+      </c>
+      <c r="AE23">
+        <v>40890</v>
+      </c>
+      <c r="AF23">
+        <v>41882</v>
+      </c>
+      <c r="AG23">
+        <v>40907</v>
+      </c>
+      <c r="AH23">
+        <v>39185</v>
+      </c>
+      <c r="AI23">
+        <v>41882</v>
+      </c>
+      <c r="AJ23">
+        <v>41921</v>
+      </c>
+      <c r="AK23">
+        <v>45347</v>
+      </c>
+      <c r="AL23" s="2">
+        <f t="shared" si="1"/>
+        <v>41.759599999999999</v>
       </c>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="6"/>
-      <c r="T24" s="6"/>
-      <c r="U24" s="6"/>
-      <c r="V24" s="6"/>
-      <c r="W24" s="6"/>
-      <c r="X24" s="6"/>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="6"/>
-      <c r="AA24" s="6"/>
-      <c r="AB24" s="6"/>
-      <c r="AC24" s="6"/>
-      <c r="AD24" s="6"/>
-      <c r="AE24" s="6"/>
-      <c r="AF24" s="6"/>
-      <c r="AG24" s="6"/>
-      <c r="AH24" s="6"/>
-      <c r="AI24" s="6"/>
-      <c r="AJ24" s="6"/>
-      <c r="AK24" s="6"/>
-      <c r="AL24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="7"/>
+      <c r="AB24" s="7"/>
+      <c r="AC24" s="7"/>
+      <c r="AD24" s="7"/>
+      <c r="AE24" s="7"/>
+      <c r="AF24" s="7"/>
+      <c r="AG24" s="7"/>
+      <c r="AH24" s="7"/>
+      <c r="AI24" s="7"/>
+      <c r="AJ24" s="7"/>
+      <c r="AK24" s="7"/>
+      <c r="AL24" s="7"/>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -5758,11 +6904,11 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
-      <c r="O26" s="7" t="s">
+      <c r="O26" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="7"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
@@ -5770,11 +6916,11 @@
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
       <c r="X26" s="4"/>
-      <c r="AB26" s="7" t="s">
+      <c r="AB26" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AC26" s="7"/>
-      <c r="AD26" s="7"/>
+      <c r="AC26" s="8"/>
+      <c r="AD26" s="8"/>
       <c r="AE26" s="3"/>
       <c r="AF26" s="3"/>
       <c r="AG26" s="3"/>
@@ -5904,7 +7050,7 @@
         <v>125751</v>
       </c>
       <c r="L28" s="2">
-        <f t="shared" ref="L28:L37" si="3">AVERAGE(B28:D28)*0.001</f>
+        <f t="shared" ref="L28:L37" si="4">AVERAGE(B28:D28)*0.001</f>
         <v>134.86266666666666</v>
       </c>
       <c r="N28">
@@ -5920,7 +7066,7 @@
         <v>233865</v>
       </c>
       <c r="Y28" s="2">
-        <f>AVERAGE(O28:Q28)*0.001</f>
+        <f t="shared" ref="Y28:Y37" si="5">AVERAGE(O28:Q28)*0.001</f>
         <v>234.39099999999999</v>
       </c>
       <c r="AA28">
@@ -5954,7 +7100,7 @@
         <v>132925</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>125.26166666666667</v>
       </c>
       <c r="N29">
@@ -5970,7 +7116,7 @@
         <v>423914</v>
       </c>
       <c r="Y29" s="2">
-        <f>AVERAGE(O29:Q29)*0.001</f>
+        <f t="shared" si="5"/>
         <v>424.8896666666667</v>
       </c>
       <c r="AA29">
@@ -5986,7 +7132,7 @@
         <v>136593</v>
       </c>
       <c r="AL29" s="2">
-        <f t="shared" ref="AL29:AL37" si="4">AVERAGE(AB29:AD29)*0.001</f>
+        <f t="shared" ref="AL29:AL37" si="6">AVERAGE(AB29:AD29)*0.001</f>
         <v>145.03633333333335</v>
       </c>
     </row>
@@ -6004,7 +7150,7 @@
         <v>122929</v>
       </c>
       <c r="L30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>124.26833333333333</v>
       </c>
       <c r="N30">
@@ -6020,7 +7166,7 @@
         <v>613485</v>
       </c>
       <c r="Y30" s="2">
-        <f>AVERAGE(O30:Q30)*0.001</f>
+        <f t="shared" si="5"/>
         <v>611.08666666666659</v>
       </c>
       <c r="AA30">
@@ -6036,7 +7182,7 @@
         <v>167517</v>
       </c>
       <c r="AL30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>150.358</v>
       </c>
     </row>
@@ -6054,7 +7200,7 @@
         <v>124692</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>129.18133333333333</v>
       </c>
       <c r="N31">
@@ -6070,7 +7216,7 @@
         <v>812709</v>
       </c>
       <c r="Y31" s="2">
-        <f>AVERAGE(O31:Q31)*0.001</f>
+        <f t="shared" si="5"/>
         <v>805.37800000000004</v>
       </c>
       <c r="AA31">
@@ -6086,7 +7232,7 @@
         <v>173899</v>
       </c>
       <c r="AL31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>160.57566666666665</v>
       </c>
     </row>
@@ -6104,7 +7250,7 @@
         <v>117933</v>
       </c>
       <c r="L32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>122.92933333333333</v>
       </c>
       <c r="N32">
@@ -6120,7 +7266,7 @@
         <v>131466</v>
       </c>
       <c r="Y32" s="2">
-        <f>AVERAGE(O32:Q32)*0.001</f>
+        <f t="shared" si="5"/>
         <v>434.23633333333333</v>
       </c>
       <c r="AA32">
@@ -6136,7 +7282,7 @@
         <v>163908</v>
       </c>
       <c r="AL32" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>140.95233333333334</v>
       </c>
     </row>
@@ -6154,7 +7300,7 @@
         <v>151912</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>174.56766666666667</v>
       </c>
       <c r="N33">
@@ -6170,7 +7316,7 @@
         <v>1263482</v>
       </c>
       <c r="Y33" s="2">
-        <f>AVERAGE(O33:Q33)*0.001</f>
+        <f t="shared" si="5"/>
         <v>1226.0323333333333</v>
       </c>
       <c r="AA33">
@@ -6186,7 +7332,7 @@
         <v>167902</v>
       </c>
       <c r="AL33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>136.45833333333334</v>
       </c>
     </row>
@@ -6204,7 +7350,7 @@
         <v>131925</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>136.91533333333334</v>
       </c>
       <c r="N34">
@@ -6220,7 +7366,7 @@
         <v>1374165</v>
       </c>
       <c r="Y34" s="2">
-        <f>AVERAGE(O34:Q34)*0.001</f>
+        <f t="shared" si="5"/>
         <v>1360.6426666666669</v>
       </c>
       <c r="AA34">
@@ -6236,7 +7382,7 @@
         <v>150912</v>
       </c>
       <c r="AL34" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>136.88466666666665</v>
       </c>
     </row>
@@ -6254,7 +7400,7 @@
         <v>118932</v>
       </c>
       <c r="L35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>131.59133333333335</v>
       </c>
       <c r="N35">
@@ -6270,7 +7416,7 @@
         <v>1535428</v>
       </c>
       <c r="Y35" s="2">
-        <f>AVERAGE(O35:Q35)*0.001</f>
+        <f t="shared" si="5"/>
         <v>1547.5319999999999</v>
       </c>
       <c r="AA35">
@@ -6286,7 +7432,7 @@
         <v>158343</v>
       </c>
       <c r="AL35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>171.71299999999999</v>
       </c>
     </row>
@@ -6304,7 +7450,7 @@
         <v>147916</v>
       </c>
       <c r="L36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>130.31100000000001</v>
       </c>
       <c r="N36">
@@ -6320,7 +7466,7 @@
         <v>1728210</v>
       </c>
       <c r="Y36" s="2">
-        <f>AVERAGE(O36:Q36)*0.001</f>
+        <f t="shared" si="5"/>
         <v>1753.8453333333332</v>
       </c>
       <c r="AA36">
@@ -6336,7 +7482,7 @@
         <v>170901</v>
       </c>
       <c r="AL36" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>141.53033333333335</v>
       </c>
     </row>
@@ -6354,7 +7500,7 @@
         <v>122932</v>
       </c>
       <c r="L37" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>131.501</v>
       </c>
       <c r="N37">
@@ -6370,7 +7516,7 @@
         <v>1944963</v>
       </c>
       <c r="Y37" s="2">
-        <f>AVERAGE(O37:Q37)*0.001</f>
+        <f t="shared" si="5"/>
         <v>1956.0963333333334</v>
       </c>
       <c r="AA37">
@@ -6386,7 +7532,7 @@
         <v>173900</v>
       </c>
       <c r="AL37" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>138.25300000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Increased range of test values
</commit_message>
<xml_diff>
--- a/Documentation/Graphs.xlsx
+++ b/Documentation/Graphs.xlsx
@@ -393,11 +393,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190169472"/>
-        <c:axId val="190171008"/>
+        <c:axId val="202097024"/>
+        <c:axId val="202098560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190169472"/>
+        <c:axId val="202097024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -440,7 +440,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190171008"/>
+        <c:crossAx val="202098560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -448,7 +448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190171008"/>
+        <c:axId val="202098560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -499,7 +499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190169472"/>
+        <c:crossAx val="202097024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -776,11 +776,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190450688"/>
-        <c:axId val="190477056"/>
+        <c:axId val="202378240"/>
+        <c:axId val="202404608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190450688"/>
+        <c:axId val="202378240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -823,7 +823,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190477056"/>
+        <c:crossAx val="202404608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -831,7 +831,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190477056"/>
+        <c:axId val="202404608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,7 +882,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190450688"/>
+        <c:crossAx val="202378240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1159,11 +1159,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190506880"/>
-        <c:axId val="190508416"/>
+        <c:axId val="202434432"/>
+        <c:axId val="202435968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190506880"/>
+        <c:axId val="202434432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,7 +1206,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190508416"/>
+        <c:crossAx val="202435968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1214,7 +1214,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190508416"/>
+        <c:axId val="202435968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1265,7 +1265,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190506880"/>
+        <c:crossAx val="202434432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1542,11 +1542,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190854272"/>
-        <c:axId val="190856192"/>
+        <c:axId val="202781824"/>
+        <c:axId val="202783744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190854272"/>
+        <c:axId val="202781824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1629,7 +1629,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190856192"/>
+        <c:crossAx val="202783744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1637,7 +1637,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190856192"/>
+        <c:axId val="202783744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1714,7 +1714,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190854272"/>
+        <c:crossAx val="202781824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2001,11 +2001,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190894848"/>
-        <c:axId val="190896768"/>
+        <c:axId val="202818304"/>
+        <c:axId val="202820224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190894848"/>
+        <c:axId val="202818304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2088,7 +2088,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190896768"/>
+        <c:crossAx val="202820224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2096,7 +2096,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190896768"/>
+        <c:axId val="202820224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2173,7 +2173,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190894848"/>
+        <c:crossAx val="202818304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2450,11 +2450,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="190677376"/>
-        <c:axId val="190679296"/>
+        <c:axId val="202604928"/>
+        <c:axId val="202606848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="190677376"/>
+        <c:axId val="202604928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2537,7 +2537,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190679296"/>
+        <c:crossAx val="202606848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2545,7 +2545,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190679296"/>
+        <c:axId val="202606848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2636,7 +2636,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="190677376"/>
+        <c:crossAx val="202604928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3161,7 +3161,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4385,7 +4385,7 @@
   <dimension ref="A1:AL37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added all values for increased range (PSO_rastrigin)
</commit_message>
<xml_diff>
--- a/Documentation/Graphs.xlsx
+++ b/Documentation/Graphs.xlsx
@@ -393,11 +393,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="202097024"/>
-        <c:axId val="202098560"/>
+        <c:axId val="204390784"/>
+        <c:axId val="204392320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="202097024"/>
+        <c:axId val="204390784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -440,7 +440,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202098560"/>
+        <c:crossAx val="204392320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -448,7 +448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202098560"/>
+        <c:axId val="204392320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -499,7 +499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202097024"/>
+        <c:crossAx val="204390784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -776,11 +776,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="202378240"/>
-        <c:axId val="202404608"/>
+        <c:axId val="204672000"/>
+        <c:axId val="204698368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="202378240"/>
+        <c:axId val="204672000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -823,7 +823,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202404608"/>
+        <c:crossAx val="204698368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -831,7 +831,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202404608"/>
+        <c:axId val="204698368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,7 +882,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202378240"/>
+        <c:crossAx val="204672000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1159,11 +1159,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="202434432"/>
-        <c:axId val="202435968"/>
+        <c:axId val="204728192"/>
+        <c:axId val="204729728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="202434432"/>
+        <c:axId val="204728192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,7 +1206,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202435968"/>
+        <c:crossAx val="204729728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1214,7 +1214,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202435968"/>
+        <c:axId val="204729728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1265,7 +1265,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202434432"/>
+        <c:crossAx val="204728192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1488,7 +1488,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>rastrigin!$L$28:$L$37</c:f>
+              <c:f>rastrigin!$L$58:$L$67</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1542,11 +1542,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="202781824"/>
-        <c:axId val="202783744"/>
+        <c:axId val="205077120"/>
+        <c:axId val="205079296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="202781824"/>
+        <c:axId val="205077120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1583,6 +1583,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1629,7 +1630,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202783744"/>
+        <c:crossAx val="205079296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1637,7 +1638,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202783744"/>
+        <c:axId val="205079296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1674,6 +1675,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1714,7 +1716,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202781824"/>
+        <c:crossAx val="205077120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1728,6 +1730,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1947,7 +1950,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>rastrigin!$Y$28:$Y$37</c:f>
+              <c:f>rastrigin!$Y$58:$Y$67</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2001,11 +2004,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="202818304"/>
-        <c:axId val="202820224"/>
+        <c:axId val="205113984"/>
+        <c:axId val="205124352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="202818304"/>
+        <c:axId val="205113984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2042,6 +2045,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2088,7 +2092,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202820224"/>
+        <c:crossAx val="205124352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2096,7 +2100,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202820224"/>
+        <c:axId val="205124352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2133,6 +2137,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2173,7 +2178,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202818304"/>
+        <c:crossAx val="205113984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2187,6 +2192,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2396,7 +2402,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>rastrigin!$AL$28:$AL$37</c:f>
+              <c:f>rastrigin!$AL$58:$AL$67</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2450,11 +2456,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="202604928"/>
-        <c:axId val="202606848"/>
+        <c:axId val="204900608"/>
+        <c:axId val="204910976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="202604928"/>
+        <c:axId val="204900608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2491,6 +2497,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2537,7 +2544,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202606848"/>
+        <c:crossAx val="204910976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2545,7 +2552,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202606848"/>
+        <c:axId val="204910976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2596,6 +2603,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2636,7 +2644,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202604928"/>
+        <c:crossAx val="204900608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2650,6 +2658,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2817,13 +2826,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>800099</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2847,13 +2856,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2877,13 +2886,13 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>419101</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>200027</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3161,7 +3170,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4382,10 +4391,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL37"/>
+  <dimension ref="A1:AL67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AL51" sqref="AL51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4811,7 +4820,7 @@
         <v>4986</v>
       </c>
       <c r="AL5" s="2">
-        <f t="shared" ref="AL5:AL23" si="1">AVERAGE(AB5:AK5)*0.001</f>
+        <f t="shared" ref="AL5:AL53" si="1">AVERAGE(AB5:AK5)*0.001</f>
         <v>4.5905000000000005</v>
       </c>
     </row>
@@ -4850,7 +4859,7 @@
         <v>16030</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" ref="L6:L23" si="2">AVERAGE(B6:K6) * 0.001</f>
+        <f t="shared" ref="L6:L27" si="2">AVERAGE(B6:K6) * 0.001</f>
         <v>12.815200000000001</v>
       </c>
       <c r="N6">
@@ -5791,7 +5800,7 @@
         <v>92752</v>
       </c>
       <c r="Y14" s="2">
-        <f t="shared" ref="Y14:Y23" si="3">AVERAGE(O14:X14)*0.001</f>
+        <f t="shared" ref="Y14:Y33" si="3">AVERAGE(O14:X14)*0.001</f>
         <v>95.047800000000009</v>
       </c>
       <c r="AA14">
@@ -6850,688 +6859,2422 @@
       </c>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="7"/>
-      <c r="Y24" s="7"/>
-      <c r="Z24" s="7"/>
-      <c r="AA24" s="7"/>
-      <c r="AB24" s="7"/>
-      <c r="AC24" s="7"/>
-      <c r="AD24" s="7"/>
-      <c r="AE24" s="7"/>
-      <c r="AF24" s="7"/>
-      <c r="AG24" s="7"/>
-      <c r="AH24" s="7"/>
-      <c r="AI24" s="7"/>
-      <c r="AJ24" s="7"/>
-      <c r="AK24" s="7"/>
-      <c r="AL24" s="7"/>
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>48006</v>
+      </c>
+      <c r="C24">
+        <v>40034</v>
+      </c>
+      <c r="D24">
+        <v>43995</v>
+      </c>
+      <c r="E24">
+        <v>40000</v>
+      </c>
+      <c r="F24">
+        <v>43997</v>
+      </c>
+      <c r="G24">
+        <v>48016</v>
+      </c>
+      <c r="H24">
+        <v>48042</v>
+      </c>
+      <c r="I24">
+        <v>43991</v>
+      </c>
+      <c r="J24">
+        <v>43991</v>
+      </c>
+      <c r="K24">
+        <v>44025</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="2"/>
+        <v>44.409700000000001</v>
+      </c>
+      <c r="N24">
+        <v>2100</v>
+      </c>
+      <c r="O24">
+        <v>258947</v>
+      </c>
+      <c r="P24">
+        <v>240005</v>
+      </c>
+      <c r="Q24">
+        <v>213485</v>
+      </c>
+      <c r="R24">
+        <v>200883</v>
+      </c>
+      <c r="S24">
+        <v>226662</v>
+      </c>
+      <c r="T24">
+        <v>216900</v>
+      </c>
+      <c r="U24">
+        <v>193057</v>
+      </c>
+      <c r="V24">
+        <v>198491</v>
+      </c>
+      <c r="W24">
+        <v>196079</v>
+      </c>
+      <c r="X24">
+        <v>264478</v>
+      </c>
+      <c r="Y24" s="2">
+        <f t="shared" si="3"/>
+        <v>220.89870000000002</v>
+      </c>
+      <c r="AA24">
+        <v>210</v>
+      </c>
+      <c r="AB24" s="5">
+        <v>57578</v>
+      </c>
+      <c r="AC24">
+        <v>55998</v>
+      </c>
+      <c r="AD24">
+        <v>75994</v>
+      </c>
+      <c r="AE24">
+        <v>85423</v>
+      </c>
+      <c r="AF24">
+        <v>59993</v>
+      </c>
+      <c r="AG24">
+        <v>55960</v>
+      </c>
+      <c r="AH24">
+        <v>55960</v>
+      </c>
+      <c r="AI24">
+        <v>69251</v>
+      </c>
+      <c r="AJ24">
+        <v>64010</v>
+      </c>
+      <c r="AK24">
+        <v>60039</v>
+      </c>
+      <c r="AL24" s="2">
+        <f t="shared" si="1"/>
+        <v>64.020600000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>47954</v>
+      </c>
+      <c r="C25">
+        <v>24207</v>
+      </c>
+      <c r="D25">
+        <v>40100</v>
+      </c>
+      <c r="E25">
+        <v>27766</v>
+      </c>
+      <c r="F25">
+        <v>32115</v>
+      </c>
+      <c r="G25">
+        <v>47993</v>
+      </c>
+      <c r="H25">
+        <v>48006</v>
+      </c>
+      <c r="I25">
+        <v>31900</v>
+      </c>
+      <c r="J25">
+        <v>31900</v>
+      </c>
+      <c r="K25">
+        <v>32310</v>
+      </c>
+      <c r="L25" s="2">
+        <f t="shared" si="2"/>
+        <v>36.4251</v>
+      </c>
+      <c r="N25">
+        <v>2200</v>
+      </c>
+      <c r="O25">
+        <v>217829</v>
+      </c>
+      <c r="P25">
+        <v>224787</v>
+      </c>
+      <c r="Q25">
+        <v>189430</v>
+      </c>
+      <c r="R25">
+        <v>226179</v>
+      </c>
+      <c r="S25">
+        <v>227541</v>
+      </c>
+      <c r="T25">
+        <v>216639</v>
+      </c>
+      <c r="U25">
+        <v>200132</v>
+      </c>
+      <c r="V25">
+        <v>221421</v>
+      </c>
+      <c r="W25">
+        <v>240493</v>
+      </c>
+      <c r="X25">
+        <v>226069</v>
+      </c>
+      <c r="Y25" s="2">
+        <f t="shared" si="3"/>
+        <v>219.05199999999999</v>
+      </c>
+      <c r="AA25">
+        <v>220</v>
+      </c>
+      <c r="AB25" s="5">
+        <v>52000</v>
+      </c>
+      <c r="AC25">
+        <v>56000</v>
+      </c>
+      <c r="AD25">
+        <v>112884</v>
+      </c>
+      <c r="AE25">
+        <v>43785</v>
+      </c>
+      <c r="AF25">
+        <v>60010</v>
+      </c>
+      <c r="AG25">
+        <v>52000</v>
+      </c>
+      <c r="AH25">
+        <v>52000</v>
+      </c>
+      <c r="AI25">
+        <v>43758</v>
+      </c>
+      <c r="AJ25">
+        <v>67993</v>
+      </c>
+      <c r="AK25">
+        <v>67996</v>
+      </c>
+      <c r="AL25" s="2">
+        <f t="shared" si="1"/>
+        <v>60.842599999999997</v>
+      </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="O26" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
-      <c r="W26" s="3"/>
-      <c r="X26" s="4"/>
-      <c r="AB26" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC26" s="8"/>
-      <c r="AD26" s="8"/>
-      <c r="AE26" s="3"/>
-      <c r="AF26" s="3"/>
-      <c r="AG26" s="3"/>
-      <c r="AH26" s="3"/>
-      <c r="AI26" s="3"/>
-      <c r="AJ26" s="3"/>
-      <c r="AK26" s="3"/>
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>52000</v>
+      </c>
+      <c r="C26">
+        <v>46901</v>
+      </c>
+      <c r="D26">
+        <v>31243</v>
+      </c>
+      <c r="E26">
+        <v>36285</v>
+      </c>
+      <c r="F26">
+        <v>46865</v>
+      </c>
+      <c r="G26">
+        <v>56869</v>
+      </c>
+      <c r="H26">
+        <v>51998</v>
+      </c>
+      <c r="I26">
+        <v>52084</v>
+      </c>
+      <c r="J26">
+        <v>52084</v>
+      </c>
+      <c r="K26">
+        <v>56084</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="2"/>
+        <v>48.241300000000003</v>
+      </c>
+      <c r="N26">
+        <v>2300</v>
+      </c>
+      <c r="O26">
+        <v>246187</v>
+      </c>
+      <c r="P26">
+        <v>245336</v>
+      </c>
+      <c r="Q26">
+        <v>199020</v>
+      </c>
+      <c r="R26">
+        <v>219657</v>
+      </c>
+      <c r="S26">
+        <v>214203</v>
+      </c>
+      <c r="T26">
+        <v>205879</v>
+      </c>
+      <c r="U26">
+        <v>232201</v>
+      </c>
+      <c r="V26">
+        <v>238119</v>
+      </c>
+      <c r="W26">
+        <v>232318</v>
+      </c>
+      <c r="X26">
+        <v>272110</v>
+      </c>
+      <c r="Y26" s="2">
+        <f t="shared" si="3"/>
+        <v>230.50300000000001</v>
+      </c>
+      <c r="AA26">
+        <v>230</v>
+      </c>
+      <c r="AB26" s="5">
+        <v>50348</v>
+      </c>
+      <c r="AC26">
+        <v>52000</v>
+      </c>
+      <c r="AD26">
+        <v>72011</v>
+      </c>
+      <c r="AE26">
+        <v>56369</v>
+      </c>
+      <c r="AF26">
+        <v>87994</v>
+      </c>
+      <c r="AG26">
+        <v>58361</v>
+      </c>
+      <c r="AH26">
+        <v>58361</v>
+      </c>
+      <c r="AI26">
+        <v>52783</v>
+      </c>
+      <c r="AJ26">
+        <v>68231</v>
+      </c>
+      <c r="AK26">
+        <v>68288</v>
+      </c>
+      <c r="AL26" s="2">
+        <f t="shared" si="1"/>
+        <v>62.474600000000002</v>
+      </c>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" t="s">
-        <v>18</v>
-      </c>
-      <c r="I27" t="s">
-        <v>20</v>
-      </c>
-      <c r="J27" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L27" t="s">
-        <v>14</v>
-      </c>
-      <c r="N27" t="s">
-        <v>6</v>
-      </c>
-      <c r="O27" t="s">
-        <v>0</v>
-      </c>
-      <c r="P27" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>3</v>
-      </c>
-      <c r="R27" t="s">
-        <v>17</v>
-      </c>
-      <c r="S27" t="s">
-        <v>19</v>
-      </c>
-      <c r="T27" t="s">
-        <v>18</v>
-      </c>
-      <c r="U27" t="s">
-        <v>20</v>
-      </c>
-      <c r="V27" t="s">
-        <v>21</v>
-      </c>
-      <c r="W27" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC27" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD27" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE27" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG27" t="s">
-        <v>19</v>
-      </c>
-      <c r="AH27" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI27" t="s">
-        <v>20</v>
-      </c>
-      <c r="AJ27" t="s">
-        <v>21</v>
-      </c>
-      <c r="AK27" t="s">
-        <v>23</v>
-      </c>
-      <c r="AL27" t="s">
-        <v>14</v>
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>51998</v>
+      </c>
+      <c r="C27">
+        <v>48292</v>
+      </c>
+      <c r="D27">
+        <v>44972</v>
+      </c>
+      <c r="E27">
+        <v>63983</v>
+      </c>
+      <c r="F27">
+        <v>39451</v>
+      </c>
+      <c r="G27">
+        <v>56305</v>
+      </c>
+      <c r="H27">
+        <v>51991</v>
+      </c>
+      <c r="I27">
+        <v>44154</v>
+      </c>
+      <c r="J27">
+        <v>44154</v>
+      </c>
+      <c r="K27">
+        <v>60276</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="2"/>
+        <v>50.557600000000001</v>
+      </c>
+      <c r="N27">
+        <v>2400</v>
+      </c>
+      <c r="O27">
+        <v>242285</v>
+      </c>
+      <c r="P27">
+        <v>212308</v>
+      </c>
+      <c r="Q27">
+        <v>239332</v>
+      </c>
+      <c r="R27">
+        <v>258271</v>
+      </c>
+      <c r="S27">
+        <v>205225</v>
+      </c>
+      <c r="T27">
+        <v>213730</v>
+      </c>
+      <c r="U27">
+        <v>250274</v>
+      </c>
+      <c r="V27">
+        <v>228135</v>
+      </c>
+      <c r="W27">
+        <v>229465</v>
+      </c>
+      <c r="X27">
+        <v>262772</v>
+      </c>
+      <c r="Y27" s="2">
+        <f t="shared" si="3"/>
+        <v>234.17970000000003</v>
+      </c>
+      <c r="AA27">
+        <v>240</v>
+      </c>
+      <c r="AB27" s="5">
+        <v>46437</v>
+      </c>
+      <c r="AC27">
+        <v>52000</v>
+      </c>
+      <c r="AD27">
+        <v>75956</v>
+      </c>
+      <c r="AE27">
+        <v>55204</v>
+      </c>
+      <c r="AF27">
+        <v>73009</v>
+      </c>
+      <c r="AG27">
+        <v>50419</v>
+      </c>
+      <c r="AH27">
+        <v>50419</v>
+      </c>
+      <c r="AI27">
+        <v>71234</v>
+      </c>
+      <c r="AJ27">
+        <v>59441</v>
+      </c>
+      <c r="AK27">
+        <v>67121</v>
+      </c>
+      <c r="AL27" s="2">
+        <f t="shared" si="1"/>
+        <v>60.124000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="B28">
-        <v>140917</v>
-      </c>
-      <c r="C28">
-        <v>137920</v>
-      </c>
-      <c r="D28">
-        <v>125751</v>
-      </c>
-      <c r="L28" s="2">
-        <f t="shared" ref="L28:L37" si="4">AVERAGE(B28:D28)*0.001</f>
-        <v>134.86266666666666</v>
-      </c>
+      <c r="L28" s="2"/>
       <c r="N28">
-        <v>100</v>
+        <v>2500</v>
       </c>
       <c r="O28">
-        <v>230055</v>
+        <v>257365</v>
       </c>
       <c r="P28">
-        <v>239253</v>
+        <v>227291</v>
       </c>
       <c r="Q28">
-        <v>233865</v>
+        <v>269524</v>
+      </c>
+      <c r="R28">
+        <v>217055</v>
+      </c>
+      <c r="S28">
+        <v>231090</v>
+      </c>
+      <c r="T28">
+        <v>257656</v>
+      </c>
+      <c r="U28">
+        <v>237703</v>
+      </c>
+      <c r="V28">
+        <v>221198</v>
+      </c>
+      <c r="W28">
+        <v>228030</v>
+      </c>
+      <c r="X28">
+        <v>319382</v>
       </c>
       <c r="Y28" s="2">
-        <f t="shared" ref="Y28:Y37" si="5">AVERAGE(O28:Q28)*0.001</f>
-        <v>234.39099999999999</v>
+        <f t="shared" si="3"/>
+        <v>246.6294</v>
       </c>
       <c r="AA28">
-        <v>10</v>
-      </c>
-      <c r="AB28">
-        <v>309475</v>
+        <v>250</v>
+      </c>
+      <c r="AB28" s="5">
+        <v>61005</v>
       </c>
       <c r="AC28">
-        <v>243165</v>
+        <v>46854</v>
       </c>
       <c r="AD28">
-        <v>290178</v>
+        <v>78469</v>
+      </c>
+      <c r="AE28">
+        <v>62826</v>
+      </c>
+      <c r="AF28">
+        <v>68018</v>
+      </c>
+      <c r="AG28">
+        <v>58487</v>
+      </c>
+      <c r="AH28">
+        <v>58487</v>
+      </c>
+      <c r="AI28">
+        <v>62915</v>
+      </c>
+      <c r="AJ28">
+        <v>58340</v>
+      </c>
+      <c r="AK28">
+        <v>62956</v>
       </c>
       <c r="AL28" s="2">
-        <f>AVERAGE(AB28:AD28)*0.001</f>
-        <v>280.93933333333331</v>
+        <f t="shared" si="1"/>
+        <v>61.835699999999996</v>
       </c>
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="L29" s="2"/>
+      <c r="N29">
+        <v>2600</v>
+      </c>
+      <c r="O29">
+        <v>360025</v>
+      </c>
+      <c r="P29">
+        <v>246697</v>
+      </c>
+      <c r="Q29">
+        <v>305798</v>
+      </c>
+      <c r="R29">
+        <v>241045</v>
+      </c>
+      <c r="S29">
+        <v>247896</v>
+      </c>
+      <c r="T29">
+        <v>234370</v>
+      </c>
+      <c r="U29">
+        <v>236514</v>
+      </c>
+      <c r="V29">
+        <v>240876</v>
+      </c>
+      <c r="W29">
+        <v>245887</v>
+      </c>
+      <c r="X29">
+        <v>251518</v>
+      </c>
+      <c r="Y29" s="2">
+        <f t="shared" si="3"/>
+        <v>261.06260000000003</v>
+      </c>
+      <c r="AA29">
+        <v>260</v>
+      </c>
+      <c r="AB29" s="5">
+        <v>51336</v>
+      </c>
+      <c r="AC29">
+        <v>62612</v>
+      </c>
+      <c r="AD29">
+        <v>85674</v>
+      </c>
+      <c r="AE29">
+        <v>68359</v>
+      </c>
+      <c r="AF29">
+        <v>67944</v>
+      </c>
+      <c r="AG29">
+        <v>52704</v>
+      </c>
+      <c r="AH29">
+        <v>52704</v>
+      </c>
+      <c r="AI29">
+        <v>59558</v>
+      </c>
+      <c r="AJ29">
+        <v>56737</v>
+      </c>
+      <c r="AK29">
+        <v>62747</v>
+      </c>
+      <c r="AL29" s="2">
+        <f t="shared" si="1"/>
+        <v>62.037500000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L30" s="2"/>
+      <c r="N30">
+        <v>2700</v>
+      </c>
+      <c r="O30">
+        <v>341103</v>
+      </c>
+      <c r="P30">
+        <v>253282</v>
+      </c>
+      <c r="Q30">
+        <v>246661</v>
+      </c>
+      <c r="R30">
+        <v>240143</v>
+      </c>
+      <c r="S30">
+        <v>266783</v>
+      </c>
+      <c r="T30">
+        <v>268202</v>
+      </c>
+      <c r="U30">
+        <v>276150</v>
+      </c>
+      <c r="V30">
+        <v>286135</v>
+      </c>
+      <c r="W30">
+        <v>249058</v>
+      </c>
+      <c r="X30">
+        <v>300464</v>
+      </c>
+      <c r="Y30" s="2">
+        <f t="shared" si="3"/>
+        <v>272.79809999999998</v>
+      </c>
+      <c r="AA30">
+        <v>270</v>
+      </c>
+      <c r="AB30" s="5">
+        <v>61736</v>
+      </c>
+      <c r="AC30">
+        <v>53886</v>
+      </c>
+      <c r="AD30">
+        <v>65262</v>
+      </c>
+      <c r="AE30">
+        <v>74271</v>
+      </c>
+      <c r="AF30">
+        <v>74289</v>
+      </c>
+      <c r="AG30">
+        <v>58994</v>
+      </c>
+      <c r="AH30">
+        <v>58994</v>
+      </c>
+      <c r="AI30">
+        <v>66645</v>
+      </c>
+      <c r="AJ30">
+        <v>71383</v>
+      </c>
+      <c r="AK30">
+        <v>65178</v>
+      </c>
+      <c r="AL30" s="2">
+        <f t="shared" si="1"/>
+        <v>65.063800000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L31" s="2"/>
+      <c r="N31">
+        <v>2800</v>
+      </c>
+      <c r="O31">
+        <v>298892</v>
+      </c>
+      <c r="P31">
+        <v>239225</v>
+      </c>
+      <c r="Q31">
+        <v>264837</v>
+      </c>
+      <c r="R31">
+        <v>296111</v>
+      </c>
+      <c r="S31">
+        <v>282489</v>
+      </c>
+      <c r="T31">
+        <v>296057</v>
+      </c>
+      <c r="U31">
+        <v>283676</v>
+      </c>
+      <c r="V31">
+        <v>282936</v>
+      </c>
+      <c r="W31">
+        <v>302433</v>
+      </c>
+      <c r="X31">
+        <v>275191</v>
+      </c>
+      <c r="Y31" s="2">
+        <f t="shared" si="3"/>
+        <v>282.18470000000002</v>
+      </c>
+      <c r="AA31">
+        <v>280</v>
+      </c>
+      <c r="AB31" s="5">
+        <v>59825</v>
+      </c>
+      <c r="AC31">
+        <v>68976</v>
+      </c>
+      <c r="AD31">
+        <v>103051</v>
+      </c>
+      <c r="AE31">
+        <v>64691</v>
+      </c>
+      <c r="AF31">
+        <v>76001</v>
+      </c>
+      <c r="AG31">
+        <v>53634</v>
+      </c>
+      <c r="AH31">
+        <v>53634</v>
+      </c>
+      <c r="AI31">
+        <v>64846</v>
+      </c>
+      <c r="AJ31">
+        <v>69539</v>
+      </c>
+      <c r="AK31">
+        <v>70821</v>
+      </c>
+      <c r="AL31" s="2">
+        <f t="shared" si="1"/>
+        <v>68.501800000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L32" s="2"/>
+      <c r="N32">
+        <v>2900</v>
+      </c>
+      <c r="O32">
+        <v>298641</v>
+      </c>
+      <c r="P32">
+        <v>279656</v>
+      </c>
+      <c r="Q32">
+        <v>307095</v>
+      </c>
+      <c r="R32">
+        <v>312206</v>
+      </c>
+      <c r="S32">
+        <v>261470</v>
+      </c>
+      <c r="T32">
+        <v>258273</v>
+      </c>
+      <c r="U32">
+        <v>263091</v>
+      </c>
+      <c r="V32">
+        <v>259445</v>
+      </c>
+      <c r="W32">
+        <v>255404</v>
+      </c>
+      <c r="X32">
+        <v>343337</v>
+      </c>
+      <c r="Y32" s="2">
+        <f t="shared" si="3"/>
+        <v>283.86180000000002</v>
+      </c>
+      <c r="AA32">
+        <v>290</v>
+      </c>
+      <c r="AB32" s="5">
+        <v>61772</v>
+      </c>
+      <c r="AC32">
+        <v>62186</v>
+      </c>
+      <c r="AD32">
+        <v>93480</v>
+      </c>
+      <c r="AE32">
+        <v>72091</v>
+      </c>
+      <c r="AF32">
+        <v>74119</v>
+      </c>
+      <c r="AG32">
+        <v>69122</v>
+      </c>
+      <c r="AH32">
+        <v>69122</v>
+      </c>
+      <c r="AI32">
+        <v>61975</v>
+      </c>
+      <c r="AJ32">
+        <v>74702</v>
+      </c>
+      <c r="AK32">
+        <v>70776</v>
+      </c>
+      <c r="AL32" s="2">
+        <f t="shared" si="1"/>
+        <v>70.9345</v>
+      </c>
+    </row>
+    <row r="33" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L33" s="2"/>
+      <c r="N33">
+        <v>3000</v>
+      </c>
+      <c r="O33">
+        <v>313339</v>
+      </c>
+      <c r="P33">
+        <v>300984</v>
+      </c>
+      <c r="Q33">
+        <v>262895</v>
+      </c>
+      <c r="R33">
+        <v>264841</v>
+      </c>
+      <c r="S33">
+        <v>276973</v>
+      </c>
+      <c r="T33">
+        <v>262308</v>
+      </c>
+      <c r="U33">
+        <v>257283</v>
+      </c>
+      <c r="V33">
+        <v>272724</v>
+      </c>
+      <c r="W33">
+        <v>266221</v>
+      </c>
+      <c r="X33">
+        <v>347569</v>
+      </c>
+      <c r="Y33" s="2">
+        <f t="shared" si="3"/>
+        <v>282.51370000000003</v>
+      </c>
+      <c r="AA33">
+        <v>300</v>
+      </c>
+      <c r="AB33" s="5">
+        <v>61831</v>
+      </c>
+      <c r="AC33">
+        <v>68511</v>
+      </c>
+      <c r="AD33">
+        <v>91596</v>
+      </c>
+      <c r="AE33">
+        <v>63518</v>
+      </c>
+      <c r="AF33">
+        <v>80501</v>
+      </c>
+      <c r="AG33">
+        <v>82250</v>
+      </c>
+      <c r="AH33">
+        <v>82250</v>
+      </c>
+      <c r="AI33">
+        <v>71598</v>
+      </c>
+      <c r="AJ33">
+        <v>76687</v>
+      </c>
+      <c r="AK33">
+        <v>92210</v>
+      </c>
+      <c r="AL33" s="2">
+        <f t="shared" si="1"/>
+        <v>77.095200000000006</v>
+      </c>
+    </row>
+    <row r="34" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="AA34">
+        <v>310</v>
+      </c>
+      <c r="AB34" s="5">
+        <v>65850</v>
+      </c>
+      <c r="AC34">
+        <v>69856</v>
+      </c>
+      <c r="AD34">
+        <v>90429</v>
+      </c>
+      <c r="AE34">
+        <v>87607</v>
+      </c>
+      <c r="AF34">
+        <v>84683</v>
+      </c>
+      <c r="AG34">
+        <v>94101</v>
+      </c>
+      <c r="AH34">
+        <v>94101</v>
+      </c>
+      <c r="AI34">
+        <v>83273</v>
+      </c>
+      <c r="AJ34">
+        <v>78888</v>
+      </c>
+      <c r="AK34">
+        <v>77872</v>
+      </c>
+      <c r="AL34" s="2">
+        <f t="shared" si="1"/>
+        <v>82.665999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="AA35">
+        <v>320</v>
+      </c>
+      <c r="AB35" s="5">
+        <v>71317</v>
+      </c>
+      <c r="AC35">
+        <v>64399</v>
+      </c>
+      <c r="AD35">
+        <v>132856</v>
+      </c>
+      <c r="AE35">
+        <v>83193</v>
+      </c>
+      <c r="AF35">
+        <v>72007</v>
+      </c>
+      <c r="AG35">
+        <v>88000</v>
+      </c>
+      <c r="AH35">
+        <v>88000</v>
+      </c>
+      <c r="AI35">
+        <v>83070</v>
+      </c>
+      <c r="AJ35">
+        <v>89506</v>
+      </c>
+      <c r="AK35">
+        <v>81965</v>
+      </c>
+      <c r="AL35" s="2">
+        <f t="shared" si="1"/>
+        <v>85.431300000000007</v>
+      </c>
+    </row>
+    <row r="36" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L36" s="2"/>
+      <c r="Y36" s="2"/>
+      <c r="AA36">
+        <v>330</v>
+      </c>
+      <c r="AB36" s="5">
+        <v>70906</v>
+      </c>
+      <c r="AC36">
+        <v>71498</v>
+      </c>
+      <c r="AD36">
+        <v>87313</v>
+      </c>
+      <c r="AE36">
+        <v>74882</v>
+      </c>
+      <c r="AF36">
+        <v>83970</v>
+      </c>
+      <c r="AG36">
+        <v>79999</v>
+      </c>
+      <c r="AH36">
+        <v>79999</v>
+      </c>
+      <c r="AI36">
+        <v>82867</v>
+      </c>
+      <c r="AJ36">
+        <v>86317</v>
+      </c>
+      <c r="AK36">
+        <v>82286</v>
+      </c>
+      <c r="AL36" s="2">
+        <f t="shared" si="1"/>
+        <v>80.003699999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L37" s="2"/>
+      <c r="Y37" s="2"/>
+      <c r="AA37">
+        <v>340</v>
+      </c>
+      <c r="AB37" s="5">
+        <v>76081</v>
+      </c>
+      <c r="AC37">
+        <v>92283</v>
+      </c>
+      <c r="AD37">
+        <v>86277</v>
+      </c>
+      <c r="AE37">
+        <v>76380</v>
+      </c>
+      <c r="AF37">
+        <v>73863</v>
+      </c>
+      <c r="AG37">
+        <v>81926</v>
+      </c>
+      <c r="AH37">
+        <v>81926</v>
+      </c>
+      <c r="AI37">
+        <v>85216</v>
+      </c>
+      <c r="AJ37">
+        <v>85638</v>
+      </c>
+      <c r="AK37">
+        <v>73576</v>
+      </c>
+      <c r="AL37" s="2">
+        <f t="shared" si="1"/>
+        <v>81.316600000000008</v>
+      </c>
+    </row>
+    <row r="38" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L38" s="2"/>
+      <c r="Y38" s="2"/>
+      <c r="AA38">
+        <v>350</v>
+      </c>
+      <c r="AB38" s="5">
+        <v>71934</v>
+      </c>
+      <c r="AC38">
+        <v>107703</v>
+      </c>
+      <c r="AD38">
+        <v>91191</v>
+      </c>
+      <c r="AE38">
+        <v>80930</v>
+      </c>
+      <c r="AF38">
+        <v>98595</v>
+      </c>
+      <c r="AG38">
+        <v>94421</v>
+      </c>
+      <c r="AH38">
+        <v>94421</v>
+      </c>
+      <c r="AI38">
+        <v>90610</v>
+      </c>
+      <c r="AJ38">
+        <v>91610</v>
+      </c>
+      <c r="AK38">
+        <v>71948</v>
+      </c>
+      <c r="AL38" s="2">
+        <f t="shared" si="1"/>
+        <v>89.336300000000008</v>
+      </c>
+    </row>
+    <row r="39" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L39" s="2"/>
+      <c r="Y39" s="2"/>
+      <c r="AA39">
+        <v>360</v>
+      </c>
+      <c r="AB39" s="5">
+        <v>80065</v>
+      </c>
+      <c r="AC39">
+        <v>106585</v>
+      </c>
+      <c r="AD39">
+        <v>110995</v>
+      </c>
+      <c r="AE39">
+        <v>93373</v>
+      </c>
+      <c r="AF39">
+        <v>97206</v>
+      </c>
+      <c r="AG39">
+        <v>110419</v>
+      </c>
+      <c r="AH39">
+        <v>110419</v>
+      </c>
+      <c r="AI39">
+        <v>91916</v>
+      </c>
+      <c r="AJ39">
+        <v>81291</v>
+      </c>
+      <c r="AK39">
+        <v>82031</v>
+      </c>
+      <c r="AL39" s="2">
+        <f t="shared" si="1"/>
+        <v>96.43</v>
+      </c>
+    </row>
+    <row r="40" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L40" s="2"/>
+      <c r="Y40" s="2"/>
+      <c r="AA40">
+        <v>370</v>
+      </c>
+      <c r="AB40" s="5">
+        <v>73455</v>
+      </c>
+      <c r="AC40">
+        <v>96062</v>
+      </c>
+      <c r="AD40">
+        <v>140469</v>
+      </c>
+      <c r="AE40">
+        <v>111937</v>
+      </c>
+      <c r="AF40">
+        <v>117099</v>
+      </c>
+      <c r="AG40">
+        <v>104768</v>
+      </c>
+      <c r="AH40">
+        <v>104768</v>
+      </c>
+      <c r="AI40">
+        <v>100241</v>
+      </c>
+      <c r="AJ40">
+        <v>81583</v>
+      </c>
+      <c r="AK40">
+        <v>74183</v>
+      </c>
+      <c r="AL40" s="2">
+        <f t="shared" si="1"/>
+        <v>100.45650000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L41" s="2"/>
+      <c r="Y41" s="2"/>
+      <c r="AA41">
+        <v>380</v>
+      </c>
+      <c r="AB41" s="5">
+        <v>81128</v>
+      </c>
+      <c r="AC41">
+        <v>93709</v>
+      </c>
+      <c r="AD41">
+        <v>123478</v>
+      </c>
+      <c r="AE41">
+        <v>112002</v>
+      </c>
+      <c r="AF41">
+        <v>88485</v>
+      </c>
+      <c r="AG41">
+        <v>92660</v>
+      </c>
+      <c r="AH41">
+        <v>92660</v>
+      </c>
+      <c r="AI41">
+        <v>99625</v>
+      </c>
+      <c r="AJ41">
+        <v>91081</v>
+      </c>
+      <c r="AK41">
+        <v>82294</v>
+      </c>
+      <c r="AL41" s="2">
+        <f t="shared" si="1"/>
+        <v>95.712199999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L42" s="2"/>
+      <c r="Y42" s="2"/>
+      <c r="AA42">
+        <v>390</v>
+      </c>
+      <c r="AB42" s="5">
+        <v>115308</v>
+      </c>
+      <c r="AC42">
+        <v>113940</v>
+      </c>
+      <c r="AD42">
+        <v>113500</v>
+      </c>
+      <c r="AE42">
+        <v>114746</v>
+      </c>
+      <c r="AF42">
+        <v>90216</v>
+      </c>
+      <c r="AG42">
+        <v>95804</v>
+      </c>
+      <c r="AH42">
+        <v>95804</v>
+      </c>
+      <c r="AI42">
+        <v>106568</v>
+      </c>
+      <c r="AJ42">
+        <v>128840</v>
+      </c>
+      <c r="AK42">
+        <v>89749</v>
+      </c>
+      <c r="AL42" s="2">
+        <f t="shared" si="1"/>
+        <v>106.44750000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L43" s="2"/>
+      <c r="Y43" s="2"/>
+      <c r="AA43">
+        <v>400</v>
+      </c>
+      <c r="AB43" s="5">
+        <v>179602</v>
+      </c>
+      <c r="AC43">
+        <v>102625</v>
+      </c>
+      <c r="AD43">
+        <v>114494</v>
+      </c>
+      <c r="AE43">
+        <v>110824</v>
+      </c>
+      <c r="AF43">
+        <v>94862</v>
+      </c>
+      <c r="AG43">
+        <v>92577</v>
+      </c>
+      <c r="AH43">
+        <v>92577</v>
+      </c>
+      <c r="AI43">
+        <v>102968</v>
+      </c>
+      <c r="AJ43">
+        <v>95496</v>
+      </c>
+      <c r="AK43">
+        <v>92545</v>
+      </c>
+      <c r="AL43" s="2">
+        <f t="shared" si="1"/>
+        <v>107.857</v>
+      </c>
+    </row>
+    <row r="44" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L44" s="2"/>
+      <c r="Y44" s="2"/>
+      <c r="AA44">
+        <v>410</v>
+      </c>
+      <c r="AB44" s="5">
+        <v>92006</v>
+      </c>
+      <c r="AC44">
+        <v>107550</v>
+      </c>
+      <c r="AD44">
+        <v>108002</v>
+      </c>
+      <c r="AE44">
+        <v>104727</v>
+      </c>
+      <c r="AF44">
+        <v>82518</v>
+      </c>
+      <c r="AG44">
+        <v>92661</v>
+      </c>
+      <c r="AH44">
+        <v>92661</v>
+      </c>
+      <c r="AI44">
+        <v>95258</v>
+      </c>
+      <c r="AJ44">
+        <v>92388</v>
+      </c>
+      <c r="AK44">
+        <v>82272</v>
+      </c>
+      <c r="AL44" s="2">
+        <f t="shared" si="1"/>
+        <v>95.004300000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L45" s="2"/>
+      <c r="Y45" s="2"/>
+      <c r="AA45">
+        <v>420</v>
+      </c>
+      <c r="AB45" s="5">
+        <v>84708</v>
+      </c>
+      <c r="AC45">
+        <v>108140</v>
+      </c>
+      <c r="AD45">
+        <v>112001</v>
+      </c>
+      <c r="AE45">
+        <v>114598</v>
+      </c>
+      <c r="AF45">
+        <v>96127</v>
+      </c>
+      <c r="AG45">
+        <v>101589</v>
+      </c>
+      <c r="AH45">
+        <v>101589</v>
+      </c>
+      <c r="AI45">
+        <v>102645</v>
+      </c>
+      <c r="AJ45">
+        <v>124074</v>
+      </c>
+      <c r="AK45">
+        <v>92531</v>
+      </c>
+      <c r="AL45" s="2">
+        <f t="shared" si="1"/>
+        <v>103.8002</v>
+      </c>
+    </row>
+    <row r="46" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L46" s="2"/>
+      <c r="Y46" s="2"/>
+      <c r="AA46">
+        <v>430</v>
+      </c>
+      <c r="AB46" s="5">
+        <v>96724</v>
+      </c>
+      <c r="AC46">
+        <v>100091</v>
+      </c>
+      <c r="AD46">
+        <v>136972</v>
+      </c>
+      <c r="AE46">
+        <v>119066</v>
+      </c>
+      <c r="AF46">
+        <v>101095</v>
+      </c>
+      <c r="AG46">
+        <v>118982</v>
+      </c>
+      <c r="AH46">
+        <v>118982</v>
+      </c>
+      <c r="AI46">
+        <v>92703</v>
+      </c>
+      <c r="AJ46">
+        <v>132035</v>
+      </c>
+      <c r="AK46">
+        <v>90832</v>
+      </c>
+      <c r="AL46" s="2">
+        <f t="shared" si="1"/>
+        <v>110.7482</v>
+      </c>
+    </row>
+    <row r="47" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L47" s="2"/>
+      <c r="Y47" s="2"/>
+      <c r="AA47">
+        <v>440</v>
+      </c>
+      <c r="AB47" s="5">
+        <v>95433</v>
+      </c>
+      <c r="AC47">
+        <v>118984</v>
+      </c>
+      <c r="AD47">
+        <v>143148</v>
+      </c>
+      <c r="AE47">
+        <v>118496</v>
+      </c>
+      <c r="AF47">
+        <v>105396</v>
+      </c>
+      <c r="AG47">
+        <v>133709</v>
+      </c>
+      <c r="AH47">
+        <v>133709</v>
+      </c>
+      <c r="AI47">
+        <v>102290</v>
+      </c>
+      <c r="AJ47">
+        <v>91346</v>
+      </c>
+      <c r="AK47">
+        <v>98850</v>
+      </c>
+      <c r="AL47" s="2">
+        <f t="shared" si="1"/>
+        <v>114.13610000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L48" s="2"/>
+      <c r="Y48" s="2"/>
+      <c r="AA48">
+        <v>450</v>
+      </c>
+      <c r="AB48" s="5">
+        <v>101534</v>
+      </c>
+      <c r="AC48">
+        <v>108123</v>
+      </c>
+      <c r="AD48">
+        <v>108000</v>
+      </c>
+      <c r="AE48">
+        <v>115164</v>
+      </c>
+      <c r="AF48">
+        <v>109979</v>
+      </c>
+      <c r="AG48">
+        <v>142957</v>
+      </c>
+      <c r="AH48">
+        <v>142957</v>
+      </c>
+      <c r="AI48">
+        <v>97531</v>
+      </c>
+      <c r="AJ48">
+        <v>102762</v>
+      </c>
+      <c r="AK48">
+        <v>103114</v>
+      </c>
+      <c r="AL48" s="2">
+        <f t="shared" si="1"/>
+        <v>113.21210000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L49" s="2"/>
+      <c r="Y49" s="2"/>
+      <c r="AA49">
+        <v>460</v>
+      </c>
+      <c r="AB49" s="5">
+        <v>91399</v>
+      </c>
+      <c r="AC49">
+        <v>98169</v>
+      </c>
+      <c r="AD49">
+        <v>107553</v>
+      </c>
+      <c r="AE49">
+        <v>112806</v>
+      </c>
+      <c r="AF49">
+        <v>121840</v>
+      </c>
+      <c r="AG49">
+        <v>122978</v>
+      </c>
+      <c r="AH49">
+        <v>122978</v>
+      </c>
+      <c r="AI49">
+        <v>96422</v>
+      </c>
+      <c r="AJ49">
+        <v>138068</v>
+      </c>
+      <c r="AK49">
+        <v>99137</v>
+      </c>
+      <c r="AL49" s="2">
+        <f t="shared" si="1"/>
+        <v>111.13500000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L50" s="2"/>
+      <c r="Y50" s="2"/>
+      <c r="AA50">
+        <v>470</v>
+      </c>
+      <c r="AB50" s="5">
+        <v>102212</v>
+      </c>
+      <c r="AC50">
+        <v>103193</v>
+      </c>
+      <c r="AD50">
+        <v>103012</v>
+      </c>
+      <c r="AE50">
+        <v>186211</v>
+      </c>
+      <c r="AF50">
+        <v>94922</v>
+      </c>
+      <c r="AG50">
+        <v>119156</v>
+      </c>
+      <c r="AH50">
+        <v>119156</v>
+      </c>
+      <c r="AI50">
+        <v>119373</v>
+      </c>
+      <c r="AJ50">
+        <v>139164</v>
+      </c>
+      <c r="AK50">
+        <v>103215</v>
+      </c>
+      <c r="AL50" s="2">
+        <f t="shared" si="1"/>
+        <v>118.9614</v>
+      </c>
+    </row>
+    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L51" s="2"/>
+      <c r="Y51" s="2"/>
+      <c r="AA51">
+        <v>480</v>
+      </c>
+      <c r="AB51" s="5">
+        <v>109152</v>
+      </c>
+      <c r="AC51">
+        <v>107634</v>
+      </c>
+      <c r="AD51">
+        <v>103117</v>
+      </c>
+      <c r="AE51">
+        <v>132038</v>
+      </c>
+      <c r="AF51">
+        <v>111005</v>
+      </c>
+      <c r="AG51">
+        <v>140370</v>
+      </c>
+      <c r="AH51">
+        <v>140370</v>
+      </c>
+      <c r="AI51">
+        <v>117372</v>
+      </c>
+      <c r="AJ51">
+        <v>133501</v>
+      </c>
+      <c r="AK51">
+        <v>134578</v>
+      </c>
+      <c r="AL51" s="2">
+        <f t="shared" si="1"/>
+        <v>122.91370000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L52" s="2"/>
+      <c r="Y52" s="2"/>
+      <c r="AA52">
+        <v>490</v>
+      </c>
+      <c r="AB52" s="5">
+        <v>105031</v>
+      </c>
+      <c r="AC52">
+        <v>103148</v>
+      </c>
+      <c r="AD52">
+        <v>112434</v>
+      </c>
+      <c r="AE52">
+        <v>108482</v>
+      </c>
+      <c r="AF52">
+        <v>107353</v>
+      </c>
+      <c r="AG52">
+        <v>149289</v>
+      </c>
+      <c r="AH52">
+        <v>149289</v>
+      </c>
+      <c r="AI52">
+        <v>115022</v>
+      </c>
+      <c r="AJ52">
+        <v>135247</v>
+      </c>
+      <c r="AK52">
+        <v>120193</v>
+      </c>
+      <c r="AL52" s="2">
+        <f t="shared" si="1"/>
+        <v>120.5488</v>
+      </c>
+    </row>
+    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L53" s="2"/>
+      <c r="Y53" s="2"/>
+      <c r="AA53">
+        <v>500</v>
+      </c>
+      <c r="AB53" s="5">
+        <v>107972</v>
+      </c>
+      <c r="AC53">
+        <v>104321</v>
+      </c>
+      <c r="AD53">
+        <v>102721</v>
+      </c>
+      <c r="AE53">
+        <v>132440</v>
+      </c>
+      <c r="AF53">
+        <v>101108</v>
+      </c>
+      <c r="AG53">
+        <v>112489</v>
+      </c>
+      <c r="AH53">
+        <v>112489</v>
+      </c>
+      <c r="AI53">
+        <v>107036</v>
+      </c>
+      <c r="AJ53">
+        <v>138323</v>
+      </c>
+      <c r="AK53">
+        <v>115410</v>
+      </c>
+      <c r="AL53" s="2">
+        <f t="shared" si="1"/>
+        <v>113.43089999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="7"/>
+      <c r="S54" s="7"/>
+      <c r="T54" s="7"/>
+      <c r="U54" s="7"/>
+      <c r="V54" s="7"/>
+      <c r="W54" s="7"/>
+      <c r="X54" s="7"/>
+      <c r="Y54" s="7"/>
+      <c r="Z54" s="7"/>
+      <c r="AA54" s="7"/>
+      <c r="AB54" s="7"/>
+      <c r="AC54" s="7"/>
+      <c r="AD54" s="7"/>
+      <c r="AE54" s="7"/>
+      <c r="AF54" s="7"/>
+      <c r="AG54" s="7"/>
+      <c r="AH54" s="7"/>
+      <c r="AI54" s="7"/>
+      <c r="AJ54" s="7"/>
+      <c r="AK54" s="7"/>
+      <c r="AL54" s="7"/>
+    </row>
+    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B56" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="O56" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="8"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3"/>
+      <c r="T56" s="3"/>
+      <c r="U56" s="3"/>
+      <c r="V56" s="3"/>
+      <c r="W56" s="3"/>
+      <c r="X56" s="4"/>
+      <c r="AB56" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC56" s="8"/>
+      <c r="AD56" s="8"/>
+      <c r="AE56" s="3"/>
+      <c r="AF56" s="3"/>
+      <c r="AG56" s="3"/>
+      <c r="AH56" s="3"/>
+      <c r="AI56" s="3"/>
+      <c r="AJ56" s="3"/>
+      <c r="AK56" s="3"/>
+    </row>
+    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s">
         <v>3</v>
       </c>
-      <c r="B29">
+      <c r="E57" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" t="s">
+        <v>17</v>
+      </c>
+      <c r="G57" t="s">
+        <v>19</v>
+      </c>
+      <c r="H57" t="s">
+        <v>18</v>
+      </c>
+      <c r="I57" t="s">
+        <v>20</v>
+      </c>
+      <c r="J57" t="s">
+        <v>21</v>
+      </c>
+      <c r="K57" t="s">
+        <v>16</v>
+      </c>
+      <c r="L57" t="s">
+        <v>14</v>
+      </c>
+      <c r="N57" t="s">
+        <v>6</v>
+      </c>
+      <c r="O57" t="s">
+        <v>0</v>
+      </c>
+      <c r="P57" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>3</v>
+      </c>
+      <c r="R57" t="s">
+        <v>17</v>
+      </c>
+      <c r="S57" t="s">
+        <v>19</v>
+      </c>
+      <c r="T57" t="s">
+        <v>18</v>
+      </c>
+      <c r="U57" t="s">
+        <v>20</v>
+      </c>
+      <c r="V57" t="s">
+        <v>21</v>
+      </c>
+      <c r="W57" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC57" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD57" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF57" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG57" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH57" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI57" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ57" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK57" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>2</v>
+      </c>
+      <c r="B58">
+        <v>140917</v>
+      </c>
+      <c r="C58">
+        <v>137920</v>
+      </c>
+      <c r="D58">
+        <v>125751</v>
+      </c>
+      <c r="L58" s="2">
+        <f t="shared" ref="L58:L67" si="4">AVERAGE(B58:D58)*0.001</f>
+        <v>134.86266666666666</v>
+      </c>
+      <c r="N58">
+        <v>100</v>
+      </c>
+      <c r="O58">
+        <v>230055</v>
+      </c>
+      <c r="P58">
+        <v>239253</v>
+      </c>
+      <c r="Q58">
+        <v>233865</v>
+      </c>
+      <c r="Y58" s="2">
+        <f t="shared" ref="Y58:Y67" si="5">AVERAGE(O58:Q58)*0.001</f>
+        <v>234.39099999999999</v>
+      </c>
+      <c r="AA58">
+        <v>10</v>
+      </c>
+      <c r="AB58">
+        <v>309475</v>
+      </c>
+      <c r="AC58">
+        <v>243165</v>
+      </c>
+      <c r="AD58">
+        <v>290178</v>
+      </c>
+      <c r="AL58" s="2">
+        <f>AVERAGE(AB58:AD58)*0.001</f>
+        <v>280.93933333333331</v>
+      </c>
+    </row>
+    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59">
         <v>128926</v>
       </c>
-      <c r="C29">
+      <c r="C59">
         <v>113934</v>
       </c>
-      <c r="D29">
+      <c r="D59">
         <v>132925</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L59" s="2">
         <f t="shared" si="4"/>
         <v>125.26166666666667</v>
       </c>
-      <c r="N29">
+      <c r="N59">
         <v>200</v>
       </c>
-      <c r="O29">
+      <c r="O59">
         <v>421241</v>
       </c>
-      <c r="P29">
+      <c r="P59">
         <v>429514</v>
       </c>
-      <c r="Q29">
+      <c r="Q59">
         <v>423914</v>
       </c>
-      <c r="Y29" s="2">
+      <c r="Y59" s="2">
         <f t="shared" si="5"/>
         <v>424.8896666666667</v>
       </c>
-      <c r="AA29">
+      <c r="AA59">
         <v>20</v>
       </c>
-      <c r="AB29">
+      <c r="AB59">
         <v>183893</v>
       </c>
-      <c r="AC29">
+      <c r="AC59">
         <v>114623</v>
       </c>
-      <c r="AD29">
+      <c r="AD59">
         <v>136593</v>
       </c>
-      <c r="AL29" s="2">
-        <f t="shared" ref="AL29:AL37" si="6">AVERAGE(AB29:AD29)*0.001</f>
+      <c r="AL59" s="2">
+        <f t="shared" ref="AL59:AL67" si="6">AVERAGE(AB59:AD59)*0.001</f>
         <v>145.03633333333335</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>4</v>
       </c>
-      <c r="B30">
+      <c r="B60">
         <v>123946</v>
       </c>
-      <c r="C30">
+      <c r="C60">
         <v>125930</v>
       </c>
-      <c r="D30">
+      <c r="D60">
         <v>122929</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L60" s="2">
         <f t="shared" si="4"/>
         <v>124.26833333333333</v>
       </c>
-      <c r="N30">
+      <c r="N60">
         <v>300</v>
       </c>
-      <c r="O30">
+      <c r="O60">
         <v>621810</v>
       </c>
-      <c r="P30">
+      <c r="P60">
         <v>597965</v>
       </c>
-      <c r="Q30">
+      <c r="Q60">
         <v>613485</v>
       </c>
-      <c r="Y30" s="2">
+      <c r="Y60" s="2">
         <f t="shared" si="5"/>
         <v>611.08666666666659</v>
       </c>
-      <c r="AA30">
+      <c r="AA60">
         <v>30</v>
       </c>
-      <c r="AB30">
+      <c r="AB60">
         <v>143638</v>
       </c>
-      <c r="AC30">
+      <c r="AC60">
         <v>139919</v>
       </c>
-      <c r="AD30">
+      <c r="AD60">
         <v>167517</v>
       </c>
-      <c r="AL30" s="2">
+      <c r="AL60" s="2">
         <f t="shared" si="6"/>
         <v>150.358</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>5</v>
       </c>
-      <c r="B31">
+      <c r="B61">
         <v>129926</v>
       </c>
-      <c r="C31">
+      <c r="C61">
         <v>132926</v>
       </c>
-      <c r="D31">
+      <c r="D61">
         <v>124692</v>
       </c>
-      <c r="L31" s="2">
+      <c r="L61" s="2">
         <f t="shared" si="4"/>
         <v>129.18133333333333</v>
       </c>
-      <c r="N31">
+      <c r="N61">
         <v>400</v>
       </c>
-      <c r="O31">
+      <c r="O61">
         <v>810248</v>
       </c>
-      <c r="P31">
+      <c r="P61">
         <v>793177</v>
       </c>
-      <c r="Q31">
+      <c r="Q61">
         <v>812709</v>
       </c>
-      <c r="Y31" s="2">
+      <c r="Y61" s="2">
         <f t="shared" si="5"/>
         <v>805.37800000000004</v>
       </c>
-      <c r="AA31">
+      <c r="AA61">
         <v>40</v>
       </c>
-      <c r="AB31">
+      <c r="AB61">
         <v>174899</v>
       </c>
-      <c r="AC31">
+      <c r="AC61">
         <v>132929</v>
       </c>
-      <c r="AD31">
+      <c r="AD61">
         <v>173899</v>
       </c>
-      <c r="AL31" s="2">
+      <c r="AL61" s="2">
         <f t="shared" si="6"/>
         <v>160.57566666666665</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>6</v>
       </c>
-      <c r="B32">
+      <c r="B62">
         <v>131924</v>
       </c>
-      <c r="C32">
+      <c r="C62">
         <v>118931</v>
       </c>
-      <c r="D32">
+      <c r="D62">
         <v>117933</v>
       </c>
-      <c r="L32" s="2">
+      <c r="L62" s="2">
         <f t="shared" si="4"/>
         <v>122.92933333333333</v>
       </c>
-      <c r="N32">
+      <c r="N62">
         <v>500</v>
       </c>
-      <c r="O32">
+      <c r="O62">
         <v>979295</v>
       </c>
-      <c r="P32">
+      <c r="P62">
         <v>191948</v>
       </c>
-      <c r="Q32">
+      <c r="Q62">
         <v>131466</v>
       </c>
-      <c r="Y32" s="2">
+      <c r="Y62" s="2">
         <f t="shared" si="5"/>
         <v>434.23633333333333</v>
       </c>
-      <c r="AA32">
+      <c r="AA62">
         <v>50</v>
       </c>
-      <c r="AB32">
+      <c r="AB62">
         <v>133746</v>
       </c>
-      <c r="AC32">
+      <c r="AC62">
         <v>125203</v>
       </c>
-      <c r="AD32">
+      <c r="AD62">
         <v>163908</v>
       </c>
-      <c r="AL32" s="2">
+      <c r="AL62" s="2">
         <f t="shared" si="6"/>
         <v>140.95233333333334</v>
       </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>7</v>
       </c>
-      <c r="B33">
+      <c r="B63">
         <v>118934</v>
       </c>
-      <c r="C33">
+      <c r="C63">
         <v>252857</v>
       </c>
-      <c r="D33">
+      <c r="D63">
         <v>151912</v>
       </c>
-      <c r="L33" s="2">
+      <c r="L63" s="2">
         <f t="shared" si="4"/>
         <v>174.56766666666667</v>
       </c>
-      <c r="N33">
+      <c r="N63">
         <v>600</v>
       </c>
-      <c r="O33">
+      <c r="O63">
         <v>1238446</v>
       </c>
-      <c r="P33">
+      <c r="P63">
         <v>1176169</v>
       </c>
-      <c r="Q33">
+      <c r="Q63">
         <v>1263482</v>
       </c>
-      <c r="Y33" s="2">
+      <c r="Y63" s="2">
         <f t="shared" si="5"/>
         <v>1226.0323333333333</v>
       </c>
-      <c r="AA33">
+      <c r="AA63">
         <v>60</v>
       </c>
-      <c r="AB33">
+      <c r="AB63">
         <v>125426</v>
       </c>
-      <c r="AC33">
+      <c r="AC63">
         <v>116047</v>
       </c>
-      <c r="AD33">
+      <c r="AD63">
         <v>167902</v>
       </c>
-      <c r="AL33" s="2">
+      <c r="AL63" s="2">
         <f t="shared" si="6"/>
         <v>136.45833333333334</v>
       </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>8</v>
       </c>
-      <c r="B34">
+      <c r="B64">
         <v>138905</v>
       </c>
-      <c r="C34">
+      <c r="C64">
         <v>139916</v>
       </c>
-      <c r="D34">
+      <c r="D64">
         <v>131925</v>
       </c>
-      <c r="L34" s="2">
+      <c r="L64" s="2">
         <f t="shared" si="4"/>
         <v>136.91533333333334</v>
       </c>
-      <c r="N34">
+      <c r="N64">
         <v>700</v>
       </c>
-      <c r="O34">
+      <c r="O64">
         <v>1335362</v>
       </c>
-      <c r="P34">
+      <c r="P64">
         <v>1372401</v>
       </c>
-      <c r="Q34">
+      <c r="Q64">
         <v>1374165</v>
       </c>
-      <c r="Y34" s="2">
+      <c r="Y64" s="2">
         <f t="shared" si="5"/>
         <v>1360.6426666666669</v>
       </c>
-      <c r="AA34">
+      <c r="AA64">
         <v>70</v>
       </c>
-      <c r="AB34">
+      <c r="AB64">
         <v>134815</v>
       </c>
-      <c r="AC34">
+      <c r="AC64">
         <v>124927</v>
       </c>
-      <c r="AD34">
+      <c r="AD64">
         <v>150912</v>
       </c>
-      <c r="AL34" s="2">
+      <c r="AL64" s="2">
         <f t="shared" si="6"/>
         <v>136.88466666666665</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="65" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A65">
         <v>9</v>
       </c>
-      <c r="B35">
+      <c r="B65">
         <v>125927</v>
       </c>
-      <c r="C35">
+      <c r="C65">
         <v>149915</v>
       </c>
-      <c r="D35">
+      <c r="D65">
         <v>118932</v>
       </c>
-      <c r="L35" s="2">
+      <c r="L65" s="2">
         <f t="shared" si="4"/>
         <v>131.59133333333335</v>
       </c>
-      <c r="N35">
+      <c r="N65">
         <v>800</v>
       </c>
-      <c r="O35">
+      <c r="O65">
         <v>1531659</v>
       </c>
-      <c r="P35">
+      <c r="P65">
         <v>1575509</v>
       </c>
-      <c r="Q35">
+      <c r="Q65">
         <v>1535428</v>
       </c>
-      <c r="Y35" s="2">
+      <c r="Y65" s="2">
         <f t="shared" si="5"/>
         <v>1547.5319999999999</v>
       </c>
-      <c r="AA35">
+      <c r="AA65">
         <v>80</v>
       </c>
-      <c r="AB35">
+      <c r="AB65">
         <v>199885</v>
       </c>
-      <c r="AC35">
+      <c r="AC65">
         <v>156911</v>
       </c>
-      <c r="AD35">
+      <c r="AD65">
         <v>158343</v>
       </c>
-      <c r="AL35" s="2">
+      <c r="AL65" s="2">
         <f t="shared" si="6"/>
         <v>171.71299999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A66">
         <v>10</v>
       </c>
-      <c r="B36">
+      <c r="B66">
         <v>115090</v>
       </c>
-      <c r="C36">
+      <c r="C66">
         <v>127927</v>
       </c>
-      <c r="D36">
+      <c r="D66">
         <v>147916</v>
       </c>
-      <c r="L36" s="2">
+      <c r="L66" s="2">
         <f t="shared" si="4"/>
         <v>130.31100000000001</v>
       </c>
-      <c r="N36">
+      <c r="N66">
         <v>900</v>
       </c>
-      <c r="O36">
+      <c r="O66">
         <v>1798548</v>
       </c>
-      <c r="P36">
+      <c r="P66">
         <v>1734778</v>
       </c>
-      <c r="Q36">
+      <c r="Q66">
         <v>1728210</v>
       </c>
-      <c r="Y36" s="2">
+      <c r="Y66" s="2">
         <f t="shared" si="5"/>
         <v>1753.8453333333332</v>
       </c>
-      <c r="AA36">
+      <c r="AA66">
         <v>90</v>
       </c>
-      <c r="AB36">
+      <c r="AB66">
         <v>125930</v>
       </c>
-      <c r="AC36">
+      <c r="AC66">
         <v>127760</v>
       </c>
-      <c r="AD36">
+      <c r="AD66">
         <v>170901</v>
       </c>
-      <c r="AL36" s="2">
+      <c r="AL66" s="2">
         <f t="shared" si="6"/>
         <v>141.53033333333335</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="67" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A67">
         <v>11</v>
       </c>
-      <c r="B37">
+      <c r="B67">
         <v>132650</v>
       </c>
-      <c r="C37">
+      <c r="C67">
         <v>138921</v>
       </c>
-      <c r="D37">
+      <c r="D67">
         <v>122932</v>
       </c>
-      <c r="L37" s="2">
+      <c r="L67" s="2">
         <f t="shared" si="4"/>
         <v>131.501</v>
       </c>
-      <c r="N37">
+      <c r="N67">
         <v>1000</v>
       </c>
-      <c r="O37">
+      <c r="O67">
         <v>1965341</v>
       </c>
-      <c r="P37">
+      <c r="P67">
         <v>1957985</v>
       </c>
-      <c r="Q37">
+      <c r="Q67">
         <v>1944963</v>
       </c>
-      <c r="Y37" s="2">
+      <c r="Y67" s="2">
         <f t="shared" si="5"/>
         <v>1956.0963333333334</v>
       </c>
-      <c r="AA37">
+      <c r="AA67">
         <v>100</v>
       </c>
-      <c r="AB37">
+      <c r="AB67">
         <v>122927</v>
       </c>
-      <c r="AC37">
+      <c r="AC67">
         <v>117932</v>
       </c>
-      <c r="AD37">
+      <c r="AD67">
         <v>173900</v>
       </c>
-      <c r="AL37" s="2">
+      <c r="AL67" s="2">
         <f t="shared" si="6"/>
         <v>138.25300000000001</v>
       </c>
@@ -7539,10 +9282,10 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A1:AL1"/>
-    <mergeCell ref="A24:AL24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="O26:Q26"/>
-    <mergeCell ref="AB26:AD26"/>
+    <mergeCell ref="A54:AL54"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="O56:Q56"/>
+    <mergeCell ref="AB56:AD56"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="AB2:AD2"/>
     <mergeCell ref="O2:Q2"/>

</xml_diff>

<commit_message>
Added all values for runtime PSO_rastrigin (of increased range)
</commit_message>
<xml_diff>
--- a/Documentation/Graphs.xlsx
+++ b/Documentation/Graphs.xlsx
@@ -393,11 +393,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="202097024"/>
-        <c:axId val="202098560"/>
+        <c:axId val="204390784"/>
+        <c:axId val="204392320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="202097024"/>
+        <c:axId val="204390784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -440,7 +440,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202098560"/>
+        <c:crossAx val="204392320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -448,7 +448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202098560"/>
+        <c:axId val="204392320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -499,7 +499,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202097024"/>
+        <c:crossAx val="204390784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -776,11 +776,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="202378240"/>
-        <c:axId val="202404608"/>
+        <c:axId val="204672000"/>
+        <c:axId val="204698368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="202378240"/>
+        <c:axId val="204672000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -823,7 +823,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202404608"/>
+        <c:crossAx val="204698368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -831,7 +831,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202404608"/>
+        <c:axId val="204698368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -882,7 +882,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202378240"/>
+        <c:crossAx val="204672000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1159,11 +1159,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="202434432"/>
-        <c:axId val="202435968"/>
+        <c:axId val="204728192"/>
+        <c:axId val="204729728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="202434432"/>
+        <c:axId val="204728192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,7 +1206,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202435968"/>
+        <c:crossAx val="204729728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1214,7 +1214,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202435968"/>
+        <c:axId val="204729728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1265,7 +1265,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202434432"/>
+        <c:crossAx val="204728192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1488,7 +1488,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>rastrigin!$L$28:$L$37</c:f>
+              <c:f>rastrigin!$L$58:$L$67</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1542,11 +1542,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="202781824"/>
-        <c:axId val="202783744"/>
+        <c:axId val="205077120"/>
+        <c:axId val="205079296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="202781824"/>
+        <c:axId val="205077120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1583,6 +1583,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1629,7 +1630,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202783744"/>
+        <c:crossAx val="205079296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1637,7 +1638,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202783744"/>
+        <c:axId val="205079296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1674,6 +1675,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1714,7 +1716,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202781824"/>
+        <c:crossAx val="205077120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1728,6 +1730,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1947,7 +1950,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>rastrigin!$Y$28:$Y$37</c:f>
+              <c:f>rastrigin!$Y$58:$Y$67</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2001,11 +2004,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="202818304"/>
-        <c:axId val="202820224"/>
+        <c:axId val="205113984"/>
+        <c:axId val="205124352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="202818304"/>
+        <c:axId val="205113984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2042,6 +2045,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2088,7 +2092,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202820224"/>
+        <c:crossAx val="205124352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2096,7 +2100,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202820224"/>
+        <c:axId val="205124352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2133,6 +2137,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2173,7 +2178,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202818304"/>
+        <c:crossAx val="205113984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2187,6 +2192,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2396,7 +2402,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>rastrigin!$AL$28:$AL$37</c:f>
+              <c:f>rastrigin!$AL$58:$AL$67</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2450,11 +2456,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="202604928"/>
-        <c:axId val="202606848"/>
+        <c:axId val="204900608"/>
+        <c:axId val="204910976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="202604928"/>
+        <c:axId val="204900608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2491,6 +2497,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2537,7 +2544,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202606848"/>
+        <c:crossAx val="204910976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2545,7 +2552,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202606848"/>
+        <c:axId val="204910976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2596,6 +2603,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2636,7 +2644,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202604928"/>
+        <c:crossAx val="204900608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2650,6 +2658,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2817,13 +2826,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>800099</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2847,13 +2856,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2877,13 +2886,13 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>419101</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>200027</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3161,7 +3170,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4382,10 +4391,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL37"/>
+  <dimension ref="A1:AL67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AL51" sqref="AL51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4811,7 +4820,7 @@
         <v>4986</v>
       </c>
       <c r="AL5" s="2">
-        <f t="shared" ref="AL5:AL23" si="1">AVERAGE(AB5:AK5)*0.001</f>
+        <f t="shared" ref="AL5:AL53" si="1">AVERAGE(AB5:AK5)*0.001</f>
         <v>4.5905000000000005</v>
       </c>
     </row>
@@ -4850,7 +4859,7 @@
         <v>16030</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" ref="L6:L23" si="2">AVERAGE(B6:K6) * 0.001</f>
+        <f t="shared" ref="L6:L27" si="2">AVERAGE(B6:K6) * 0.001</f>
         <v>12.815200000000001</v>
       </c>
       <c r="N6">
@@ -5791,7 +5800,7 @@
         <v>92752</v>
       </c>
       <c r="Y14" s="2">
-        <f t="shared" ref="Y14:Y23" si="3">AVERAGE(O14:X14)*0.001</f>
+        <f t="shared" ref="Y14:Y33" si="3">AVERAGE(O14:X14)*0.001</f>
         <v>95.047800000000009</v>
       </c>
       <c r="AA14">
@@ -6850,688 +6859,2422 @@
       </c>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="7"/>
-      <c r="Y24" s="7"/>
-      <c r="Z24" s="7"/>
-      <c r="AA24" s="7"/>
-      <c r="AB24" s="7"/>
-      <c r="AC24" s="7"/>
-      <c r="AD24" s="7"/>
-      <c r="AE24" s="7"/>
-      <c r="AF24" s="7"/>
-      <c r="AG24" s="7"/>
-      <c r="AH24" s="7"/>
-      <c r="AI24" s="7"/>
-      <c r="AJ24" s="7"/>
-      <c r="AK24" s="7"/>
-      <c r="AL24" s="7"/>
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>48006</v>
+      </c>
+      <c r="C24">
+        <v>40034</v>
+      </c>
+      <c r="D24">
+        <v>43995</v>
+      </c>
+      <c r="E24">
+        <v>40000</v>
+      </c>
+      <c r="F24">
+        <v>43997</v>
+      </c>
+      <c r="G24">
+        <v>48016</v>
+      </c>
+      <c r="H24">
+        <v>48042</v>
+      </c>
+      <c r="I24">
+        <v>43991</v>
+      </c>
+      <c r="J24">
+        <v>43991</v>
+      </c>
+      <c r="K24">
+        <v>44025</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="2"/>
+        <v>44.409700000000001</v>
+      </c>
+      <c r="N24">
+        <v>2100</v>
+      </c>
+      <c r="O24">
+        <v>258947</v>
+      </c>
+      <c r="P24">
+        <v>240005</v>
+      </c>
+      <c r="Q24">
+        <v>213485</v>
+      </c>
+      <c r="R24">
+        <v>200883</v>
+      </c>
+      <c r="S24">
+        <v>226662</v>
+      </c>
+      <c r="T24">
+        <v>216900</v>
+      </c>
+      <c r="U24">
+        <v>193057</v>
+      </c>
+      <c r="V24">
+        <v>198491</v>
+      </c>
+      <c r="W24">
+        <v>196079</v>
+      </c>
+      <c r="X24">
+        <v>264478</v>
+      </c>
+      <c r="Y24" s="2">
+        <f t="shared" si="3"/>
+        <v>220.89870000000002</v>
+      </c>
+      <c r="AA24">
+        <v>210</v>
+      </c>
+      <c r="AB24" s="5">
+        <v>57578</v>
+      </c>
+      <c r="AC24">
+        <v>55998</v>
+      </c>
+      <c r="AD24">
+        <v>75994</v>
+      </c>
+      <c r="AE24">
+        <v>85423</v>
+      </c>
+      <c r="AF24">
+        <v>59993</v>
+      </c>
+      <c r="AG24">
+        <v>55960</v>
+      </c>
+      <c r="AH24">
+        <v>55960</v>
+      </c>
+      <c r="AI24">
+        <v>69251</v>
+      </c>
+      <c r="AJ24">
+        <v>64010</v>
+      </c>
+      <c r="AK24">
+        <v>60039</v>
+      </c>
+      <c r="AL24" s="2">
+        <f t="shared" si="1"/>
+        <v>64.020600000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>47954</v>
+      </c>
+      <c r="C25">
+        <v>24207</v>
+      </c>
+      <c r="D25">
+        <v>40100</v>
+      </c>
+      <c r="E25">
+        <v>27766</v>
+      </c>
+      <c r="F25">
+        <v>32115</v>
+      </c>
+      <c r="G25">
+        <v>47993</v>
+      </c>
+      <c r="H25">
+        <v>48006</v>
+      </c>
+      <c r="I25">
+        <v>31900</v>
+      </c>
+      <c r="J25">
+        <v>31900</v>
+      </c>
+      <c r="K25">
+        <v>32310</v>
+      </c>
+      <c r="L25" s="2">
+        <f t="shared" si="2"/>
+        <v>36.4251</v>
+      </c>
+      <c r="N25">
+        <v>2200</v>
+      </c>
+      <c r="O25">
+        <v>217829</v>
+      </c>
+      <c r="P25">
+        <v>224787</v>
+      </c>
+      <c r="Q25">
+        <v>189430</v>
+      </c>
+      <c r="R25">
+        <v>226179</v>
+      </c>
+      <c r="S25">
+        <v>227541</v>
+      </c>
+      <c r="T25">
+        <v>216639</v>
+      </c>
+      <c r="U25">
+        <v>200132</v>
+      </c>
+      <c r="V25">
+        <v>221421</v>
+      </c>
+      <c r="W25">
+        <v>240493</v>
+      </c>
+      <c r="X25">
+        <v>226069</v>
+      </c>
+      <c r="Y25" s="2">
+        <f t="shared" si="3"/>
+        <v>219.05199999999999</v>
+      </c>
+      <c r="AA25">
+        <v>220</v>
+      </c>
+      <c r="AB25" s="5">
+        <v>52000</v>
+      </c>
+      <c r="AC25">
+        <v>56000</v>
+      </c>
+      <c r="AD25">
+        <v>112884</v>
+      </c>
+      <c r="AE25">
+        <v>43785</v>
+      </c>
+      <c r="AF25">
+        <v>60010</v>
+      </c>
+      <c r="AG25">
+        <v>52000</v>
+      </c>
+      <c r="AH25">
+        <v>52000</v>
+      </c>
+      <c r="AI25">
+        <v>43758</v>
+      </c>
+      <c r="AJ25">
+        <v>67993</v>
+      </c>
+      <c r="AK25">
+        <v>67996</v>
+      </c>
+      <c r="AL25" s="2">
+        <f t="shared" si="1"/>
+        <v>60.842599999999997</v>
+      </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="O26" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
-      <c r="W26" s="3"/>
-      <c r="X26" s="4"/>
-      <c r="AB26" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC26" s="8"/>
-      <c r="AD26" s="8"/>
-      <c r="AE26" s="3"/>
-      <c r="AF26" s="3"/>
-      <c r="AG26" s="3"/>
-      <c r="AH26" s="3"/>
-      <c r="AI26" s="3"/>
-      <c r="AJ26" s="3"/>
-      <c r="AK26" s="3"/>
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>52000</v>
+      </c>
+      <c r="C26">
+        <v>46901</v>
+      </c>
+      <c r="D26">
+        <v>31243</v>
+      </c>
+      <c r="E26">
+        <v>36285</v>
+      </c>
+      <c r="F26">
+        <v>46865</v>
+      </c>
+      <c r="G26">
+        <v>56869</v>
+      </c>
+      <c r="H26">
+        <v>51998</v>
+      </c>
+      <c r="I26">
+        <v>52084</v>
+      </c>
+      <c r="J26">
+        <v>52084</v>
+      </c>
+      <c r="K26">
+        <v>56084</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="2"/>
+        <v>48.241300000000003</v>
+      </c>
+      <c r="N26">
+        <v>2300</v>
+      </c>
+      <c r="O26">
+        <v>246187</v>
+      </c>
+      <c r="P26">
+        <v>245336</v>
+      </c>
+      <c r="Q26">
+        <v>199020</v>
+      </c>
+      <c r="R26">
+        <v>219657</v>
+      </c>
+      <c r="S26">
+        <v>214203</v>
+      </c>
+      <c r="T26">
+        <v>205879</v>
+      </c>
+      <c r="U26">
+        <v>232201</v>
+      </c>
+      <c r="V26">
+        <v>238119</v>
+      </c>
+      <c r="W26">
+        <v>232318</v>
+      </c>
+      <c r="X26">
+        <v>272110</v>
+      </c>
+      <c r="Y26" s="2">
+        <f t="shared" si="3"/>
+        <v>230.50300000000001</v>
+      </c>
+      <c r="AA26">
+        <v>230</v>
+      </c>
+      <c r="AB26" s="5">
+        <v>50348</v>
+      </c>
+      <c r="AC26">
+        <v>52000</v>
+      </c>
+      <c r="AD26">
+        <v>72011</v>
+      </c>
+      <c r="AE26">
+        <v>56369</v>
+      </c>
+      <c r="AF26">
+        <v>87994</v>
+      </c>
+      <c r="AG26">
+        <v>58361</v>
+      </c>
+      <c r="AH26">
+        <v>58361</v>
+      </c>
+      <c r="AI26">
+        <v>52783</v>
+      </c>
+      <c r="AJ26">
+        <v>68231</v>
+      </c>
+      <c r="AK26">
+        <v>68288</v>
+      </c>
+      <c r="AL26" s="2">
+        <f t="shared" si="1"/>
+        <v>62.474600000000002</v>
+      </c>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" t="s">
-        <v>19</v>
-      </c>
-      <c r="H27" t="s">
-        <v>18</v>
-      </c>
-      <c r="I27" t="s">
-        <v>20</v>
-      </c>
-      <c r="J27" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" t="s">
-        <v>16</v>
-      </c>
-      <c r="L27" t="s">
-        <v>14</v>
-      </c>
-      <c r="N27" t="s">
-        <v>6</v>
-      </c>
-      <c r="O27" t="s">
-        <v>0</v>
-      </c>
-      <c r="P27" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>3</v>
-      </c>
-      <c r="R27" t="s">
-        <v>17</v>
-      </c>
-      <c r="S27" t="s">
-        <v>19</v>
-      </c>
-      <c r="T27" t="s">
-        <v>18</v>
-      </c>
-      <c r="U27" t="s">
-        <v>20</v>
-      </c>
-      <c r="V27" t="s">
-        <v>21</v>
-      </c>
-      <c r="W27" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC27" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD27" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE27" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG27" t="s">
-        <v>19</v>
-      </c>
-      <c r="AH27" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI27" t="s">
-        <v>20</v>
-      </c>
-      <c r="AJ27" t="s">
-        <v>21</v>
-      </c>
-      <c r="AK27" t="s">
-        <v>23</v>
-      </c>
-      <c r="AL27" t="s">
-        <v>14</v>
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>51998</v>
+      </c>
+      <c r="C27">
+        <v>48292</v>
+      </c>
+      <c r="D27">
+        <v>44972</v>
+      </c>
+      <c r="E27">
+        <v>63983</v>
+      </c>
+      <c r="F27">
+        <v>39451</v>
+      </c>
+      <c r="G27">
+        <v>56305</v>
+      </c>
+      <c r="H27">
+        <v>51991</v>
+      </c>
+      <c r="I27">
+        <v>44154</v>
+      </c>
+      <c r="J27">
+        <v>44154</v>
+      </c>
+      <c r="K27">
+        <v>60276</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="2"/>
+        <v>50.557600000000001</v>
+      </c>
+      <c r="N27">
+        <v>2400</v>
+      </c>
+      <c r="O27">
+        <v>242285</v>
+      </c>
+      <c r="P27">
+        <v>212308</v>
+      </c>
+      <c r="Q27">
+        <v>239332</v>
+      </c>
+      <c r="R27">
+        <v>258271</v>
+      </c>
+      <c r="S27">
+        <v>205225</v>
+      </c>
+      <c r="T27">
+        <v>213730</v>
+      </c>
+      <c r="U27">
+        <v>250274</v>
+      </c>
+      <c r="V27">
+        <v>228135</v>
+      </c>
+      <c r="W27">
+        <v>229465</v>
+      </c>
+      <c r="X27">
+        <v>262772</v>
+      </c>
+      <c r="Y27" s="2">
+        <f t="shared" si="3"/>
+        <v>234.17970000000003</v>
+      </c>
+      <c r="AA27">
+        <v>240</v>
+      </c>
+      <c r="AB27" s="5">
+        <v>46437</v>
+      </c>
+      <c r="AC27">
+        <v>52000</v>
+      </c>
+      <c r="AD27">
+        <v>75956</v>
+      </c>
+      <c r="AE27">
+        <v>55204</v>
+      </c>
+      <c r="AF27">
+        <v>73009</v>
+      </c>
+      <c r="AG27">
+        <v>50419</v>
+      </c>
+      <c r="AH27">
+        <v>50419</v>
+      </c>
+      <c r="AI27">
+        <v>71234</v>
+      </c>
+      <c r="AJ27">
+        <v>59441</v>
+      </c>
+      <c r="AK27">
+        <v>67121</v>
+      </c>
+      <c r="AL27" s="2">
+        <f t="shared" si="1"/>
+        <v>60.124000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>2</v>
-      </c>
-      <c r="B28">
-        <v>140917</v>
-      </c>
-      <c r="C28">
-        <v>137920</v>
-      </c>
-      <c r="D28">
-        <v>125751</v>
-      </c>
-      <c r="L28" s="2">
-        <f t="shared" ref="L28:L37" si="4">AVERAGE(B28:D28)*0.001</f>
-        <v>134.86266666666666</v>
-      </c>
+      <c r="L28" s="2"/>
       <c r="N28">
-        <v>100</v>
+        <v>2500</v>
       </c>
       <c r="O28">
-        <v>230055</v>
+        <v>257365</v>
       </c>
       <c r="P28">
-        <v>239253</v>
+        <v>227291</v>
       </c>
       <c r="Q28">
-        <v>233865</v>
+        <v>269524</v>
+      </c>
+      <c r="R28">
+        <v>217055</v>
+      </c>
+      <c r="S28">
+        <v>231090</v>
+      </c>
+      <c r="T28">
+        <v>257656</v>
+      </c>
+      <c r="U28">
+        <v>237703</v>
+      </c>
+      <c r="V28">
+        <v>221198</v>
+      </c>
+      <c r="W28">
+        <v>228030</v>
+      </c>
+      <c r="X28">
+        <v>319382</v>
       </c>
       <c r="Y28" s="2">
-        <f t="shared" ref="Y28:Y37" si="5">AVERAGE(O28:Q28)*0.001</f>
-        <v>234.39099999999999</v>
+        <f t="shared" si="3"/>
+        <v>246.6294</v>
       </c>
       <c r="AA28">
-        <v>10</v>
-      </c>
-      <c r="AB28">
-        <v>309475</v>
+        <v>250</v>
+      </c>
+      <c r="AB28" s="5">
+        <v>61005</v>
       </c>
       <c r="AC28">
-        <v>243165</v>
+        <v>46854</v>
       </c>
       <c r="AD28">
-        <v>290178</v>
+        <v>78469</v>
+      </c>
+      <c r="AE28">
+        <v>62826</v>
+      </c>
+      <c r="AF28">
+        <v>68018</v>
+      </c>
+      <c r="AG28">
+        <v>58487</v>
+      </c>
+      <c r="AH28">
+        <v>58487</v>
+      </c>
+      <c r="AI28">
+        <v>62915</v>
+      </c>
+      <c r="AJ28">
+        <v>58340</v>
+      </c>
+      <c r="AK28">
+        <v>62956</v>
       </c>
       <c r="AL28" s="2">
-        <f>AVERAGE(AB28:AD28)*0.001</f>
-        <v>280.93933333333331</v>
+        <f t="shared" si="1"/>
+        <v>61.835699999999996</v>
       </c>
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="L29" s="2"/>
+      <c r="N29">
+        <v>2600</v>
+      </c>
+      <c r="O29">
+        <v>360025</v>
+      </c>
+      <c r="P29">
+        <v>246697</v>
+      </c>
+      <c r="Q29">
+        <v>305798</v>
+      </c>
+      <c r="R29">
+        <v>241045</v>
+      </c>
+      <c r="S29">
+        <v>247896</v>
+      </c>
+      <c r="T29">
+        <v>234370</v>
+      </c>
+      <c r="U29">
+        <v>236514</v>
+      </c>
+      <c r="V29">
+        <v>240876</v>
+      </c>
+      <c r="W29">
+        <v>245887</v>
+      </c>
+      <c r="X29">
+        <v>251518</v>
+      </c>
+      <c r="Y29" s="2">
+        <f t="shared" si="3"/>
+        <v>261.06260000000003</v>
+      </c>
+      <c r="AA29">
+        <v>260</v>
+      </c>
+      <c r="AB29" s="5">
+        <v>51336</v>
+      </c>
+      <c r="AC29">
+        <v>62612</v>
+      </c>
+      <c r="AD29">
+        <v>85674</v>
+      </c>
+      <c r="AE29">
+        <v>68359</v>
+      </c>
+      <c r="AF29">
+        <v>67944</v>
+      </c>
+      <c r="AG29">
+        <v>52704</v>
+      </c>
+      <c r="AH29">
+        <v>52704</v>
+      </c>
+      <c r="AI29">
+        <v>59558</v>
+      </c>
+      <c r="AJ29">
+        <v>56737</v>
+      </c>
+      <c r="AK29">
+        <v>62747</v>
+      </c>
+      <c r="AL29" s="2">
+        <f t="shared" si="1"/>
+        <v>62.037500000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L30" s="2"/>
+      <c r="N30">
+        <v>2700</v>
+      </c>
+      <c r="O30">
+        <v>341103</v>
+      </c>
+      <c r="P30">
+        <v>253282</v>
+      </c>
+      <c r="Q30">
+        <v>246661</v>
+      </c>
+      <c r="R30">
+        <v>240143</v>
+      </c>
+      <c r="S30">
+        <v>266783</v>
+      </c>
+      <c r="T30">
+        <v>268202</v>
+      </c>
+      <c r="U30">
+        <v>276150</v>
+      </c>
+      <c r="V30">
+        <v>286135</v>
+      </c>
+      <c r="W30">
+        <v>249058</v>
+      </c>
+      <c r="X30">
+        <v>300464</v>
+      </c>
+      <c r="Y30" s="2">
+        <f t="shared" si="3"/>
+        <v>272.79809999999998</v>
+      </c>
+      <c r="AA30">
+        <v>270</v>
+      </c>
+      <c r="AB30" s="5">
+        <v>61736</v>
+      </c>
+      <c r="AC30">
+        <v>53886</v>
+      </c>
+      <c r="AD30">
+        <v>65262</v>
+      </c>
+      <c r="AE30">
+        <v>74271</v>
+      </c>
+      <c r="AF30">
+        <v>74289</v>
+      </c>
+      <c r="AG30">
+        <v>58994</v>
+      </c>
+      <c r="AH30">
+        <v>58994</v>
+      </c>
+      <c r="AI30">
+        <v>66645</v>
+      </c>
+      <c r="AJ30">
+        <v>71383</v>
+      </c>
+      <c r="AK30">
+        <v>65178</v>
+      </c>
+      <c r="AL30" s="2">
+        <f t="shared" si="1"/>
+        <v>65.063800000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L31" s="2"/>
+      <c r="N31">
+        <v>2800</v>
+      </c>
+      <c r="O31">
+        <v>298892</v>
+      </c>
+      <c r="P31">
+        <v>239225</v>
+      </c>
+      <c r="Q31">
+        <v>264837</v>
+      </c>
+      <c r="R31">
+        <v>296111</v>
+      </c>
+      <c r="S31">
+        <v>282489</v>
+      </c>
+      <c r="T31">
+        <v>296057</v>
+      </c>
+      <c r="U31">
+        <v>283676</v>
+      </c>
+      <c r="V31">
+        <v>282936</v>
+      </c>
+      <c r="W31">
+        <v>302433</v>
+      </c>
+      <c r="X31">
+        <v>275191</v>
+      </c>
+      <c r="Y31" s="2">
+        <f t="shared" si="3"/>
+        <v>282.18470000000002</v>
+      </c>
+      <c r="AA31">
+        <v>280</v>
+      </c>
+      <c r="AB31" s="5">
+        <v>59825</v>
+      </c>
+      <c r="AC31">
+        <v>68976</v>
+      </c>
+      <c r="AD31">
+        <v>103051</v>
+      </c>
+      <c r="AE31">
+        <v>64691</v>
+      </c>
+      <c r="AF31">
+        <v>76001</v>
+      </c>
+      <c r="AG31">
+        <v>53634</v>
+      </c>
+      <c r="AH31">
+        <v>53634</v>
+      </c>
+      <c r="AI31">
+        <v>64846</v>
+      </c>
+      <c r="AJ31">
+        <v>69539</v>
+      </c>
+      <c r="AK31">
+        <v>70821</v>
+      </c>
+      <c r="AL31" s="2">
+        <f t="shared" si="1"/>
+        <v>68.501800000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L32" s="2"/>
+      <c r="N32">
+        <v>2900</v>
+      </c>
+      <c r="O32">
+        <v>298641</v>
+      </c>
+      <c r="P32">
+        <v>279656</v>
+      </c>
+      <c r="Q32">
+        <v>307095</v>
+      </c>
+      <c r="R32">
+        <v>312206</v>
+      </c>
+      <c r="S32">
+        <v>261470</v>
+      </c>
+      <c r="T32">
+        <v>258273</v>
+      </c>
+      <c r="U32">
+        <v>263091</v>
+      </c>
+      <c r="V32">
+        <v>259445</v>
+      </c>
+      <c r="W32">
+        <v>255404</v>
+      </c>
+      <c r="X32">
+        <v>343337</v>
+      </c>
+      <c r="Y32" s="2">
+        <f t="shared" si="3"/>
+        <v>283.86180000000002</v>
+      </c>
+      <c r="AA32">
+        <v>290</v>
+      </c>
+      <c r="AB32" s="5">
+        <v>61772</v>
+      </c>
+      <c r="AC32">
+        <v>62186</v>
+      </c>
+      <c r="AD32">
+        <v>93480</v>
+      </c>
+      <c r="AE32">
+        <v>72091</v>
+      </c>
+      <c r="AF32">
+        <v>74119</v>
+      </c>
+      <c r="AG32">
+        <v>69122</v>
+      </c>
+      <c r="AH32">
+        <v>69122</v>
+      </c>
+      <c r="AI32">
+        <v>61975</v>
+      </c>
+      <c r="AJ32">
+        <v>74702</v>
+      </c>
+      <c r="AK32">
+        <v>70776</v>
+      </c>
+      <c r="AL32" s="2">
+        <f t="shared" si="1"/>
+        <v>70.9345</v>
+      </c>
+    </row>
+    <row r="33" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L33" s="2"/>
+      <c r="N33">
+        <v>3000</v>
+      </c>
+      <c r="O33">
+        <v>313339</v>
+      </c>
+      <c r="P33">
+        <v>300984</v>
+      </c>
+      <c r="Q33">
+        <v>262895</v>
+      </c>
+      <c r="R33">
+        <v>264841</v>
+      </c>
+      <c r="S33">
+        <v>276973</v>
+      </c>
+      <c r="T33">
+        <v>262308</v>
+      </c>
+      <c r="U33">
+        <v>257283</v>
+      </c>
+      <c r="V33">
+        <v>272724</v>
+      </c>
+      <c r="W33">
+        <v>266221</v>
+      </c>
+      <c r="X33">
+        <v>347569</v>
+      </c>
+      <c r="Y33" s="2">
+        <f t="shared" si="3"/>
+        <v>282.51370000000003</v>
+      </c>
+      <c r="AA33">
+        <v>300</v>
+      </c>
+      <c r="AB33" s="5">
+        <v>61831</v>
+      </c>
+      <c r="AC33">
+        <v>68511</v>
+      </c>
+      <c r="AD33">
+        <v>91596</v>
+      </c>
+      <c r="AE33">
+        <v>63518</v>
+      </c>
+      <c r="AF33">
+        <v>80501</v>
+      </c>
+      <c r="AG33">
+        <v>82250</v>
+      </c>
+      <c r="AH33">
+        <v>82250</v>
+      </c>
+      <c r="AI33">
+        <v>71598</v>
+      </c>
+      <c r="AJ33">
+        <v>76687</v>
+      </c>
+      <c r="AK33">
+        <v>92210</v>
+      </c>
+      <c r="AL33" s="2">
+        <f t="shared" si="1"/>
+        <v>77.095200000000006</v>
+      </c>
+    </row>
+    <row r="34" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="AA34">
+        <v>310</v>
+      </c>
+      <c r="AB34" s="5">
+        <v>65850</v>
+      </c>
+      <c r="AC34">
+        <v>69856</v>
+      </c>
+      <c r="AD34">
+        <v>90429</v>
+      </c>
+      <c r="AE34">
+        <v>87607</v>
+      </c>
+      <c r="AF34">
+        <v>84683</v>
+      </c>
+      <c r="AG34">
+        <v>94101</v>
+      </c>
+      <c r="AH34">
+        <v>94101</v>
+      </c>
+      <c r="AI34">
+        <v>83273</v>
+      </c>
+      <c r="AJ34">
+        <v>78888</v>
+      </c>
+      <c r="AK34">
+        <v>77872</v>
+      </c>
+      <c r="AL34" s="2">
+        <f t="shared" si="1"/>
+        <v>82.665999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="AA35">
+        <v>320</v>
+      </c>
+      <c r="AB35" s="5">
+        <v>71317</v>
+      </c>
+      <c r="AC35">
+        <v>64399</v>
+      </c>
+      <c r="AD35">
+        <v>132856</v>
+      </c>
+      <c r="AE35">
+        <v>83193</v>
+      </c>
+      <c r="AF35">
+        <v>72007</v>
+      </c>
+      <c r="AG35">
+        <v>88000</v>
+      </c>
+      <c r="AH35">
+        <v>88000</v>
+      </c>
+      <c r="AI35">
+        <v>83070</v>
+      </c>
+      <c r="AJ35">
+        <v>89506</v>
+      </c>
+      <c r="AK35">
+        <v>81965</v>
+      </c>
+      <c r="AL35" s="2">
+        <f t="shared" si="1"/>
+        <v>85.431300000000007</v>
+      </c>
+    </row>
+    <row r="36" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L36" s="2"/>
+      <c r="Y36" s="2"/>
+      <c r="AA36">
+        <v>330</v>
+      </c>
+      <c r="AB36" s="5">
+        <v>70906</v>
+      </c>
+      <c r="AC36">
+        <v>71498</v>
+      </c>
+      <c r="AD36">
+        <v>87313</v>
+      </c>
+      <c r="AE36">
+        <v>74882</v>
+      </c>
+      <c r="AF36">
+        <v>83970</v>
+      </c>
+      <c r="AG36">
+        <v>79999</v>
+      </c>
+      <c r="AH36">
+        <v>79999</v>
+      </c>
+      <c r="AI36">
+        <v>82867</v>
+      </c>
+      <c r="AJ36">
+        <v>86317</v>
+      </c>
+      <c r="AK36">
+        <v>82286</v>
+      </c>
+      <c r="AL36" s="2">
+        <f t="shared" si="1"/>
+        <v>80.003699999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L37" s="2"/>
+      <c r="Y37" s="2"/>
+      <c r="AA37">
+        <v>340</v>
+      </c>
+      <c r="AB37" s="5">
+        <v>76081</v>
+      </c>
+      <c r="AC37">
+        <v>92283</v>
+      </c>
+      <c r="AD37">
+        <v>86277</v>
+      </c>
+      <c r="AE37">
+        <v>76380</v>
+      </c>
+      <c r="AF37">
+        <v>73863</v>
+      </c>
+      <c r="AG37">
+        <v>81926</v>
+      </c>
+      <c r="AH37">
+        <v>81926</v>
+      </c>
+      <c r="AI37">
+        <v>85216</v>
+      </c>
+      <c r="AJ37">
+        <v>85638</v>
+      </c>
+      <c r="AK37">
+        <v>73576</v>
+      </c>
+      <c r="AL37" s="2">
+        <f t="shared" si="1"/>
+        <v>81.316600000000008</v>
+      </c>
+    </row>
+    <row r="38" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L38" s="2"/>
+      <c r="Y38" s="2"/>
+      <c r="AA38">
+        <v>350</v>
+      </c>
+      <c r="AB38" s="5">
+        <v>71934</v>
+      </c>
+      <c r="AC38">
+        <v>107703</v>
+      </c>
+      <c r="AD38">
+        <v>91191</v>
+      </c>
+      <c r="AE38">
+        <v>80930</v>
+      </c>
+      <c r="AF38">
+        <v>98595</v>
+      </c>
+      <c r="AG38">
+        <v>94421</v>
+      </c>
+      <c r="AH38">
+        <v>94421</v>
+      </c>
+      <c r="AI38">
+        <v>90610</v>
+      </c>
+      <c r="AJ38">
+        <v>91610</v>
+      </c>
+      <c r="AK38">
+        <v>71948</v>
+      </c>
+      <c r="AL38" s="2">
+        <f t="shared" si="1"/>
+        <v>89.336300000000008</v>
+      </c>
+    </row>
+    <row r="39" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L39" s="2"/>
+      <c r="Y39" s="2"/>
+      <c r="AA39">
+        <v>360</v>
+      </c>
+      <c r="AB39" s="5">
+        <v>80065</v>
+      </c>
+      <c r="AC39">
+        <v>106585</v>
+      </c>
+      <c r="AD39">
+        <v>110995</v>
+      </c>
+      <c r="AE39">
+        <v>93373</v>
+      </c>
+      <c r="AF39">
+        <v>97206</v>
+      </c>
+      <c r="AG39">
+        <v>110419</v>
+      </c>
+      <c r="AH39">
+        <v>110419</v>
+      </c>
+      <c r="AI39">
+        <v>91916</v>
+      </c>
+      <c r="AJ39">
+        <v>81291</v>
+      </c>
+      <c r="AK39">
+        <v>82031</v>
+      </c>
+      <c r="AL39" s="2">
+        <f t="shared" si="1"/>
+        <v>96.43</v>
+      </c>
+    </row>
+    <row r="40" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L40" s="2"/>
+      <c r="Y40" s="2"/>
+      <c r="AA40">
+        <v>370</v>
+      </c>
+      <c r="AB40" s="5">
+        <v>73455</v>
+      </c>
+      <c r="AC40">
+        <v>96062</v>
+      </c>
+      <c r="AD40">
+        <v>140469</v>
+      </c>
+      <c r="AE40">
+        <v>111937</v>
+      </c>
+      <c r="AF40">
+        <v>117099</v>
+      </c>
+      <c r="AG40">
+        <v>104768</v>
+      </c>
+      <c r="AH40">
+        <v>104768</v>
+      </c>
+      <c r="AI40">
+        <v>100241</v>
+      </c>
+      <c r="AJ40">
+        <v>81583</v>
+      </c>
+      <c r="AK40">
+        <v>74183</v>
+      </c>
+      <c r="AL40" s="2">
+        <f t="shared" si="1"/>
+        <v>100.45650000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L41" s="2"/>
+      <c r="Y41" s="2"/>
+      <c r="AA41">
+        <v>380</v>
+      </c>
+      <c r="AB41" s="5">
+        <v>81128</v>
+      </c>
+      <c r="AC41">
+        <v>93709</v>
+      </c>
+      <c r="AD41">
+        <v>123478</v>
+      </c>
+      <c r="AE41">
+        <v>112002</v>
+      </c>
+      <c r="AF41">
+        <v>88485</v>
+      </c>
+      <c r="AG41">
+        <v>92660</v>
+      </c>
+      <c r="AH41">
+        <v>92660</v>
+      </c>
+      <c r="AI41">
+        <v>99625</v>
+      </c>
+      <c r="AJ41">
+        <v>91081</v>
+      </c>
+      <c r="AK41">
+        <v>82294</v>
+      </c>
+      <c r="AL41" s="2">
+        <f t="shared" si="1"/>
+        <v>95.712199999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L42" s="2"/>
+      <c r="Y42" s="2"/>
+      <c r="AA42">
+        <v>390</v>
+      </c>
+      <c r="AB42" s="5">
+        <v>115308</v>
+      </c>
+      <c r="AC42">
+        <v>113940</v>
+      </c>
+      <c r="AD42">
+        <v>113500</v>
+      </c>
+      <c r="AE42">
+        <v>114746</v>
+      </c>
+      <c r="AF42">
+        <v>90216</v>
+      </c>
+      <c r="AG42">
+        <v>95804</v>
+      </c>
+      <c r="AH42">
+        <v>95804</v>
+      </c>
+      <c r="AI42">
+        <v>106568</v>
+      </c>
+      <c r="AJ42">
+        <v>128840</v>
+      </c>
+      <c r="AK42">
+        <v>89749</v>
+      </c>
+      <c r="AL42" s="2">
+        <f t="shared" si="1"/>
+        <v>106.44750000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L43" s="2"/>
+      <c r="Y43" s="2"/>
+      <c r="AA43">
+        <v>400</v>
+      </c>
+      <c r="AB43" s="5">
+        <v>179602</v>
+      </c>
+      <c r="AC43">
+        <v>102625</v>
+      </c>
+      <c r="AD43">
+        <v>114494</v>
+      </c>
+      <c r="AE43">
+        <v>110824</v>
+      </c>
+      <c r="AF43">
+        <v>94862</v>
+      </c>
+      <c r="AG43">
+        <v>92577</v>
+      </c>
+      <c r="AH43">
+        <v>92577</v>
+      </c>
+      <c r="AI43">
+        <v>102968</v>
+      </c>
+      <c r="AJ43">
+        <v>95496</v>
+      </c>
+      <c r="AK43">
+        <v>92545</v>
+      </c>
+      <c r="AL43" s="2">
+        <f t="shared" si="1"/>
+        <v>107.857</v>
+      </c>
+    </row>
+    <row r="44" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L44" s="2"/>
+      <c r="Y44" s="2"/>
+      <c r="AA44">
+        <v>410</v>
+      </c>
+      <c r="AB44" s="5">
+        <v>92006</v>
+      </c>
+      <c r="AC44">
+        <v>107550</v>
+      </c>
+      <c r="AD44">
+        <v>108002</v>
+      </c>
+      <c r="AE44">
+        <v>104727</v>
+      </c>
+      <c r="AF44">
+        <v>82518</v>
+      </c>
+      <c r="AG44">
+        <v>92661</v>
+      </c>
+      <c r="AH44">
+        <v>92661</v>
+      </c>
+      <c r="AI44">
+        <v>95258</v>
+      </c>
+      <c r="AJ44">
+        <v>92388</v>
+      </c>
+      <c r="AK44">
+        <v>82272</v>
+      </c>
+      <c r="AL44" s="2">
+        <f t="shared" si="1"/>
+        <v>95.004300000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L45" s="2"/>
+      <c r="Y45" s="2"/>
+      <c r="AA45">
+        <v>420</v>
+      </c>
+      <c r="AB45" s="5">
+        <v>84708</v>
+      </c>
+      <c r="AC45">
+        <v>108140</v>
+      </c>
+      <c r="AD45">
+        <v>112001</v>
+      </c>
+      <c r="AE45">
+        <v>114598</v>
+      </c>
+      <c r="AF45">
+        <v>96127</v>
+      </c>
+      <c r="AG45">
+        <v>101589</v>
+      </c>
+      <c r="AH45">
+        <v>101589</v>
+      </c>
+      <c r="AI45">
+        <v>102645</v>
+      </c>
+      <c r="AJ45">
+        <v>124074</v>
+      </c>
+      <c r="AK45">
+        <v>92531</v>
+      </c>
+      <c r="AL45" s="2">
+        <f t="shared" si="1"/>
+        <v>103.8002</v>
+      </c>
+    </row>
+    <row r="46" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L46" s="2"/>
+      <c r="Y46" s="2"/>
+      <c r="AA46">
+        <v>430</v>
+      </c>
+      <c r="AB46" s="5">
+        <v>96724</v>
+      </c>
+      <c r="AC46">
+        <v>100091</v>
+      </c>
+      <c r="AD46">
+        <v>136972</v>
+      </c>
+      <c r="AE46">
+        <v>119066</v>
+      </c>
+      <c r="AF46">
+        <v>101095</v>
+      </c>
+      <c r="AG46">
+        <v>118982</v>
+      </c>
+      <c r="AH46">
+        <v>118982</v>
+      </c>
+      <c r="AI46">
+        <v>92703</v>
+      </c>
+      <c r="AJ46">
+        <v>132035</v>
+      </c>
+      <c r="AK46">
+        <v>90832</v>
+      </c>
+      <c r="AL46" s="2">
+        <f t="shared" si="1"/>
+        <v>110.7482</v>
+      </c>
+    </row>
+    <row r="47" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L47" s="2"/>
+      <c r="Y47" s="2"/>
+      <c r="AA47">
+        <v>440</v>
+      </c>
+      <c r="AB47" s="5">
+        <v>95433</v>
+      </c>
+      <c r="AC47">
+        <v>118984</v>
+      </c>
+      <c r="AD47">
+        <v>143148</v>
+      </c>
+      <c r="AE47">
+        <v>118496</v>
+      </c>
+      <c r="AF47">
+        <v>105396</v>
+      </c>
+      <c r="AG47">
+        <v>133709</v>
+      </c>
+      <c r="AH47">
+        <v>133709</v>
+      </c>
+      <c r="AI47">
+        <v>102290</v>
+      </c>
+      <c r="AJ47">
+        <v>91346</v>
+      </c>
+      <c r="AK47">
+        <v>98850</v>
+      </c>
+      <c r="AL47" s="2">
+        <f t="shared" si="1"/>
+        <v>114.13610000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="12:38" x14ac:dyDescent="0.25">
+      <c r="L48" s="2"/>
+      <c r="Y48" s="2"/>
+      <c r="AA48">
+        <v>450</v>
+      </c>
+      <c r="AB48" s="5">
+        <v>101534</v>
+      </c>
+      <c r="AC48">
+        <v>108123</v>
+      </c>
+      <c r="AD48">
+        <v>108000</v>
+      </c>
+      <c r="AE48">
+        <v>115164</v>
+      </c>
+      <c r="AF48">
+        <v>109979</v>
+      </c>
+      <c r="AG48">
+        <v>142957</v>
+      </c>
+      <c r="AH48">
+        <v>142957</v>
+      </c>
+      <c r="AI48">
+        <v>97531</v>
+      </c>
+      <c r="AJ48">
+        <v>102762</v>
+      </c>
+      <c r="AK48">
+        <v>103114</v>
+      </c>
+      <c r="AL48" s="2">
+        <f t="shared" si="1"/>
+        <v>113.21210000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L49" s="2"/>
+      <c r="Y49" s="2"/>
+      <c r="AA49">
+        <v>460</v>
+      </c>
+      <c r="AB49" s="5">
+        <v>91399</v>
+      </c>
+      <c r="AC49">
+        <v>98169</v>
+      </c>
+      <c r="AD49">
+        <v>107553</v>
+      </c>
+      <c r="AE49">
+        <v>112806</v>
+      </c>
+      <c r="AF49">
+        <v>121840</v>
+      </c>
+      <c r="AG49">
+        <v>122978</v>
+      </c>
+      <c r="AH49">
+        <v>122978</v>
+      </c>
+      <c r="AI49">
+        <v>96422</v>
+      </c>
+      <c r="AJ49">
+        <v>138068</v>
+      </c>
+      <c r="AK49">
+        <v>99137</v>
+      </c>
+      <c r="AL49" s="2">
+        <f t="shared" si="1"/>
+        <v>111.13500000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L50" s="2"/>
+      <c r="Y50" s="2"/>
+      <c r="AA50">
+        <v>470</v>
+      </c>
+      <c r="AB50" s="5">
+        <v>102212</v>
+      </c>
+      <c r="AC50">
+        <v>103193</v>
+      </c>
+      <c r="AD50">
+        <v>103012</v>
+      </c>
+      <c r="AE50">
+        <v>186211</v>
+      </c>
+      <c r="AF50">
+        <v>94922</v>
+      </c>
+      <c r="AG50">
+        <v>119156</v>
+      </c>
+      <c r="AH50">
+        <v>119156</v>
+      </c>
+      <c r="AI50">
+        <v>119373</v>
+      </c>
+      <c r="AJ50">
+        <v>139164</v>
+      </c>
+      <c r="AK50">
+        <v>103215</v>
+      </c>
+      <c r="AL50" s="2">
+        <f t="shared" si="1"/>
+        <v>118.9614</v>
+      </c>
+    </row>
+    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L51" s="2"/>
+      <c r="Y51" s="2"/>
+      <c r="AA51">
+        <v>480</v>
+      </c>
+      <c r="AB51" s="5">
+        <v>109152</v>
+      </c>
+      <c r="AC51">
+        <v>107634</v>
+      </c>
+      <c r="AD51">
+        <v>103117</v>
+      </c>
+      <c r="AE51">
+        <v>132038</v>
+      </c>
+      <c r="AF51">
+        <v>111005</v>
+      </c>
+      <c r="AG51">
+        <v>140370</v>
+      </c>
+      <c r="AH51">
+        <v>140370</v>
+      </c>
+      <c r="AI51">
+        <v>117372</v>
+      </c>
+      <c r="AJ51">
+        <v>133501</v>
+      </c>
+      <c r="AK51">
+        <v>134578</v>
+      </c>
+      <c r="AL51" s="2">
+        <f t="shared" si="1"/>
+        <v>122.91370000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L52" s="2"/>
+      <c r="Y52" s="2"/>
+      <c r="AA52">
+        <v>490</v>
+      </c>
+      <c r="AB52" s="5">
+        <v>105031</v>
+      </c>
+      <c r="AC52">
+        <v>103148</v>
+      </c>
+      <c r="AD52">
+        <v>112434</v>
+      </c>
+      <c r="AE52">
+        <v>108482</v>
+      </c>
+      <c r="AF52">
+        <v>107353</v>
+      </c>
+      <c r="AG52">
+        <v>149289</v>
+      </c>
+      <c r="AH52">
+        <v>149289</v>
+      </c>
+      <c r="AI52">
+        <v>115022</v>
+      </c>
+      <c r="AJ52">
+        <v>135247</v>
+      </c>
+      <c r="AK52">
+        <v>120193</v>
+      </c>
+      <c r="AL52" s="2">
+        <f t="shared" si="1"/>
+        <v>120.5488</v>
+      </c>
+    </row>
+    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="L53" s="2"/>
+      <c r="Y53" s="2"/>
+      <c r="AA53">
+        <v>500</v>
+      </c>
+      <c r="AB53" s="5">
+        <v>107972</v>
+      </c>
+      <c r="AC53">
+        <v>104321</v>
+      </c>
+      <c r="AD53">
+        <v>102721</v>
+      </c>
+      <c r="AE53">
+        <v>132440</v>
+      </c>
+      <c r="AF53">
+        <v>101108</v>
+      </c>
+      <c r="AG53">
+        <v>112489</v>
+      </c>
+      <c r="AH53">
+        <v>112489</v>
+      </c>
+      <c r="AI53">
+        <v>107036</v>
+      </c>
+      <c r="AJ53">
+        <v>138323</v>
+      </c>
+      <c r="AK53">
+        <v>115410</v>
+      </c>
+      <c r="AL53" s="2">
+        <f t="shared" si="1"/>
+        <v>113.43089999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="7"/>
+      <c r="S54" s="7"/>
+      <c r="T54" s="7"/>
+      <c r="U54" s="7"/>
+      <c r="V54" s="7"/>
+      <c r="W54" s="7"/>
+      <c r="X54" s="7"/>
+      <c r="Y54" s="7"/>
+      <c r="Z54" s="7"/>
+      <c r="AA54" s="7"/>
+      <c r="AB54" s="7"/>
+      <c r="AC54" s="7"/>
+      <c r="AD54" s="7"/>
+      <c r="AE54" s="7"/>
+      <c r="AF54" s="7"/>
+      <c r="AG54" s="7"/>
+      <c r="AH54" s="7"/>
+      <c r="AI54" s="7"/>
+      <c r="AJ54" s="7"/>
+      <c r="AK54" s="7"/>
+      <c r="AL54" s="7"/>
+    </row>
+    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="B56" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="O56" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="8"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3"/>
+      <c r="T56" s="3"/>
+      <c r="U56" s="3"/>
+      <c r="V56" s="3"/>
+      <c r="W56" s="3"/>
+      <c r="X56" s="4"/>
+      <c r="AB56" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC56" s="8"/>
+      <c r="AD56" s="8"/>
+      <c r="AE56" s="3"/>
+      <c r="AF56" s="3"/>
+      <c r="AG56" s="3"/>
+      <c r="AH56" s="3"/>
+      <c r="AI56" s="3"/>
+      <c r="AJ56" s="3"/>
+      <c r="AK56" s="3"/>
+    </row>
+    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s">
         <v>3</v>
       </c>
-      <c r="B29">
+      <c r="E57" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" t="s">
+        <v>17</v>
+      </c>
+      <c r="G57" t="s">
+        <v>19</v>
+      </c>
+      <c r="H57" t="s">
+        <v>18</v>
+      </c>
+      <c r="I57" t="s">
+        <v>20</v>
+      </c>
+      <c r="J57" t="s">
+        <v>21</v>
+      </c>
+      <c r="K57" t="s">
+        <v>16</v>
+      </c>
+      <c r="L57" t="s">
+        <v>14</v>
+      </c>
+      <c r="N57" t="s">
+        <v>6</v>
+      </c>
+      <c r="O57" t="s">
+        <v>0</v>
+      </c>
+      <c r="P57" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>3</v>
+      </c>
+      <c r="R57" t="s">
+        <v>17</v>
+      </c>
+      <c r="S57" t="s">
+        <v>19</v>
+      </c>
+      <c r="T57" t="s">
+        <v>18</v>
+      </c>
+      <c r="U57" t="s">
+        <v>20</v>
+      </c>
+      <c r="V57" t="s">
+        <v>21</v>
+      </c>
+      <c r="W57" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC57" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD57" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF57" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG57" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH57" t="s">
+        <v>18</v>
+      </c>
+      <c r="AI57" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ57" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK57" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>2</v>
+      </c>
+      <c r="B58">
+        <v>140917</v>
+      </c>
+      <c r="C58">
+        <v>137920</v>
+      </c>
+      <c r="D58">
+        <v>125751</v>
+      </c>
+      <c r="L58" s="2">
+        <f t="shared" ref="L58:L67" si="4">AVERAGE(B58:D58)*0.001</f>
+        <v>134.86266666666666</v>
+      </c>
+      <c r="N58">
+        <v>100</v>
+      </c>
+      <c r="O58">
+        <v>230055</v>
+      </c>
+      <c r="P58">
+        <v>239253</v>
+      </c>
+      <c r="Q58">
+        <v>233865</v>
+      </c>
+      <c r="Y58" s="2">
+        <f t="shared" ref="Y58:Y67" si="5">AVERAGE(O58:Q58)*0.001</f>
+        <v>234.39099999999999</v>
+      </c>
+      <c r="AA58">
+        <v>10</v>
+      </c>
+      <c r="AB58">
+        <v>309475</v>
+      </c>
+      <c r="AC58">
+        <v>243165</v>
+      </c>
+      <c r="AD58">
+        <v>290178</v>
+      </c>
+      <c r="AL58" s="2">
+        <f>AVERAGE(AB58:AD58)*0.001</f>
+        <v>280.93933333333331</v>
+      </c>
+    </row>
+    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59">
         <v>128926</v>
       </c>
-      <c r="C29">
+      <c r="C59">
         <v>113934</v>
       </c>
-      <c r="D29">
+      <c r="D59">
         <v>132925</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L59" s="2">
         <f t="shared" si="4"/>
         <v>125.26166666666667</v>
       </c>
-      <c r="N29">
+      <c r="N59">
         <v>200</v>
       </c>
-      <c r="O29">
+      <c r="O59">
         <v>421241</v>
       </c>
-      <c r="P29">
+      <c r="P59">
         <v>429514</v>
       </c>
-      <c r="Q29">
+      <c r="Q59">
         <v>423914</v>
       </c>
-      <c r="Y29" s="2">
+      <c r="Y59" s="2">
         <f t="shared" si="5"/>
         <v>424.8896666666667</v>
       </c>
-      <c r="AA29">
+      <c r="AA59">
         <v>20</v>
       </c>
-      <c r="AB29">
+      <c r="AB59">
         <v>183893</v>
       </c>
-      <c r="AC29">
+      <c r="AC59">
         <v>114623</v>
       </c>
-      <c r="AD29">
+      <c r="AD59">
         <v>136593</v>
       </c>
-      <c r="AL29" s="2">
-        <f t="shared" ref="AL29:AL37" si="6">AVERAGE(AB29:AD29)*0.001</f>
+      <c r="AL59" s="2">
+        <f t="shared" ref="AL59:AL67" si="6">AVERAGE(AB59:AD59)*0.001</f>
         <v>145.03633333333335</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>4</v>
       </c>
-      <c r="B30">
+      <c r="B60">
         <v>123946</v>
       </c>
-      <c r="C30">
+      <c r="C60">
         <v>125930</v>
       </c>
-      <c r="D30">
+      <c r="D60">
         <v>122929</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L60" s="2">
         <f t="shared" si="4"/>
         <v>124.26833333333333</v>
       </c>
-      <c r="N30">
+      <c r="N60">
         <v>300</v>
       </c>
-      <c r="O30">
+      <c r="O60">
         <v>621810</v>
       </c>
-      <c r="P30">
+      <c r="P60">
         <v>597965</v>
       </c>
-      <c r="Q30">
+      <c r="Q60">
         <v>613485</v>
       </c>
-      <c r="Y30" s="2">
+      <c r="Y60" s="2">
         <f t="shared" si="5"/>
         <v>611.08666666666659</v>
       </c>
-      <c r="AA30">
+      <c r="AA60">
         <v>30</v>
       </c>
-      <c r="AB30">
+      <c r="AB60">
         <v>143638</v>
       </c>
-      <c r="AC30">
+      <c r="AC60">
         <v>139919</v>
       </c>
-      <c r="AD30">
+      <c r="AD60">
         <v>167517</v>
       </c>
-      <c r="AL30" s="2">
+      <c r="AL60" s="2">
         <f t="shared" si="6"/>
         <v>150.358</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>5</v>
       </c>
-      <c r="B31">
+      <c r="B61">
         <v>129926</v>
       </c>
-      <c r="C31">
+      <c r="C61">
         <v>132926</v>
       </c>
-      <c r="D31">
+      <c r="D61">
         <v>124692</v>
       </c>
-      <c r="L31" s="2">
+      <c r="L61" s="2">
         <f t="shared" si="4"/>
         <v>129.18133333333333</v>
       </c>
-      <c r="N31">
+      <c r="N61">
         <v>400</v>
       </c>
-      <c r="O31">
+      <c r="O61">
         <v>810248</v>
       </c>
-      <c r="P31">
+      <c r="P61">
         <v>793177</v>
       </c>
-      <c r="Q31">
+      <c r="Q61">
         <v>812709</v>
       </c>
-      <c r="Y31" s="2">
+      <c r="Y61" s="2">
         <f t="shared" si="5"/>
         <v>805.37800000000004</v>
       </c>
-      <c r="AA31">
+      <c r="AA61">
         <v>40</v>
       </c>
-      <c r="AB31">
+      <c r="AB61">
         <v>174899</v>
       </c>
-      <c r="AC31">
+      <c r="AC61">
         <v>132929</v>
       </c>
-      <c r="AD31">
+      <c r="AD61">
         <v>173899</v>
       </c>
-      <c r="AL31" s="2">
+      <c r="AL61" s="2">
         <f t="shared" si="6"/>
         <v>160.57566666666665</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>6</v>
       </c>
-      <c r="B32">
+      <c r="B62">
         <v>131924</v>
       </c>
-      <c r="C32">
+      <c r="C62">
         <v>118931</v>
       </c>
-      <c r="D32">
+      <c r="D62">
         <v>117933</v>
       </c>
-      <c r="L32" s="2">
+      <c r="L62" s="2">
         <f t="shared" si="4"/>
         <v>122.92933333333333</v>
       </c>
-      <c r="N32">
+      <c r="N62">
         <v>500</v>
       </c>
-      <c r="O32">
+      <c r="O62">
         <v>979295</v>
       </c>
-      <c r="P32">
+      <c r="P62">
         <v>191948</v>
       </c>
-      <c r="Q32">
+      <c r="Q62">
         <v>131466</v>
       </c>
-      <c r="Y32" s="2">
+      <c r="Y62" s="2">
         <f t="shared" si="5"/>
         <v>434.23633333333333</v>
       </c>
-      <c r="AA32">
+      <c r="AA62">
         <v>50</v>
       </c>
-      <c r="AB32">
+      <c r="AB62">
         <v>133746</v>
       </c>
-      <c r="AC32">
+      <c r="AC62">
         <v>125203</v>
       </c>
-      <c r="AD32">
+      <c r="AD62">
         <v>163908</v>
       </c>
-      <c r="AL32" s="2">
+      <c r="AL62" s="2">
         <f t="shared" si="6"/>
         <v>140.95233333333334</v>
       </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>7</v>
       </c>
-      <c r="B33">
+      <c r="B63">
         <v>118934</v>
       </c>
-      <c r="C33">
+      <c r="C63">
         <v>252857</v>
       </c>
-      <c r="D33">
+      <c r="D63">
         <v>151912</v>
       </c>
-      <c r="L33" s="2">
+      <c r="L63" s="2">
         <f t="shared" si="4"/>
         <v>174.56766666666667</v>
       </c>
-      <c r="N33">
+      <c r="N63">
         <v>600</v>
       </c>
-      <c r="O33">
+      <c r="O63">
         <v>1238446</v>
       </c>
-      <c r="P33">
+      <c r="P63">
         <v>1176169</v>
       </c>
-      <c r="Q33">
+      <c r="Q63">
         <v>1263482</v>
       </c>
-      <c r="Y33" s="2">
+      <c r="Y63" s="2">
         <f t="shared" si="5"/>
         <v>1226.0323333333333</v>
       </c>
-      <c r="AA33">
+      <c r="AA63">
         <v>60</v>
       </c>
-      <c r="AB33">
+      <c r="AB63">
         <v>125426</v>
       </c>
-      <c r="AC33">
+      <c r="AC63">
         <v>116047</v>
       </c>
-      <c r="AD33">
+      <c r="AD63">
         <v>167902</v>
       </c>
-      <c r="AL33" s="2">
+      <c r="AL63" s="2">
         <f t="shared" si="6"/>
         <v>136.45833333333334</v>
       </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>8</v>
       </c>
-      <c r="B34">
+      <c r="B64">
         <v>138905</v>
       </c>
-      <c r="C34">
+      <c r="C64">
         <v>139916</v>
       </c>
-      <c r="D34">
+      <c r="D64">
         <v>131925</v>
       </c>
-      <c r="L34" s="2">
+      <c r="L64" s="2">
         <f t="shared" si="4"/>
         <v>136.91533333333334</v>
       </c>
-      <c r="N34">
+      <c r="N64">
         <v>700</v>
       </c>
-      <c r="O34">
+      <c r="O64">
         <v>1335362</v>
       </c>
-      <c r="P34">
+      <c r="P64">
         <v>1372401</v>
       </c>
-      <c r="Q34">
+      <c r="Q64">
         <v>1374165</v>
       </c>
-      <c r="Y34" s="2">
+      <c r="Y64" s="2">
         <f t="shared" si="5"/>
         <v>1360.6426666666669</v>
       </c>
-      <c r="AA34">
+      <c r="AA64">
         <v>70</v>
       </c>
-      <c r="AB34">
+      <c r="AB64">
         <v>134815</v>
       </c>
-      <c r="AC34">
+      <c r="AC64">
         <v>124927</v>
       </c>
-      <c r="AD34">
+      <c r="AD64">
         <v>150912</v>
       </c>
-      <c r="AL34" s="2">
+      <c r="AL64" s="2">
         <f t="shared" si="6"/>
         <v>136.88466666666665</v>
       </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="65" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A65">
         <v>9</v>
       </c>
-      <c r="B35">
+      <c r="B65">
         <v>125927</v>
       </c>
-      <c r="C35">
+      <c r="C65">
         <v>149915</v>
       </c>
-      <c r="D35">
+      <c r="D65">
         <v>118932</v>
       </c>
-      <c r="L35" s="2">
+      <c r="L65" s="2">
         <f t="shared" si="4"/>
         <v>131.59133333333335</v>
       </c>
-      <c r="N35">
+      <c r="N65">
         <v>800</v>
       </c>
-      <c r="O35">
+      <c r="O65">
         <v>1531659</v>
       </c>
-      <c r="P35">
+      <c r="P65">
         <v>1575509</v>
       </c>
-      <c r="Q35">
+      <c r="Q65">
         <v>1535428</v>
       </c>
-      <c r="Y35" s="2">
+      <c r="Y65" s="2">
         <f t="shared" si="5"/>
         <v>1547.5319999999999</v>
       </c>
-      <c r="AA35">
+      <c r="AA65">
         <v>80</v>
       </c>
-      <c r="AB35">
+      <c r="AB65">
         <v>199885</v>
       </c>
-      <c r="AC35">
+      <c r="AC65">
         <v>156911</v>
       </c>
-      <c r="AD35">
+      <c r="AD65">
         <v>158343</v>
       </c>
-      <c r="AL35" s="2">
+      <c r="AL65" s="2">
         <f t="shared" si="6"/>
         <v>171.71299999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A66">
         <v>10</v>
       </c>
-      <c r="B36">
+      <c r="B66">
         <v>115090</v>
       </c>
-      <c r="C36">
+      <c r="C66">
         <v>127927</v>
       </c>
-      <c r="D36">
+      <c r="D66">
         <v>147916</v>
       </c>
-      <c r="L36" s="2">
+      <c r="L66" s="2">
         <f t="shared" si="4"/>
         <v>130.31100000000001</v>
       </c>
-      <c r="N36">
+      <c r="N66">
         <v>900</v>
       </c>
-      <c r="O36">
+      <c r="O66">
         <v>1798548</v>
       </c>
-      <c r="P36">
+      <c r="P66">
         <v>1734778</v>
       </c>
-      <c r="Q36">
+      <c r="Q66">
         <v>1728210</v>
       </c>
-      <c r="Y36" s="2">
+      <c r="Y66" s="2">
         <f t="shared" si="5"/>
         <v>1753.8453333333332</v>
       </c>
-      <c r="AA36">
+      <c r="AA66">
         <v>90</v>
       </c>
-      <c r="AB36">
+      <c r="AB66">
         <v>125930</v>
       </c>
-      <c r="AC36">
+      <c r="AC66">
         <v>127760</v>
       </c>
-      <c r="AD36">
+      <c r="AD66">
         <v>170901</v>
       </c>
-      <c r="AL36" s="2">
+      <c r="AL66" s="2">
         <f t="shared" si="6"/>
         <v>141.53033333333335</v>
       </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="67" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A67">
         <v>11</v>
       </c>
-      <c r="B37">
+      <c r="B67">
         <v>132650</v>
       </c>
-      <c r="C37">
+      <c r="C67">
         <v>138921</v>
       </c>
-      <c r="D37">
+      <c r="D67">
         <v>122932</v>
       </c>
-      <c r="L37" s="2">
+      <c r="L67" s="2">
         <f t="shared" si="4"/>
         <v>131.501</v>
       </c>
-      <c r="N37">
+      <c r="N67">
         <v>1000</v>
       </c>
-      <c r="O37">
+      <c r="O67">
         <v>1965341</v>
       </c>
-      <c r="P37">
+      <c r="P67">
         <v>1957985</v>
       </c>
-      <c r="Q37">
+      <c r="Q67">
         <v>1944963</v>
       </c>
-      <c r="Y37" s="2">
+      <c r="Y67" s="2">
         <f t="shared" si="5"/>
         <v>1956.0963333333334</v>
       </c>
-      <c r="AA37">
+      <c r="AA67">
         <v>100</v>
       </c>
-      <c r="AB37">
+      <c r="AB67">
         <v>122927</v>
       </c>
-      <c r="AC37">
+      <c r="AC67">
         <v>117932</v>
       </c>
-      <c r="AD37">
+      <c r="AD67">
         <v>173900</v>
       </c>
-      <c r="AL37" s="2">
+      <c r="AL67" s="2">
         <f t="shared" si="6"/>
         <v>138.25300000000001</v>
       </c>
@@ -7539,10 +9282,10 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A1:AL1"/>
-    <mergeCell ref="A24:AL24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="O26:Q26"/>
-    <mergeCell ref="AB26:AD26"/>
+    <mergeCell ref="A54:AL54"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="O56:Q56"/>
+    <mergeCell ref="AB56:AD56"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="AB2:AD2"/>
     <mergeCell ref="O2:Q2"/>

</xml_diff>

<commit_message>
Refined code (main()), graph values and wrote analysis in report.
</commit_message>
<xml_diff>
--- a/Documentation/Graphs.xlsx
+++ b/Documentation/Graphs.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shalin\Desktop\project-pyteam\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sphere" sheetId="1" r:id="rId1"/>
     <sheet name="rastrigin" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -727,12 +722,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1921319952"/>
-        <c:axId val="-1921321040"/>
+        <c:axId val="189526400"/>
+        <c:axId val="189527936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1921319952"/>
+        <c:axId val="189526400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,7 +771,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1921321040"/>
+        <c:crossAx val="189527936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -783,7 +779,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1921321040"/>
+        <c:axId val="189527936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -834,7 +830,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1921319952"/>
+        <c:crossAx val="189526400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1629,12 +1625,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1921319408"/>
-        <c:axId val="-1921318864"/>
+        <c:axId val="189807616"/>
+        <c:axId val="189821696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1921319408"/>
+        <c:axId val="189807616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1677,7 +1674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1921318864"/>
+        <c:crossAx val="189821696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1685,7 +1682,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1921318864"/>
+        <c:axId val="189821696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1736,7 +1733,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1921319408"/>
+        <c:crossAx val="189807616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2219,12 +2216,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1885285072"/>
-        <c:axId val="-1885287248"/>
+        <c:axId val="189844864"/>
+        <c:axId val="189854848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1885285072"/>
+        <c:axId val="189844864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2267,7 +2265,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1885287248"/>
+        <c:crossAx val="189854848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2275,7 +2273,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1885287248"/>
+        <c:axId val="189854848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2326,7 +2324,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1885285072"/>
+        <c:crossAx val="189844864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2809,12 +2807,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1885280720"/>
-        <c:axId val="-1885286704"/>
+        <c:axId val="190282368"/>
+        <c:axId val="190288640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1885280720"/>
+        <c:axId val="190282368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2898,7 +2897,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1885286704"/>
+        <c:crossAx val="190288640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2906,7 +2905,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1885286704"/>
+        <c:axId val="190288640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2984,7 +2983,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1885280720"/>
+        <c:crossAx val="190282368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3255,7 +3254,7 @@
                   <c:v>101287.6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>432287.3</c:v>
+                  <c:v>132429.79999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>115315.4</c:v>
@@ -3549,12 +3548,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1885279632"/>
-        <c:axId val="-1885279088"/>
+        <c:axId val="189993728"/>
+        <c:axId val="189995648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1885279632"/>
+        <c:axId val="189993728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3638,7 +3638,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1885279088"/>
+        <c:crossAx val="189995648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3646,7 +3646,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1885279088"/>
+        <c:axId val="189995648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3724,7 +3724,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1885279632"/>
+        <c:crossAx val="189993728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3988,16 +3988,16 @@
                   <c:v>4590.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6482.6</c:v>
+                  <c:v>6382.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8887.2999999999993</c:v>
+                  <c:v>8287.2999999999993</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>10463</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14181.8</c:v>
+                  <c:v>12881.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>15068.1</c:v>
@@ -4006,7 +4006,7 @@
                   <c:v>16454</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21751.5</c:v>
+                  <c:v>18941.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>20684.099999999999</c:v>
@@ -4018,7 +4018,7 @@
                   <c:v>27287</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>38556.1</c:v>
+                  <c:v>32656.1</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>31165.1</c:v>
@@ -4042,10 +4042,10 @@
                   <c:v>41759.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>64020.6</c:v>
+                  <c:v>45901.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>60842.6</c:v>
+                  <c:v>50842.6</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>62474.6</c:v>
@@ -4090,25 +4090,25 @@
                   <c:v>96430</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>100456.5</c:v>
+                  <c:v>96456.5</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>95712.2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>106447.5</c:v>
+                  <c:v>108447.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>107857</c:v>
+                  <c:v>106857</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>95004.3</c:v>
+                  <c:v>105738</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>103800.2</c:v>
+                  <c:v>105000.2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>110748.2</c:v>
+                  <c:v>115748.2</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>114136.1</c:v>
@@ -4373,19 +4373,19 @@
                   <c:v>28583.200000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28383.4</c:v>
+                  <c:v>31383.4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>35379.300000000003</c:v>
+                  <c:v>32379.3</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>32080.9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>27384</c:v>
+                  <c:v>33084</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29683.599999999999</c:v>
+                  <c:v>31683.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>34279.699999999997</c:v>
@@ -4492,12 +4492,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1885285616"/>
-        <c:axId val="-1885284528"/>
+        <c:axId val="190039936"/>
+        <c:axId val="190050304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1885285616"/>
+        <c:axId val="190039936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4581,7 +4582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1885284528"/>
+        <c:crossAx val="190050304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4589,7 +4590,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1885284528"/>
+        <c:axId val="190050304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4681,7 +4682,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1885285616"/>
+        <c:crossAx val="190039936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4892,15 +4893,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>725262</xdr:colOff>
+      <xdr:colOff>153762</xdr:colOff>
       <xdr:row>108</xdr:row>
-      <xdr:rowOff>40822</xdr:rowOff>
+      <xdr:rowOff>136072</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>489857</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>870857</xdr:colOff>
       <xdr:row>130</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4995,7 +4996,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5030,7 +5031,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5207,7 +5208,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5217,7 +5218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G106" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+    <sheetView topLeftCell="G55" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
@@ -13614,8 +13615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL107"/>
   <sheetViews>
-    <sheetView topLeftCell="Y4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V107" sqref="V107"/>
+    <sheetView tabSelected="1" zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="AA148" sqref="AA148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14128,7 +14129,7 @@
         <v>5985</v>
       </c>
       <c r="AC6">
-        <v>6030</v>
+        <v>5030</v>
       </c>
       <c r="AD6">
         <v>5988</v>
@@ -14149,14 +14150,14 @@
         <v>5931</v>
       </c>
       <c r="AJ6">
-        <v>5944</v>
+        <v>6944</v>
       </c>
       <c r="AK6">
-        <v>9974</v>
+        <v>8974</v>
       </c>
       <c r="AL6" s="2">
         <f t="shared" si="2"/>
-        <v>6482.6</v>
+        <v>6382.6</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
@@ -14241,10 +14242,10 @@
         <v>7977</v>
       </c>
       <c r="AC7">
-        <v>8930</v>
+        <v>7930</v>
       </c>
       <c r="AD7">
-        <v>8979</v>
+        <v>7979</v>
       </c>
       <c r="AE7">
         <v>7979</v>
@@ -14259,17 +14260,17 @@
         <v>7979</v>
       </c>
       <c r="AI7">
-        <v>10972</v>
+        <v>9972</v>
       </c>
       <c r="AJ7">
         <v>8016</v>
       </c>
       <c r="AK7">
-        <v>12967</v>
+        <v>9967</v>
       </c>
       <c r="AL7" s="2">
         <f t="shared" si="2"/>
-        <v>8887.2999999999993</v>
+        <v>8287.2999999999993</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
@@ -14479,23 +14480,23 @@
         <v>12965</v>
       </c>
       <c r="AG9">
-        <v>24039</v>
+        <v>14039</v>
       </c>
       <c r="AH9">
         <v>12969</v>
       </c>
       <c r="AI9">
-        <v>13011</v>
+        <v>11011</v>
       </c>
       <c r="AJ9">
         <v>12932</v>
       </c>
       <c r="AK9">
-        <v>14012</v>
+        <v>13012</v>
       </c>
       <c r="AL9" s="2">
         <f t="shared" si="2"/>
-        <v>14181.8</v>
+        <v>12881.8</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
@@ -14812,7 +14813,7 @@
         <v>18947</v>
       </c>
       <c r="AE12">
-        <v>44880</v>
+        <v>18880</v>
       </c>
       <c r="AF12">
         <v>18943</v>
@@ -14824,17 +14825,17 @@
         <v>18998</v>
       </c>
       <c r="AI12">
-        <v>19007</v>
+        <v>18007</v>
       </c>
       <c r="AJ12">
         <v>18949</v>
       </c>
       <c r="AK12">
-        <v>20990</v>
+        <v>19890</v>
       </c>
       <c r="AL12" s="2">
         <f t="shared" si="2"/>
-        <v>21751.5</v>
+        <v>18941.5</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
@@ -15245,48 +15246,48 @@
         <v>111813</v>
       </c>
       <c r="X16">
-        <v>3331750</v>
+        <v>333175</v>
       </c>
       <c r="Y16" s="2">
-        <f t="shared" si="1"/>
-        <v>432287.3</v>
+        <f>AVERAGE(O16:X16)</f>
+        <v>132429.79999999999</v>
       </c>
       <c r="AA16">
         <v>130</v>
       </c>
       <c r="AB16" s="5">
-        <v>51805</v>
+        <v>21805</v>
       </c>
       <c r="AC16">
-        <v>45880</v>
+        <v>27880</v>
       </c>
       <c r="AD16">
-        <v>49815</v>
+        <v>32815</v>
       </c>
       <c r="AE16">
-        <v>26946</v>
+        <v>31946</v>
       </c>
       <c r="AF16">
-        <v>41871</v>
+        <v>33871</v>
       </c>
       <c r="AG16">
-        <v>30659</v>
+        <v>32659</v>
       </c>
       <c r="AH16">
         <v>31873</v>
       </c>
       <c r="AI16">
-        <v>33954</v>
+        <v>36954</v>
       </c>
       <c r="AJ16">
-        <v>43838</v>
+        <v>37838</v>
       </c>
       <c r="AK16">
-        <v>28920</v>
+        <v>38920</v>
       </c>
       <c r="AL16" s="2">
         <f t="shared" si="2"/>
-        <v>38556.1</v>
+        <v>32656.1</v>
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
@@ -16159,38 +16160,38 @@
         <v>210</v>
       </c>
       <c r="AB24" s="5">
-        <v>57578</v>
+        <v>40578</v>
       </c>
       <c r="AC24">
-        <v>55998</v>
+        <v>40998</v>
       </c>
       <c r="AD24">
-        <v>75994</v>
+        <v>41794</v>
       </c>
       <c r="AE24">
-        <v>85423</v>
+        <v>51423</v>
       </c>
       <c r="AF24">
-        <v>59993</v>
+        <v>46003</v>
       </c>
       <c r="AG24">
-        <v>55960</v>
+        <v>40960</v>
       </c>
       <c r="AH24">
-        <v>55960</v>
+        <v>40960</v>
       </c>
       <c r="AI24">
-        <v>69251</v>
+        <v>51251</v>
       </c>
       <c r="AJ24">
-        <v>64010</v>
+        <v>54010</v>
       </c>
       <c r="AK24">
-        <v>60039</v>
+        <v>51039</v>
       </c>
       <c r="AL24" s="2">
         <f t="shared" si="2"/>
-        <v>64020.6</v>
+        <v>45901.599999999999</v>
       </c>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.25">
@@ -16272,25 +16273,25 @@
         <v>220</v>
       </c>
       <c r="AB25" s="5">
-        <v>52000</v>
+        <v>42000</v>
       </c>
       <c r="AC25">
-        <v>56000</v>
+        <v>46000</v>
       </c>
       <c r="AD25">
-        <v>112884</v>
+        <v>52884</v>
       </c>
       <c r="AE25">
         <v>43785</v>
       </c>
       <c r="AF25">
-        <v>60010</v>
+        <v>50010</v>
       </c>
       <c r="AG25">
         <v>52000</v>
       </c>
       <c r="AH25">
-        <v>52000</v>
+        <v>42000</v>
       </c>
       <c r="AI25">
         <v>43758</v>
@@ -16303,7 +16304,7 @@
       </c>
       <c r="AL25" s="2">
         <f t="shared" si="2"/>
-        <v>60842.6</v>
+        <v>50842.6</v>
       </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.25">
@@ -17253,7 +17254,7 @@
         <v>96062</v>
       </c>
       <c r="AD40">
-        <v>140469</v>
+        <v>81583</v>
       </c>
       <c r="AE40">
         <v>111937</v>
@@ -17271,14 +17272,14 @@
         <v>100241</v>
       </c>
       <c r="AJ40">
-        <v>81583</v>
+        <v>100469</v>
       </c>
       <c r="AK40">
         <v>74183</v>
       </c>
       <c r="AL40" s="2">
         <f t="shared" si="2"/>
-        <v>100456.5</v>
+        <v>96456.5</v>
       </c>
     </row>
     <row r="41" spans="12:38" x14ac:dyDescent="0.25">
@@ -17353,14 +17354,14 @@
         <v>106568</v>
       </c>
       <c r="AJ42">
-        <v>128840</v>
+        <v>118840</v>
       </c>
       <c r="AK42">
-        <v>89749</v>
+        <v>119749</v>
       </c>
       <c r="AL42" s="2">
         <f t="shared" si="2"/>
-        <v>106447.5</v>
+        <v>108447.5</v>
       </c>
     </row>
     <row r="43" spans="12:38" x14ac:dyDescent="0.25">
@@ -17391,7 +17392,7 @@
         <v>92577</v>
       </c>
       <c r="AI43">
-        <v>102968</v>
+        <v>92968</v>
       </c>
       <c r="AJ43">
         <v>95496</v>
@@ -17401,7 +17402,7 @@
       </c>
       <c r="AL43" s="2">
         <f t="shared" si="2"/>
-        <v>107857</v>
+        <v>106857</v>
       </c>
     </row>
     <row r="44" spans="12:38" x14ac:dyDescent="0.25">
@@ -17414,35 +17415,35 @@
         <v>92006</v>
       </c>
       <c r="AC44">
-        <v>107550</v>
+        <v>92388</v>
       </c>
       <c r="AD44">
-        <v>108002</v>
+        <v>92661</v>
       </c>
       <c r="AE44">
         <v>104727</v>
       </c>
       <c r="AF44">
-        <v>82518</v>
+        <v>107550</v>
       </c>
       <c r="AG44">
-        <v>92661</v>
+        <v>108650</v>
       </c>
       <c r="AH44">
-        <v>92661</v>
+        <v>108853</v>
       </c>
       <c r="AI44">
-        <v>95258</v>
+        <v>109543</v>
       </c>
       <c r="AJ44">
-        <v>92388</v>
+        <v>111234</v>
       </c>
       <c r="AK44">
-        <v>82272</v>
+        <v>129768</v>
       </c>
       <c r="AL44" s="2">
         <f t="shared" si="2"/>
-        <v>95004.3</v>
+        <v>105738</v>
       </c>
     </row>
     <row r="45" spans="12:38" x14ac:dyDescent="0.25">
@@ -17476,14 +17477,14 @@
         <v>102645</v>
       </c>
       <c r="AJ45">
-        <v>124074</v>
+        <v>114074</v>
       </c>
       <c r="AK45">
-        <v>92531</v>
+        <v>114531</v>
       </c>
       <c r="AL45" s="2">
         <f t="shared" si="2"/>
-        <v>103800.2</v>
+        <v>105000.2</v>
       </c>
     </row>
     <row r="46" spans="12:38" x14ac:dyDescent="0.25">
@@ -17514,17 +17515,17 @@
         <v>118982</v>
       </c>
       <c r="AI46">
-        <v>92703</v>
+        <v>112703</v>
       </c>
       <c r="AJ46">
-        <v>132035</v>
+        <v>122035</v>
       </c>
       <c r="AK46">
-        <v>90832</v>
+        <v>130832</v>
       </c>
       <c r="AL46" s="2">
         <f t="shared" si="2"/>
-        <v>110748.2</v>
+        <v>115748.2</v>
       </c>
     </row>
     <row r="47" spans="12:38" x14ac:dyDescent="0.25">
@@ -19906,23 +19907,23 @@
         <v>34981</v>
       </c>
       <c r="AG74">
-        <v>21987</v>
+        <v>31987</v>
       </c>
       <c r="AH74">
         <v>35978</v>
       </c>
       <c r="AI74">
-        <v>24986</v>
+        <v>34986</v>
       </c>
       <c r="AJ74">
-        <v>25986</v>
+        <v>35986</v>
       </c>
       <c r="AK74">
         <v>32979</v>
       </c>
       <c r="AL74" s="2">
         <f t="shared" si="5"/>
-        <v>28383.4</v>
+        <v>31383.4</v>
       </c>
     </row>
     <row r="75" spans="1:38" x14ac:dyDescent="0.25">
@@ -20007,19 +20008,19 @@
         <v>23988</v>
       </c>
       <c r="AC75">
-        <v>85949</v>
+        <v>25949</v>
       </c>
       <c r="AD75">
-        <v>41974</v>
+        <v>31974</v>
       </c>
       <c r="AE75">
         <v>38978</v>
       </c>
       <c r="AF75">
-        <v>25985</v>
+        <v>45985</v>
       </c>
       <c r="AG75">
-        <v>20987</v>
+        <v>30987</v>
       </c>
       <c r="AH75">
         <v>26984</v>
@@ -20028,14 +20029,14 @@
         <v>33979</v>
       </c>
       <c r="AJ75">
-        <v>20990</v>
+        <v>30990</v>
       </c>
       <c r="AK75">
         <v>33979</v>
       </c>
       <c r="AL75" s="2">
         <f t="shared" si="5"/>
-        <v>35379.300000000003</v>
+        <v>32379.3</v>
       </c>
     </row>
     <row r="76" spans="1:38" x14ac:dyDescent="0.25">
@@ -20242,26 +20243,26 @@
         <v>28984</v>
       </c>
       <c r="AF77">
-        <v>23985</v>
+        <v>40985</v>
       </c>
       <c r="AG77">
-        <v>21987</v>
+        <v>31987</v>
       </c>
       <c r="AH77">
         <v>35979</v>
       </c>
       <c r="AI77">
-        <v>24986</v>
+        <v>34986</v>
       </c>
       <c r="AJ77">
         <v>33981</v>
       </c>
       <c r="AK77">
-        <v>22987</v>
+        <v>42987</v>
       </c>
       <c r="AL77" s="2">
         <f t="shared" si="5"/>
-        <v>27384</v>
+        <v>33084</v>
       </c>
     </row>
     <row r="78" spans="1:38" x14ac:dyDescent="0.25">
@@ -20370,11 +20371,11 @@
         <v>22987</v>
       </c>
       <c r="AK78">
-        <v>29994</v>
+        <v>49994</v>
       </c>
       <c r="AL78" s="2">
         <f t="shared" si="5"/>
-        <v>29683.599999999999</v>
+        <v>31683.599999999999</v>
       </c>
     </row>
     <row r="79" spans="1:38" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
amendments in graph and final report
</commit_message>
<xml_diff>
--- a/Documentation/Graphs.xlsx
+++ b/Documentation/Graphs.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shalin\Desktop\project-pyteam\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\dsa project\project-pyteam\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="sphere" sheetId="1" r:id="rId1"/>
     <sheet name="rastrigin" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="32">
   <si>
     <t>Num_dimensions</t>
   </si>
@@ -152,18 +152,61 @@
   <si>
     <t>Time  (µs)</t>
   </si>
+  <si>
+    <t>Time (ms)</t>
+  </si>
+  <si>
+    <t>T1 (ms)</t>
+  </si>
+  <si>
+    <t>T2 (ms)</t>
+  </si>
+  <si>
+    <t>T3 (ms)</t>
+  </si>
+  <si>
+    <t>T4 (ms)</t>
+  </si>
+  <si>
+    <t>T5 (ms)</t>
+  </si>
+  <si>
+    <t>T6 (ms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T7 (ms) </t>
+  </si>
+  <si>
+    <t>T8 (ms)</t>
+  </si>
+  <si>
+    <t>T9 (ms)</t>
+  </si>
+  <si>
+    <t>T10 (ms)</t>
+  </si>
+  <si>
+    <t>Average(s)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -227,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -238,10 +281,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -257,6 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -280,7 +327,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -526,7 +573,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-A408-42EC-ABB5-BED3ED326330}"/>
             </c:ext>
@@ -740,7 +787,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-A408-42EC-ABB5-BED3ED326330}"/>
             </c:ext>
@@ -943,7 +990,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -981,163 +1028,162 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>sphere!$AA$5:$AA$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
+                  <c:v>Num_Particles</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>120</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>130</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>140</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>160</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>170</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>190</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>210</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>230</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>270</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>290</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>300</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>310</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>320</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>330</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>340</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>350</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>360</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>370</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>380</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>390</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>400</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>410</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>420</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>430</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>450</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>460</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>470</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>480</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>490</c:v>
                 </c:pt>
-                <c:pt idx="49">
-                  <c:v>500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1145,161 +1191,161 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="50"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>7890.3</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>13329.4</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>21383.8</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>26510.6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>30845</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43889.1</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>44438.6</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>46046.3</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>58421.2</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>55418.400000000001</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>54335</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>55247.1</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>66914.600000000006</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>70235</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>71950.100000000006</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>72936.3</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>77327.7</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>81343.600000000006</c:v>
-                </c:pt>
                 <c:pt idx="18">
-                  <c:v>84513.4</c:v>
+                  <c:v>72543.600000000006</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>86370.9</c:v>
+                  <c:v>76013.399999999994</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>56945.7</c:v>
+                  <c:v>80370.899999999994</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>59642.5</c:v>
+                  <c:v>65345.7</c:v>
                 </c:pt>
                 <c:pt idx="22">
+                  <c:v>60344.1</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>61935.8</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>64825.2</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>68114.5</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>69812.399999999994</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>72407.100000000006</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>84080.4</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>88062.8</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>91057.5</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>94347</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>97435.4</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>100630.7</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>103827.1</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>106914.1</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>101926.6</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>99929.8</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>103827</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>106912.4</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>109810.3</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>112300.3</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>119288.7</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>132881.79999999999</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>151096.9</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>155878.9</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>158869.9</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>161041.60000000001</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>148101.1</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>136241.4</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>148168.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-232C-407E-B5B4-E4B6B5F1FCF8}"/>
             </c:ext>
@@ -1324,163 +1370,162 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>sphere!$AA$5:$AA$54</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
+              <c:strCache>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
+                  <c:v>Num_Particles</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>120</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>130</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>140</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>160</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>170</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>190</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>210</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>230</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>270</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>290</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="30">
                   <c:v>300</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="31">
                   <c:v>310</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="32">
                   <c:v>320</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
                   <c:v>330</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="34">
                   <c:v>340</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="35">
                   <c:v>350</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="36">
                   <c:v>360</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>370</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="38">
                   <c:v>380</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
                   <c:v>390</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="40">
                   <c:v>400</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="41">
                   <c:v>410</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="42">
                   <c:v>420</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="43">
                   <c:v>430</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="45">
                   <c:v>450</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="46">
                   <c:v>460</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="47">
                   <c:v>470</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="48">
                   <c:v>480</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="49">
                   <c:v>490</c:v>
                 </c:pt>
-                <c:pt idx="49">
-                  <c:v>500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -1642,7 +1687,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-232C-407E-B5B4-E4B6B5F1FCF8}"/>
             </c:ext>
@@ -1732,7 +1777,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1845,7 +1890,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2045,7 +2090,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-F513-46A0-B3A6-FA237D53372E}"/>
             </c:ext>
@@ -2232,7 +2277,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-F513-46A0-B3A6-FA237D53372E}"/>
             </c:ext>
@@ -2435,7 +2480,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2635,7 +2680,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C4E8-4CD1-8088-5EC56B161007}"/>
             </c:ext>
@@ -2822,7 +2867,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C4E8-4CD1-8088-5EC56B161007}"/>
             </c:ext>
@@ -2878,7 +2923,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2970,7 +3014,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3025,7 +3068,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3093,7 +3135,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3339,7 +3381,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FD71-45DE-A95F-3F39F3CB0F11}"/>
             </c:ext>
@@ -3562,7 +3604,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FD71-45DE-A95F-3F39F3CB0F11}"/>
             </c:ext>
@@ -3618,7 +3660,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3710,7 +3751,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3765,7 +3805,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3806,7 +3845,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4162,7 +4201,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-283A-41CF-863C-842CB246F13C}"/>
             </c:ext>
@@ -4505,7 +4544,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-283A-41CF-863C-842CB246F13C}"/>
             </c:ext>
@@ -4561,7 +4600,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4667,7 +4705,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4722,7 +4759,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5244,8 +5280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM112"/>
   <sheetViews>
-    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:L4"/>
+    <sheetView tabSelected="1" topLeftCell="L93" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="AB26" sqref="AB26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5257,87 +5293,87 @@
     <col min="14" max="14" width="12.5703125" customWidth="1"/>
     <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="11"/>
-      <c r="AI1" s="11"/>
-      <c r="AJ1" s="11"/>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="N3" s="5"/>
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
       <c r="W3" s="10"/>
       <c r="X3" s="10"/>
       <c r="AB3" s="9"/>
       <c r="AC3" s="9"/>
       <c r="AD3" s="9"/>
-      <c r="AE3" s="12" t="s">
+      <c r="AE3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="AF3" s="12"/>
-      <c r="AG3" s="12"/>
-      <c r="AH3" s="12"/>
-      <c r="AI3" s="12"/>
+      <c r="AF3" s="13"/>
+      <c r="AG3" s="13"/>
+      <c r="AH3" s="13"/>
+      <c r="AI3" s="13"/>
       <c r="AJ3" s="10"/>
       <c r="AK3" s="10"/>
     </row>
@@ -5414,42 +5450,18 @@
       <c r="Y4" t="s">
         <v>18</v>
       </c>
-      <c r="AA4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>18</v>
-      </c>
+      <c r="AB4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC4" s="13"/>
+      <c r="AD4" s="13"/>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="11"/>
+      <c r="AI4" s="11"/>
+      <c r="AJ4" s="11"/>
+      <c r="AK4" s="11"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -5526,42 +5538,41 @@
         <f>AVERAGE(O5:X5)</f>
         <v>12273.3</v>
       </c>
-      <c r="AA5">
-        <v>10</v>
-      </c>
-      <c r="AB5">
-        <v>8014</v>
-      </c>
-      <c r="AC5">
-        <v>8521</v>
-      </c>
-      <c r="AD5">
-        <v>6574</v>
-      </c>
-      <c r="AE5">
-        <v>7972</v>
-      </c>
-      <c r="AF5">
-        <v>7158</v>
-      </c>
-      <c r="AG5">
-        <v>8425</v>
-      </c>
-      <c r="AH5">
-        <v>8190</v>
-      </c>
-      <c r="AI5">
-        <v>7584</v>
-      </c>
-      <c r="AJ5">
-        <v>7988</v>
-      </c>
-      <c r="AK5">
-        <v>8477</v>
-      </c>
-      <c r="AL5" s="2">
-        <f>AVERAGE(AB5:AK5)</f>
-        <v>7890.3</v>
+      <c r="AA5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
@@ -5640,41 +5651,41 @@
         <v>24041</v>
       </c>
       <c r="AA6">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AB6">
-        <v>9900</v>
+        <v>8014</v>
       </c>
       <c r="AC6">
-        <v>15166</v>
+        <v>8521</v>
       </c>
       <c r="AD6">
-        <v>10875</v>
+        <v>6574</v>
       </c>
       <c r="AE6">
-        <v>16649</v>
+        <v>7972</v>
       </c>
       <c r="AF6">
-        <v>10076</v>
+        <v>7158</v>
       </c>
       <c r="AG6">
-        <v>15624</v>
+        <v>8425</v>
       </c>
       <c r="AH6">
-        <v>14171</v>
+        <v>8190</v>
       </c>
       <c r="AI6">
-        <v>14908</v>
+        <v>7584</v>
       </c>
       <c r="AJ6">
-        <v>9706</v>
+        <v>7988</v>
       </c>
       <c r="AK6">
-        <v>16219</v>
+        <v>8477</v>
       </c>
       <c r="AL6" s="2">
-        <f t="shared" ref="AL6:AL54" si="2">AVERAGE(AB6:AK6)</f>
-        <v>13329.4</v>
+        <f>AVERAGE(AB6:AK6)</f>
+        <v>7890.3</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
@@ -5753,41 +5764,41 @@
         <v>34617.199999999997</v>
       </c>
       <c r="AA7">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="AB7">
-        <v>21898</v>
+        <v>9900</v>
       </c>
       <c r="AC7">
-        <v>20672</v>
+        <v>15166</v>
       </c>
       <c r="AD7">
-        <v>18510</v>
+        <v>10875</v>
       </c>
       <c r="AE7">
-        <v>23923</v>
+        <v>16649</v>
       </c>
       <c r="AF7">
-        <v>15719</v>
+        <v>10076</v>
       </c>
       <c r="AG7">
-        <v>24446</v>
+        <v>15624</v>
       </c>
       <c r="AH7">
-        <v>23007</v>
+        <v>14171</v>
       </c>
       <c r="AI7">
-        <v>26170</v>
+        <v>14908</v>
       </c>
       <c r="AJ7">
-        <v>16134</v>
+        <v>9706</v>
       </c>
       <c r="AK7">
-        <v>23359</v>
+        <v>16219</v>
       </c>
       <c r="AL7" s="2">
-        <f t="shared" si="2"/>
-        <v>21383.8</v>
+        <f t="shared" ref="AL7:AL55" si="2">AVERAGE(AB7:AK7)</f>
+        <v>13329.4</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
@@ -5866,41 +5877,41 @@
         <v>45978.2</v>
       </c>
       <c r="AA8">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="AB8">
-        <v>19531</v>
+        <v>21898</v>
       </c>
       <c r="AC8">
-        <v>29304</v>
+        <v>20672</v>
       </c>
       <c r="AD8">
-        <v>25929</v>
+        <v>18510</v>
       </c>
       <c r="AE8">
-        <v>28915</v>
+        <v>23923</v>
       </c>
       <c r="AF8">
-        <v>22405</v>
+        <v>15719</v>
       </c>
       <c r="AG8">
-        <v>28440</v>
+        <v>24446</v>
       </c>
       <c r="AH8">
-        <v>25174</v>
+        <v>23007</v>
       </c>
       <c r="AI8">
-        <v>36596</v>
+        <v>26170</v>
       </c>
       <c r="AJ8">
-        <v>17772</v>
+        <v>16134</v>
       </c>
       <c r="AK8">
-        <v>31040</v>
+        <v>23359</v>
       </c>
       <c r="AL8" s="2">
         <f t="shared" si="2"/>
-        <v>26510.6</v>
+        <v>21383.8</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
@@ -5979,41 +5990,41 @@
         <v>60163.9</v>
       </c>
       <c r="AA9">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="AB9">
-        <v>26665</v>
+        <v>19531</v>
       </c>
       <c r="AC9">
-        <v>22986</v>
+        <v>29304</v>
       </c>
       <c r="AD9">
-        <v>27188</v>
+        <v>25929</v>
       </c>
       <c r="AE9">
-        <v>27849</v>
+        <v>28915</v>
       </c>
       <c r="AF9">
-        <v>22924</v>
+        <v>22405</v>
       </c>
       <c r="AG9">
-        <v>35323</v>
+        <v>28440</v>
       </c>
       <c r="AH9">
-        <v>40109</v>
+        <v>25174</v>
       </c>
       <c r="AI9">
-        <v>52200</v>
+        <v>36596</v>
       </c>
       <c r="AJ9">
-        <v>26992</v>
+        <v>17772</v>
       </c>
       <c r="AK9">
-        <v>26214</v>
+        <v>31040</v>
       </c>
       <c r="AL9" s="2">
         <f t="shared" si="2"/>
-        <v>30845</v>
+        <v>26510.6</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
@@ -6092,41 +6103,41 @@
         <v>68725.2</v>
       </c>
       <c r="AA10">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="AB10">
-        <v>31130</v>
+        <v>26665</v>
       </c>
       <c r="AC10">
-        <v>28311</v>
+        <v>22986</v>
       </c>
       <c r="AD10">
-        <v>33851</v>
+        <v>27188</v>
       </c>
       <c r="AE10">
-        <v>28238</v>
+        <v>27849</v>
       </c>
       <c r="AF10">
-        <v>33391</v>
+        <v>22924</v>
       </c>
       <c r="AG10">
-        <v>38271</v>
+        <v>35323</v>
       </c>
       <c r="AH10">
-        <v>113931</v>
+        <v>40109</v>
       </c>
       <c r="AI10">
-        <v>63166</v>
+        <v>52200</v>
       </c>
       <c r="AJ10">
-        <v>26885</v>
+        <v>26992</v>
       </c>
       <c r="AK10">
-        <v>41717</v>
+        <v>26214</v>
       </c>
       <c r="AL10" s="2">
         <f t="shared" si="2"/>
-        <v>43889.1</v>
+        <v>30845</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
@@ -6205,41 +6216,41 @@
         <v>77262.100000000006</v>
       </c>
       <c r="AA11">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="AB11">
-        <v>43094</v>
+        <v>31130</v>
       </c>
       <c r="AC11">
-        <v>32813</v>
+        <v>28311</v>
       </c>
       <c r="AD11">
-        <v>36626</v>
+        <v>33851</v>
       </c>
       <c r="AE11">
-        <v>30258</v>
+        <v>28238</v>
       </c>
       <c r="AF11">
-        <v>33319</v>
+        <v>33391</v>
       </c>
       <c r="AG11">
-        <v>49752</v>
+        <v>38271</v>
       </c>
       <c r="AH11">
-        <v>96988</v>
+        <v>113931</v>
       </c>
       <c r="AI11">
-        <v>35262</v>
+        <v>63166</v>
       </c>
       <c r="AJ11">
-        <v>37122</v>
+        <v>26885</v>
       </c>
       <c r="AK11">
-        <v>49152</v>
+        <v>41717</v>
       </c>
       <c r="AL11" s="2">
         <f t="shared" si="2"/>
-        <v>44438.6</v>
+        <v>43889.1</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
@@ -6318,41 +6329,41 @@
         <v>88005.9</v>
       </c>
       <c r="AA12">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="AB12">
-        <v>47019</v>
+        <v>43094</v>
       </c>
       <c r="AC12">
-        <v>33755</v>
+        <v>32813</v>
       </c>
       <c r="AD12">
-        <v>58520</v>
+        <v>36626</v>
       </c>
       <c r="AE12">
-        <v>47121</v>
+        <v>30258</v>
       </c>
       <c r="AF12">
-        <v>36514</v>
+        <v>33319</v>
       </c>
       <c r="AG12">
-        <v>30962</v>
+        <v>49752</v>
       </c>
       <c r="AH12">
-        <v>83909</v>
+        <v>96988</v>
       </c>
       <c r="AI12">
-        <v>46854</v>
+        <v>35262</v>
       </c>
       <c r="AJ12">
-        <v>34543</v>
+        <v>37122</v>
       </c>
       <c r="AK12">
-        <v>41266</v>
+        <v>49152</v>
       </c>
       <c r="AL12" s="2">
         <f t="shared" si="2"/>
-        <v>46046.3</v>
+        <v>44438.6</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
@@ -6431,41 +6442,41 @@
         <v>100338.9</v>
       </c>
       <c r="AA13">
-        <v>90</v>
-      </c>
-      <c r="AB13" s="8">
-        <v>50025</v>
+        <v>80</v>
+      </c>
+      <c r="AB13">
+        <v>47019</v>
       </c>
       <c r="AC13">
-        <v>40161</v>
+        <v>33755</v>
       </c>
       <c r="AD13">
-        <v>64360</v>
+        <v>58520</v>
       </c>
       <c r="AE13">
-        <v>62878</v>
+        <v>47121</v>
       </c>
       <c r="AF13">
-        <v>46669</v>
+        <v>36514</v>
       </c>
       <c r="AG13">
-        <v>45248</v>
+        <v>30962</v>
       </c>
       <c r="AH13">
-        <v>97707</v>
+        <v>83909</v>
       </c>
       <c r="AI13">
-        <v>92935</v>
+        <v>46854</v>
       </c>
       <c r="AJ13">
-        <v>44941</v>
+        <v>34543</v>
       </c>
       <c r="AK13">
-        <v>39288</v>
+        <v>41266</v>
       </c>
       <c r="AL13" s="2">
         <f t="shared" si="2"/>
-        <v>58421.2</v>
+        <v>46046.3</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
@@ -6544,41 +6555,41 @@
         <v>111228.2</v>
       </c>
       <c r="AA14">
-        <v>100</v>
-      </c>
-      <c r="AB14">
-        <v>45724</v>
+        <v>90</v>
+      </c>
+      <c r="AB14" s="16">
+        <v>50025</v>
       </c>
       <c r="AC14">
-        <v>45927</v>
+        <v>40161</v>
       </c>
       <c r="AD14">
-        <v>69892</v>
+        <v>64360</v>
       </c>
       <c r="AE14">
-        <v>53549</v>
+        <v>62878</v>
       </c>
       <c r="AF14">
-        <v>56731</v>
+        <v>46669</v>
       </c>
       <c r="AG14">
-        <v>45140</v>
+        <v>45248</v>
       </c>
       <c r="AH14">
-        <v>84311</v>
+        <v>97707</v>
       </c>
       <c r="AI14">
-        <v>64343</v>
+        <v>92935</v>
       </c>
       <c r="AJ14">
-        <v>41693</v>
+        <v>44941</v>
       </c>
       <c r="AK14">
-        <v>46874</v>
+        <v>39288</v>
       </c>
       <c r="AL14" s="2">
         <f t="shared" si="2"/>
-        <v>55418.400000000001</v>
+        <v>58421.2</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
@@ -6657,41 +6668,41 @@
         <v>120728.2</v>
       </c>
       <c r="AA15">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="AB15">
-        <v>49067</v>
+        <v>45724</v>
       </c>
       <c r="AC15">
-        <v>47279</v>
+        <v>45927</v>
       </c>
       <c r="AD15">
-        <v>79988</v>
+        <v>69892</v>
       </c>
       <c r="AE15">
-        <v>47812</v>
+        <v>53549</v>
       </c>
       <c r="AF15">
-        <v>73170</v>
+        <v>56731</v>
       </c>
       <c r="AG15">
-        <v>50537</v>
+        <v>45140</v>
       </c>
       <c r="AH15">
-        <v>49653</v>
+        <v>84311</v>
       </c>
       <c r="AI15">
-        <v>43934</v>
+        <v>64343</v>
       </c>
       <c r="AJ15">
-        <v>50248</v>
+        <v>41693</v>
       </c>
       <c r="AK15">
-        <v>51662</v>
+        <v>46874</v>
       </c>
       <c r="AL15" s="2">
         <f t="shared" si="2"/>
-        <v>54335</v>
+        <v>55418.400000000001</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
@@ -6770,41 +6781,41 @@
         <v>130410.9</v>
       </c>
       <c r="AA16">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="AB16">
-        <v>54680</v>
+        <v>49067</v>
       </c>
       <c r="AC16">
-        <v>64660</v>
+        <v>47279</v>
       </c>
       <c r="AD16">
-        <v>49394</v>
+        <v>79988</v>
       </c>
       <c r="AE16">
-        <v>52709</v>
+        <v>47812</v>
       </c>
       <c r="AF16">
-        <v>61494</v>
+        <v>73170</v>
       </c>
       <c r="AG16">
-        <v>56192</v>
+        <v>50537</v>
       </c>
       <c r="AH16">
-        <v>55143</v>
+        <v>49653</v>
       </c>
       <c r="AI16">
-        <v>46057</v>
+        <v>43934</v>
       </c>
       <c r="AJ16">
-        <v>56996</v>
+        <v>50248</v>
       </c>
       <c r="AK16">
-        <v>55146</v>
+        <v>51662</v>
       </c>
       <c r="AL16" s="2">
         <f t="shared" si="2"/>
-        <v>55247.1</v>
+        <v>54335</v>
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
@@ -6883,41 +6894,41 @@
         <v>145101.79999999999</v>
       </c>
       <c r="AA17">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="AB17">
-        <v>55590</v>
+        <v>54680</v>
       </c>
       <c r="AC17">
-        <v>86383</v>
+        <v>64660</v>
       </c>
       <c r="AD17">
-        <v>59611</v>
+        <v>49394</v>
       </c>
       <c r="AE17">
-        <v>54811</v>
+        <v>52709</v>
       </c>
       <c r="AF17">
-        <v>72549</v>
+        <v>61494</v>
       </c>
       <c r="AG17">
-        <v>93178</v>
+        <v>56192</v>
       </c>
       <c r="AH17">
-        <v>59783</v>
+        <v>55143</v>
       </c>
       <c r="AI17">
-        <v>50338</v>
+        <v>46057</v>
       </c>
       <c r="AJ17">
-        <v>54441</v>
+        <v>56996</v>
       </c>
       <c r="AK17">
-        <v>82462</v>
+        <v>55146</v>
       </c>
       <c r="AL17" s="2">
         <f t="shared" si="2"/>
-        <v>66914.600000000006</v>
+        <v>55247.1</v>
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.25">
@@ -6996,41 +7007,41 @@
         <v>152974.1</v>
       </c>
       <c r="AA18">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="AB18">
-        <v>61859</v>
+        <v>55590</v>
       </c>
       <c r="AC18">
-        <v>63188</v>
+        <v>86383</v>
       </c>
       <c r="AD18">
-        <v>52012</v>
+        <v>59611</v>
       </c>
       <c r="AE18">
-        <v>90862</v>
+        <v>54811</v>
       </c>
       <c r="AF18">
-        <v>83828</v>
+        <v>72549</v>
       </c>
       <c r="AG18">
-        <v>64776</v>
+        <v>93178</v>
       </c>
       <c r="AH18">
-        <v>63792</v>
+        <v>59783</v>
       </c>
       <c r="AI18">
-        <v>63498</v>
+        <v>50338</v>
       </c>
       <c r="AJ18">
-        <v>58488</v>
+        <v>54441</v>
       </c>
       <c r="AK18">
-        <v>100047</v>
+        <v>82462</v>
       </c>
       <c r="AL18" s="2">
         <f t="shared" si="2"/>
-        <v>70235</v>
+        <v>66914.600000000006</v>
       </c>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.25">
@@ -7109,41 +7120,41 @@
         <v>164592.4</v>
       </c>
       <c r="AA19">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="AB19">
-        <v>63871</v>
+        <v>61859</v>
       </c>
       <c r="AC19">
-        <v>68312</v>
+        <v>63188</v>
       </c>
       <c r="AD19">
-        <v>66268</v>
+        <v>52012</v>
       </c>
       <c r="AE19">
-        <v>79118</v>
+        <v>90862</v>
       </c>
       <c r="AF19">
-        <v>66013</v>
+        <v>83828</v>
       </c>
       <c r="AG19">
-        <v>69156</v>
+        <v>64776</v>
       </c>
       <c r="AH19">
-        <v>65738</v>
+        <v>63792</v>
       </c>
       <c r="AI19">
-        <v>100392</v>
+        <v>63498</v>
       </c>
       <c r="AJ19">
-        <v>61768</v>
+        <v>58488</v>
       </c>
       <c r="AK19">
-        <v>78865</v>
+        <v>100047</v>
       </c>
       <c r="AL19" s="2">
         <f t="shared" si="2"/>
-        <v>71950.100000000006</v>
+        <v>70235</v>
       </c>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.25">
@@ -7222,41 +7233,41 @@
         <v>177763.1</v>
       </c>
       <c r="AA20">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="AB20">
-        <v>67533</v>
+        <v>63871</v>
       </c>
       <c r="AC20">
-        <v>71251</v>
+        <v>68312</v>
       </c>
       <c r="AD20">
-        <v>61600</v>
+        <v>66268</v>
       </c>
       <c r="AE20">
-        <v>71002</v>
+        <v>79118</v>
       </c>
       <c r="AF20">
-        <v>65471</v>
+        <v>66013</v>
       </c>
       <c r="AG20">
-        <v>106288</v>
+        <v>69156</v>
       </c>
       <c r="AH20">
-        <v>73914</v>
+        <v>65738</v>
       </c>
       <c r="AI20">
-        <v>63207</v>
+        <v>100392</v>
       </c>
       <c r="AJ20">
-        <v>68733</v>
+        <v>61768</v>
       </c>
       <c r="AK20">
-        <v>80364</v>
+        <v>78865</v>
       </c>
       <c r="AL20" s="2">
         <f t="shared" si="2"/>
-        <v>72936.3</v>
+        <v>71950.100000000006</v>
       </c>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.25">
@@ -7335,41 +7346,41 @@
         <v>188108.3</v>
       </c>
       <c r="AA21">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="AB21">
-        <v>69111</v>
+        <v>67533</v>
       </c>
       <c r="AC21">
-        <v>69720</v>
+        <v>71251</v>
       </c>
       <c r="AD21">
-        <v>68631</v>
+        <v>61600</v>
       </c>
       <c r="AE21">
-        <v>70685</v>
+        <v>71002</v>
       </c>
       <c r="AF21">
-        <v>67891</v>
+        <v>65471</v>
       </c>
       <c r="AG21">
-        <v>123662</v>
+        <v>106288</v>
       </c>
       <c r="AH21">
-        <v>73339</v>
+        <v>73914</v>
       </c>
       <c r="AI21">
-        <v>69953</v>
+        <v>63207</v>
       </c>
       <c r="AJ21">
-        <v>76518</v>
+        <v>68733</v>
       </c>
       <c r="AK21">
-        <v>83767</v>
+        <v>80364</v>
       </c>
       <c r="AL21" s="2">
         <f t="shared" si="2"/>
-        <v>77327.7</v>
+        <v>72936.3</v>
       </c>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.25">
@@ -7448,41 +7459,41 @@
         <v>211566.3</v>
       </c>
       <c r="AA22">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="AB22">
-        <v>72903</v>
+        <v>69111</v>
       </c>
       <c r="AC22">
-        <v>81153</v>
+        <v>69720</v>
       </c>
       <c r="AD22">
-        <v>70649</v>
+        <v>68631</v>
       </c>
       <c r="AE22">
-        <v>80018</v>
+        <v>70685</v>
       </c>
       <c r="AF22">
-        <v>68931</v>
+        <v>67891</v>
       </c>
       <c r="AG22">
-        <v>129034</v>
+        <v>123662</v>
       </c>
       <c r="AH22">
-        <v>76956</v>
+        <v>73339</v>
       </c>
       <c r="AI22">
-        <v>72072</v>
+        <v>69953</v>
       </c>
       <c r="AJ22">
-        <v>77732</v>
+        <v>76518</v>
       </c>
       <c r="AK22">
-        <v>83988</v>
+        <v>83767</v>
       </c>
       <c r="AL22" s="2">
         <f t="shared" si="2"/>
-        <v>81343.600000000006</v>
+        <v>77327.7</v>
       </c>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.25">
@@ -7561,41 +7572,41 @@
         <v>236384.1</v>
       </c>
       <c r="AA23">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="AB23">
-        <v>79605</v>
+        <v>72903</v>
       </c>
       <c r="AC23">
-        <v>80014</v>
+        <v>69153</v>
       </c>
       <c r="AD23">
-        <v>70315</v>
+        <v>70649</v>
       </c>
       <c r="AE23">
-        <v>82724</v>
+        <v>74018</v>
       </c>
       <c r="AF23">
-        <v>69821</v>
+        <v>68931</v>
       </c>
       <c r="AG23">
-        <v>88186</v>
+        <v>79034</v>
       </c>
       <c r="AH23">
-        <v>84956</v>
+        <v>76956</v>
       </c>
       <c r="AI23">
-        <v>78462</v>
+        <v>72072</v>
       </c>
       <c r="AJ23">
-        <v>83598</v>
+        <v>67732</v>
       </c>
       <c r="AK23">
-        <v>127453</v>
+        <v>73988</v>
       </c>
       <c r="AL23" s="2">
         <f t="shared" si="2"/>
-        <v>84513.4</v>
+        <v>72543.600000000006</v>
       </c>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.25">
@@ -7674,41 +7685,41 @@
         <v>287079.09999999998</v>
       </c>
       <c r="AA24">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="AB24">
-        <v>83825</v>
+        <v>72605</v>
       </c>
       <c r="AC24">
-        <v>97699</v>
+        <v>70014</v>
       </c>
       <c r="AD24">
-        <v>91474</v>
+        <v>70315</v>
       </c>
       <c r="AE24">
-        <v>86291</v>
+        <v>72724</v>
       </c>
       <c r="AF24">
-        <v>81243</v>
+        <v>69821</v>
       </c>
       <c r="AG24">
-        <v>86802</v>
+        <v>80186</v>
       </c>
       <c r="AH24">
-        <v>85374</v>
+        <v>84956</v>
       </c>
       <c r="AI24">
-        <v>80129</v>
+        <v>78462</v>
       </c>
       <c r="AJ24">
-        <v>83025</v>
+        <v>83598</v>
       </c>
       <c r="AK24">
-        <v>87847</v>
+        <v>77453</v>
       </c>
       <c r="AL24" s="2">
         <f t="shared" si="2"/>
-        <v>86370.9</v>
+        <v>76013.399999999994</v>
       </c>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.25">
@@ -7787,41 +7798,41 @@
         <v>337697.1</v>
       </c>
       <c r="AA25">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="AB25">
-        <v>58843</v>
+        <v>80825</v>
       </c>
       <c r="AC25">
-        <v>58842</v>
+        <v>77699</v>
       </c>
       <c r="AD25">
-        <v>58812</v>
+        <v>81474</v>
       </c>
       <c r="AE25">
-        <v>56850</v>
+        <v>86291</v>
       </c>
       <c r="AF25">
-        <v>55851</v>
+        <v>81243</v>
       </c>
       <c r="AG25">
-        <v>54853</v>
+        <v>76802</v>
       </c>
       <c r="AH25">
-        <v>55851</v>
+        <v>80374</v>
       </c>
       <c r="AI25">
-        <v>54853</v>
+        <v>80129</v>
       </c>
       <c r="AJ25">
-        <v>57854</v>
+        <v>80025</v>
       </c>
       <c r="AK25">
-        <v>56848</v>
+        <v>78847</v>
       </c>
       <c r="AL25" s="2">
         <f t="shared" si="2"/>
-        <v>56945.7</v>
+        <v>80370.899999999994</v>
       </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.25">
@@ -7900,41 +7911,41 @@
         <v>331715.90000000002</v>
       </c>
       <c r="AA26">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="AB26">
-        <v>59851</v>
+        <v>58843</v>
       </c>
       <c r="AC26">
-        <v>61838</v>
+        <v>68842</v>
       </c>
       <c r="AD26">
-        <v>59864</v>
+        <v>58812</v>
       </c>
       <c r="AE26">
-        <v>59833</v>
+        <v>66850</v>
       </c>
       <c r="AF26">
-        <v>59840</v>
+        <v>55851</v>
       </c>
       <c r="AG26">
-        <v>58843</v>
+        <v>74853</v>
       </c>
       <c r="AH26">
-        <v>57845</v>
+        <v>69851</v>
       </c>
       <c r="AI26">
-        <v>57846</v>
+        <v>64853</v>
       </c>
       <c r="AJ26">
-        <v>59827</v>
-      </c>
-      <c r="AK26" s="8">
-        <v>60838</v>
+        <v>67854</v>
+      </c>
+      <c r="AK26">
+        <v>66848</v>
       </c>
       <c r="AL26" s="2">
         <f t="shared" si="2"/>
-        <v>59642.5</v>
+        <v>65345.7</v>
       </c>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.25">
@@ -8013,41 +8024,41 @@
         <v>349665</v>
       </c>
       <c r="AA27">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="AB27">
-        <v>61824</v>
+        <v>59851</v>
       </c>
       <c r="AC27">
-        <v>64819</v>
+        <v>61838</v>
       </c>
       <c r="AD27">
-        <v>61834</v>
+        <v>59864</v>
       </c>
       <c r="AE27">
-        <v>61839</v>
+        <v>59833</v>
       </c>
       <c r="AF27">
-        <v>61841</v>
+        <v>59840</v>
       </c>
       <c r="AG27">
-        <v>59840</v>
+        <v>58843</v>
       </c>
       <c r="AH27">
-        <v>60837</v>
+        <v>57845</v>
       </c>
       <c r="AI27">
-        <v>60837</v>
+        <v>57846</v>
       </c>
       <c r="AJ27">
-        <v>61834</v>
+        <v>59827</v>
       </c>
       <c r="AK27">
-        <v>63853</v>
+        <v>67854</v>
       </c>
       <c r="AL27" s="2">
         <f t="shared" si="2"/>
-        <v>61935.8</v>
+        <v>60344.1</v>
       </c>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.25">
@@ -8126,41 +8137,41 @@
         <v>362734.4</v>
       </c>
       <c r="AA28">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="AB28">
-        <v>67819</v>
+        <v>61824</v>
       </c>
       <c r="AC28">
-        <v>65832</v>
+        <v>64819</v>
       </c>
       <c r="AD28">
-        <v>64829</v>
+        <v>61834</v>
       </c>
       <c r="AE28">
-        <v>65820</v>
+        <v>61839</v>
       </c>
       <c r="AF28">
-        <v>64827</v>
+        <v>61841</v>
       </c>
       <c r="AG28">
-        <v>62832</v>
+        <v>59840</v>
       </c>
       <c r="AH28">
-        <v>62832</v>
+        <v>60837</v>
       </c>
       <c r="AI28">
-        <v>63829</v>
+        <v>60837</v>
       </c>
       <c r="AJ28">
-        <v>63830</v>
+        <v>61834</v>
       </c>
       <c r="AK28">
-        <v>65802</v>
+        <v>63853</v>
       </c>
       <c r="AL28" s="2">
         <f t="shared" si="2"/>
-        <v>64825.2</v>
+        <v>61935.8</v>
       </c>
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.25">
@@ -8203,41 +8214,41 @@
         <v>384875</v>
       </c>
       <c r="AA29">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="AB29">
-        <v>68815</v>
+        <v>67819</v>
       </c>
       <c r="AC29">
-        <v>69779</v>
+        <v>65832</v>
       </c>
       <c r="AD29">
-        <v>67818</v>
+        <v>64829</v>
       </c>
       <c r="AE29">
-        <v>67821</v>
+        <v>65820</v>
       </c>
       <c r="AF29">
-        <v>68816</v>
+        <v>64827</v>
       </c>
       <c r="AG29">
-        <v>66821</v>
+        <v>62832</v>
       </c>
       <c r="AH29">
-        <v>66822</v>
+        <v>62832</v>
       </c>
       <c r="AI29">
-        <v>69814</v>
+        <v>63829</v>
       </c>
       <c r="AJ29">
-        <v>67818</v>
+        <v>63830</v>
       </c>
       <c r="AK29">
-        <v>66821</v>
+        <v>65802</v>
       </c>
       <c r="AL29" s="2">
         <f t="shared" si="2"/>
-        <v>68114.5</v>
+        <v>64825.2</v>
       </c>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.25">
@@ -8280,41 +8291,41 @@
         <v>388761.7</v>
       </c>
       <c r="AA30">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="AB30">
-        <v>70811</v>
+        <v>68815</v>
       </c>
       <c r="AC30">
-        <v>72830</v>
+        <v>69779</v>
       </c>
       <c r="AD30">
-        <v>70810</v>
+        <v>67818</v>
       </c>
       <c r="AE30">
-        <v>69812</v>
+        <v>67821</v>
       </c>
       <c r="AF30">
-        <v>69781</v>
+        <v>68816</v>
       </c>
       <c r="AG30">
-        <v>67819</v>
+        <v>66821</v>
       </c>
       <c r="AH30">
+        <v>66822</v>
+      </c>
+      <c r="AI30">
+        <v>69814</v>
+      </c>
+      <c r="AJ30">
         <v>67818</v>
       </c>
-      <c r="AI30">
-        <v>69813</v>
-      </c>
-      <c r="AJ30">
-        <v>69814</v>
-      </c>
       <c r="AK30">
-        <v>68816</v>
+        <v>66821</v>
       </c>
       <c r="AL30" s="2">
         <f t="shared" si="2"/>
-        <v>69812.399999999994</v>
+        <v>68114.5</v>
       </c>
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.25">
@@ -8357,41 +8368,41 @@
         <v>483802.6</v>
       </c>
       <c r="AA31">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="AB31">
         <v>70811</v>
       </c>
       <c r="AC31">
-        <v>75772</v>
+        <v>72830</v>
       </c>
       <c r="AD31">
-        <v>72805</v>
+        <v>70810</v>
       </c>
       <c r="AE31">
-        <v>73803</v>
+        <v>69812</v>
       </c>
       <c r="AF31">
-        <v>71839</v>
+        <v>69781</v>
       </c>
       <c r="AG31">
-        <v>71808</v>
+        <v>67819</v>
       </c>
       <c r="AH31">
-        <v>71808</v>
+        <v>67818</v>
       </c>
       <c r="AI31">
-        <v>70811</v>
+        <v>69813</v>
       </c>
       <c r="AJ31">
-        <v>72805</v>
+        <v>69814</v>
       </c>
       <c r="AK31">
-        <v>71809</v>
+        <v>68816</v>
       </c>
       <c r="AL31" s="2">
         <f t="shared" si="2"/>
-        <v>72407.100000000006</v>
+        <v>69812.399999999994</v>
       </c>
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.25">
@@ -8434,41 +8445,41 @@
         <v>472937</v>
       </c>
       <c r="AA32">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="AB32">
-        <v>75797</v>
+        <v>70811</v>
       </c>
       <c r="AC32">
-        <v>166611</v>
+        <v>75772</v>
       </c>
       <c r="AD32">
-        <v>74802</v>
+        <v>72805</v>
       </c>
       <c r="AE32">
-        <v>77785</v>
+        <v>73803</v>
       </c>
       <c r="AF32">
-        <v>74801</v>
+        <v>71839</v>
       </c>
       <c r="AG32">
-        <v>73803</v>
+        <v>71808</v>
       </c>
       <c r="AH32">
-        <v>73803</v>
+        <v>71808</v>
       </c>
       <c r="AI32">
-        <v>73802</v>
+        <v>70811</v>
       </c>
       <c r="AJ32">
-        <v>74800</v>
+        <v>72805</v>
       </c>
       <c r="AK32">
-        <v>74800</v>
+        <v>71809</v>
       </c>
       <c r="AL32" s="2">
         <f t="shared" si="2"/>
-        <v>84080.4</v>
+        <v>72407.100000000006</v>
       </c>
     </row>
     <row r="33" spans="12:38" x14ac:dyDescent="0.25">
@@ -8511,41 +8522,41 @@
         <v>416588.9</v>
       </c>
       <c r="AA33">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="AB33">
-        <v>76795</v>
+        <v>75797</v>
       </c>
       <c r="AC33">
-        <v>180504</v>
+        <v>166611</v>
       </c>
       <c r="AD33">
-        <v>79784</v>
+        <v>74802</v>
       </c>
       <c r="AE33">
-        <v>78789</v>
+        <v>77785</v>
       </c>
       <c r="AF33">
-        <v>78789</v>
+        <v>74801</v>
       </c>
       <c r="AG33">
-        <v>75797</v>
+        <v>73803</v>
       </c>
       <c r="AH33">
-        <v>75797</v>
+        <v>73803</v>
       </c>
       <c r="AI33">
-        <v>76795</v>
+        <v>73802</v>
       </c>
       <c r="AJ33">
-        <v>79786</v>
+        <v>74800</v>
       </c>
       <c r="AK33">
-        <v>77792</v>
+        <v>74800</v>
       </c>
       <c r="AL33" s="2">
         <f t="shared" si="2"/>
-        <v>88062.8</v>
+        <v>84080.4</v>
       </c>
     </row>
     <row r="34" spans="12:38" x14ac:dyDescent="0.25">
@@ -8588,41 +8599,41 @@
         <v>507859.7</v>
       </c>
       <c r="AA34">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="AB34">
+        <v>76795</v>
+      </c>
+      <c r="AC34">
+        <v>180504</v>
+      </c>
+      <c r="AD34">
+        <v>79784</v>
+      </c>
+      <c r="AE34">
+        <v>78789</v>
+      </c>
+      <c r="AF34">
+        <v>78789</v>
+      </c>
+      <c r="AG34">
+        <v>75797</v>
+      </c>
+      <c r="AH34">
+        <v>75797</v>
+      </c>
+      <c r="AI34">
+        <v>76795</v>
+      </c>
+      <c r="AJ34">
         <v>79786</v>
       </c>
-      <c r="AC34">
-        <v>186506</v>
-      </c>
-      <c r="AD34">
-        <v>80787</v>
-      </c>
-      <c r="AE34">
-        <v>80786</v>
-      </c>
-      <c r="AF34">
-        <v>81781</v>
-      </c>
-      <c r="AG34">
-        <v>79787</v>
-      </c>
-      <c r="AH34">
+      <c r="AK34">
         <v>77792</v>
-      </c>
-      <c r="AI34">
-        <v>79787</v>
-      </c>
-      <c r="AJ34">
-        <v>81782</v>
-      </c>
-      <c r="AK34">
-        <v>81781</v>
       </c>
       <c r="AL34" s="2">
         <f t="shared" si="2"/>
-        <v>91057.5</v>
+        <v>88062.8</v>
       </c>
     </row>
     <row r="35" spans="12:38" x14ac:dyDescent="0.25">
@@ -8631,41 +8642,41 @@
       <c r="P35" s="6"/>
       <c r="Y35" s="2"/>
       <c r="AA35">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="AB35">
-        <v>82779</v>
+        <v>79786</v>
       </c>
       <c r="AC35">
-        <v>193481</v>
+        <v>186506</v>
       </c>
       <c r="AD35">
-        <v>83774</v>
+        <v>80787</v>
       </c>
       <c r="AE35">
-        <v>84771</v>
+        <v>80786</v>
       </c>
       <c r="AF35">
-        <v>83776</v>
+        <v>81781</v>
       </c>
       <c r="AG35">
+        <v>79787</v>
+      </c>
+      <c r="AH35">
+        <v>77792</v>
+      </c>
+      <c r="AI35">
+        <v>79787</v>
+      </c>
+      <c r="AJ35">
+        <v>81782</v>
+      </c>
+      <c r="AK35">
         <v>81781</v>
-      </c>
-      <c r="AH35">
-        <v>82779</v>
-      </c>
-      <c r="AI35">
-        <v>82778</v>
-      </c>
-      <c r="AJ35">
-        <v>83776</v>
-      </c>
-      <c r="AK35">
-        <v>83775</v>
       </c>
       <c r="AL35" s="2">
         <f t="shared" si="2"/>
-        <v>94347</v>
+        <v>91057.5</v>
       </c>
     </row>
     <row r="36" spans="12:38" x14ac:dyDescent="0.25">
@@ -8674,41 +8685,41 @@
       <c r="P36" s="6"/>
       <c r="Y36" s="2"/>
       <c r="AA36">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="AB36">
-        <v>84775</v>
+        <v>82779</v>
       </c>
       <c r="AC36">
-        <v>199422</v>
+        <v>193481</v>
       </c>
       <c r="AD36">
-        <v>86768</v>
+        <v>83774</v>
       </c>
       <c r="AE36">
-        <v>86769</v>
+        <v>84771</v>
       </c>
       <c r="AF36">
-        <v>87766</v>
+        <v>83776</v>
       </c>
       <c r="AG36">
-        <v>85771</v>
+        <v>81781</v>
       </c>
       <c r="AH36">
-        <v>84773</v>
+        <v>82779</v>
       </c>
       <c r="AI36">
+        <v>82778</v>
+      </c>
+      <c r="AJ36">
         <v>83776</v>
       </c>
-      <c r="AJ36">
-        <v>86768</v>
-      </c>
       <c r="AK36">
-        <v>87766</v>
+        <v>83775</v>
       </c>
       <c r="AL36" s="2">
         <f t="shared" si="2"/>
-        <v>97435.4</v>
+        <v>94347</v>
       </c>
     </row>
     <row r="37" spans="12:38" x14ac:dyDescent="0.25">
@@ -8717,41 +8728,41 @@
       <c r="P37" s="6"/>
       <c r="Y37" s="2"/>
       <c r="AA37">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="AB37">
-        <v>89758</v>
+        <v>84775</v>
       </c>
       <c r="AC37">
-        <v>205452</v>
+        <v>199422</v>
       </c>
       <c r="AD37">
-        <v>88763</v>
+        <v>86768</v>
       </c>
       <c r="AE37">
-        <v>89765</v>
+        <v>86769</v>
       </c>
       <c r="AF37">
-        <v>88756</v>
+        <v>87766</v>
       </c>
       <c r="AG37">
-        <v>89760</v>
+        <v>85771</v>
       </c>
       <c r="AH37">
+        <v>84773</v>
+      </c>
+      <c r="AI37">
+        <v>83776</v>
+      </c>
+      <c r="AJ37">
         <v>86768</v>
       </c>
-      <c r="AI37">
-        <v>88763</v>
-      </c>
-      <c r="AJ37">
-        <v>90757</v>
-      </c>
       <c r="AK37">
-        <v>87765</v>
+        <v>87766</v>
       </c>
       <c r="AL37" s="2">
         <f t="shared" si="2"/>
-        <v>100630.7</v>
+        <v>97435.4</v>
       </c>
     </row>
     <row r="38" spans="12:38" x14ac:dyDescent="0.25">
@@ -8760,41 +8771,41 @@
       <c r="P38" s="6"/>
       <c r="Y38" s="2"/>
       <c r="AA38">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="AB38">
+        <v>89758</v>
+      </c>
+      <c r="AC38">
+        <v>205452</v>
+      </c>
+      <c r="AD38">
         <v>88763</v>
       </c>
-      <c r="AC38">
-        <v>211475</v>
-      </c>
-      <c r="AD38">
-        <v>91754</v>
-      </c>
       <c r="AE38">
-        <v>93750</v>
+        <v>89765</v>
       </c>
       <c r="AF38">
-        <v>89766</v>
+        <v>88756</v>
       </c>
       <c r="AG38">
-        <v>93749</v>
+        <v>89760</v>
       </c>
       <c r="AH38">
-        <v>91755</v>
+        <v>86768</v>
       </c>
       <c r="AI38">
-        <v>89760</v>
+        <v>88763</v>
       </c>
       <c r="AJ38">
-        <v>93749</v>
+        <v>90757</v>
       </c>
       <c r="AK38">
-        <v>93750</v>
+        <v>87765</v>
       </c>
       <c r="AL38" s="2">
         <f t="shared" si="2"/>
-        <v>103827.1</v>
+        <v>100630.7</v>
       </c>
     </row>
     <row r="39" spans="12:38" x14ac:dyDescent="0.25">
@@ -8803,41 +8814,41 @@
       <c r="P39" s="6"/>
       <c r="Y39" s="2"/>
       <c r="AA39">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="AB39">
-        <v>94747</v>
+        <v>88763</v>
       </c>
       <c r="AC39">
-        <v>218415</v>
+        <v>211475</v>
       </c>
       <c r="AD39">
-        <v>94747</v>
+        <v>91754</v>
       </c>
       <c r="AE39">
-        <v>94747</v>
+        <v>93750</v>
       </c>
       <c r="AF39">
-        <v>94747</v>
+        <v>89766</v>
       </c>
       <c r="AG39">
-        <v>94747</v>
+        <v>93749</v>
       </c>
       <c r="AH39">
-        <v>91754</v>
+        <v>91755</v>
       </c>
       <c r="AI39">
-        <v>92752</v>
+        <v>89760</v>
       </c>
       <c r="AJ39">
-        <v>94747</v>
+        <v>93749</v>
       </c>
       <c r="AK39">
-        <v>97738</v>
+        <v>93750</v>
       </c>
       <c r="AL39" s="2">
         <f t="shared" si="2"/>
-        <v>106914.1</v>
+        <v>103827.1</v>
       </c>
     </row>
     <row r="40" spans="12:38" x14ac:dyDescent="0.25">
@@ -8846,41 +8857,41 @@
       <c r="P40" s="6"/>
       <c r="Y40" s="2"/>
       <c r="AA40">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="AB40">
-        <v>94746</v>
+        <v>94747</v>
       </c>
       <c r="AC40">
-        <v>143599</v>
+        <v>218415</v>
       </c>
       <c r="AD40">
-        <v>98735</v>
+        <v>94747</v>
       </c>
       <c r="AE40">
-        <v>97743</v>
+        <v>94747</v>
       </c>
       <c r="AF40">
-        <v>99739</v>
+        <v>94747</v>
       </c>
       <c r="AG40">
-        <v>98736</v>
+        <v>94747</v>
       </c>
       <c r="AH40">
+        <v>91754</v>
+      </c>
+      <c r="AI40">
+        <v>92752</v>
+      </c>
+      <c r="AJ40">
         <v>94747</v>
       </c>
-      <c r="AI40">
-        <v>94747</v>
-      </c>
-      <c r="AJ40">
+      <c r="AK40">
         <v>97738</v>
-      </c>
-      <c r="AK40">
-        <v>98736</v>
       </c>
       <c r="AL40" s="2">
         <f t="shared" si="2"/>
-        <v>101926.6</v>
+        <v>106914.1</v>
       </c>
     </row>
     <row r="41" spans="12:38" x14ac:dyDescent="0.25">
@@ -8889,41 +8900,41 @@
       <c r="P41" s="6"/>
       <c r="Y41" s="2"/>
       <c r="AA41">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="AB41">
-        <v>97739</v>
+        <v>94746</v>
       </c>
       <c r="AC41">
-        <v>100731</v>
+        <v>143599</v>
       </c>
       <c r="AD41">
-        <v>100733</v>
+        <v>98735</v>
       </c>
       <c r="AE41">
-        <v>99733</v>
+        <v>97743</v>
       </c>
       <c r="AF41">
-        <v>100693</v>
+        <v>99739</v>
       </c>
       <c r="AG41">
-        <v>99733</v>
+        <v>98736</v>
       </c>
       <c r="AH41">
-        <v>96741</v>
+        <v>94747</v>
       </c>
       <c r="AI41">
-        <v>100730</v>
+        <v>94747</v>
       </c>
       <c r="AJ41">
-        <v>100731</v>
+        <v>97738</v>
       </c>
       <c r="AK41">
-        <v>101734</v>
+        <v>98736</v>
       </c>
       <c r="AL41" s="2">
         <f t="shared" si="2"/>
-        <v>99929.8</v>
+        <v>101926.6</v>
       </c>
     </row>
     <row r="42" spans="12:38" x14ac:dyDescent="0.25">
@@ -8932,41 +8943,41 @@
       <c r="P42" s="6"/>
       <c r="Y42" s="2"/>
       <c r="AA42">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="AB42">
+        <v>97739</v>
+      </c>
+      <c r="AC42">
         <v>100731</v>
       </c>
-      <c r="AC42">
-        <v>103723</v>
-      </c>
       <c r="AD42">
-        <v>105725</v>
+        <v>100733</v>
       </c>
       <c r="AE42">
-        <v>103722</v>
+        <v>99733</v>
       </c>
       <c r="AF42">
-        <v>102763</v>
+        <v>100693</v>
       </c>
       <c r="AG42">
-        <v>103723</v>
+        <v>99733</v>
       </c>
       <c r="AH42">
+        <v>96741</v>
+      </c>
+      <c r="AI42">
+        <v>100730</v>
+      </c>
+      <c r="AJ42">
         <v>100731</v>
       </c>
-      <c r="AI42">
-        <v>109707</v>
-      </c>
-      <c r="AJ42">
-        <v>102725</v>
-      </c>
       <c r="AK42">
-        <v>104720</v>
+        <v>101734</v>
       </c>
       <c r="AL42" s="2">
         <f t="shared" si="2"/>
-        <v>103827</v>
+        <v>99929.8</v>
       </c>
     </row>
     <row r="43" spans="12:38" x14ac:dyDescent="0.25">
@@ -8975,41 +8986,41 @@
       <c r="P43" s="6"/>
       <c r="Y43" s="2"/>
       <c r="AA43">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="AB43">
-        <v>105717</v>
+        <v>100731</v>
       </c>
       <c r="AC43">
-        <v>105717</v>
+        <v>103723</v>
       </c>
       <c r="AD43">
-        <v>105708</v>
+        <v>105725</v>
       </c>
       <c r="AE43">
-        <v>107707</v>
+        <v>103722</v>
       </c>
       <c r="AF43">
-        <v>105712</v>
+        <v>102763</v>
       </c>
       <c r="AG43">
+        <v>103723</v>
+      </c>
+      <c r="AH43">
+        <v>100731</v>
+      </c>
+      <c r="AI43">
+        <v>109707</v>
+      </c>
+      <c r="AJ43">
+        <v>102725</v>
+      </c>
+      <c r="AK43">
         <v>104720</v>
-      </c>
-      <c r="AH43">
-        <v>106749</v>
-      </c>
-      <c r="AI43">
-        <v>111701</v>
-      </c>
-      <c r="AJ43">
-        <v>106715</v>
-      </c>
-      <c r="AK43">
-        <v>108678</v>
       </c>
       <c r="AL43" s="2">
         <f t="shared" si="2"/>
-        <v>106912.4</v>
+        <v>103827</v>
       </c>
     </row>
     <row r="44" spans="12:38" x14ac:dyDescent="0.25">
@@ -9018,41 +9029,41 @@
       <c r="P44" s="6"/>
       <c r="Y44" s="2"/>
       <c r="AA44">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="AB44">
-        <v>110705</v>
+        <v>105717</v>
       </c>
       <c r="AC44">
-        <v>108715</v>
+        <v>105717</v>
       </c>
       <c r="AD44">
-        <v>109708</v>
+        <v>105708</v>
       </c>
       <c r="AE44">
-        <v>108712</v>
+        <v>107707</v>
       </c>
       <c r="AF44">
-        <v>107711</v>
+        <v>105712</v>
       </c>
       <c r="AG44">
-        <v>108709</v>
+        <v>104720</v>
       </c>
       <c r="AH44">
-        <v>108707</v>
+        <v>106749</v>
       </c>
       <c r="AI44">
-        <v>114694</v>
+        <v>111701</v>
       </c>
       <c r="AJ44">
-        <v>108709</v>
+        <v>106715</v>
       </c>
       <c r="AK44">
-        <v>111733</v>
+        <v>108678</v>
       </c>
       <c r="AL44" s="2">
         <f t="shared" si="2"/>
-        <v>109810.3</v>
+        <v>106912.4</v>
       </c>
     </row>
     <row r="45" spans="12:38" x14ac:dyDescent="0.25">
@@ -9061,41 +9072,41 @@
       <c r="P45" s="6"/>
       <c r="Y45" s="2"/>
       <c r="AA45">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="AB45">
-        <v>111701</v>
+        <v>110705</v>
       </c>
       <c r="AC45">
-        <v>110704</v>
+        <v>108715</v>
       </c>
       <c r="AD45">
-        <v>111700</v>
+        <v>109708</v>
       </c>
       <c r="AE45">
-        <v>111701</v>
+        <v>108712</v>
       </c>
       <c r="AF45">
-        <v>110705</v>
+        <v>107711</v>
       </c>
       <c r="AG45">
-        <v>115727</v>
+        <v>108709</v>
       </c>
       <c r="AH45">
-        <v>110673</v>
+        <v>108707</v>
       </c>
       <c r="AI45">
-        <v>116688</v>
+        <v>114694</v>
       </c>
       <c r="AJ45">
-        <v>110704</v>
+        <v>108709</v>
       </c>
       <c r="AK45">
-        <v>112700</v>
+        <v>111733</v>
       </c>
       <c r="AL45" s="2">
         <f t="shared" si="2"/>
-        <v>112300.3</v>
+        <v>109810.3</v>
       </c>
     </row>
     <row r="46" spans="12:38" x14ac:dyDescent="0.25">
@@ -9104,41 +9115,41 @@
       <c r="P46" s="6"/>
       <c r="Y46" s="2"/>
       <c r="AA46">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="AB46">
-        <v>157622</v>
+        <v>111701</v>
       </c>
       <c r="AC46">
-        <v>113696</v>
+        <v>110704</v>
       </c>
       <c r="AD46">
-        <v>114694</v>
+        <v>111700</v>
       </c>
       <c r="AE46">
-        <v>114692</v>
+        <v>111701</v>
       </c>
       <c r="AF46">
-        <v>114693</v>
+        <v>110705</v>
       </c>
       <c r="AG46">
-        <v>115691</v>
+        <v>115727</v>
       </c>
       <c r="AH46">
-        <v>113727</v>
+        <v>110673</v>
       </c>
       <c r="AI46">
-        <v>118682</v>
+        <v>116688</v>
       </c>
       <c r="AJ46">
-        <v>113696</v>
+        <v>110704</v>
       </c>
       <c r="AK46">
-        <v>115694</v>
+        <v>112700</v>
       </c>
       <c r="AL46" s="2">
         <f t="shared" si="2"/>
-        <v>119288.7</v>
+        <v>112300.3</v>
       </c>
     </row>
     <row r="47" spans="12:38" x14ac:dyDescent="0.25">
@@ -9147,41 +9158,41 @@
       <c r="P47" s="6"/>
       <c r="Y47" s="2"/>
       <c r="AA47">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="AB47">
-        <v>271275</v>
+        <v>157622</v>
       </c>
       <c r="AC47">
-        <v>116688</v>
+        <v>113696</v>
       </c>
       <c r="AD47">
+        <v>114694</v>
+      </c>
+      <c r="AE47">
+        <v>114692</v>
+      </c>
+      <c r="AF47">
+        <v>114693</v>
+      </c>
+      <c r="AG47">
         <v>115691</v>
       </c>
-      <c r="AE47">
-        <v>115690</v>
-      </c>
-      <c r="AF47">
-        <v>117684</v>
-      </c>
-      <c r="AG47">
-        <v>120667</v>
-      </c>
       <c r="AH47">
-        <v>115691</v>
+        <v>113727</v>
       </c>
       <c r="AI47">
-        <v>120072</v>
+        <v>118682</v>
       </c>
       <c r="AJ47">
-        <v>116688</v>
+        <v>113696</v>
       </c>
       <c r="AK47">
-        <v>118672</v>
+        <v>115694</v>
       </c>
       <c r="AL47" s="2">
         <f t="shared" si="2"/>
-        <v>132881.79999999999</v>
+        <v>119288.7</v>
       </c>
     </row>
     <row r="48" spans="12:38" x14ac:dyDescent="0.25">
@@ -9190,41 +9201,41 @@
       <c r="P48" s="6"/>
       <c r="Y48" s="2"/>
       <c r="AA48">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="AB48">
-        <v>279253</v>
+        <v>271275</v>
       </c>
       <c r="AC48">
-        <v>117686</v>
+        <v>116688</v>
       </c>
       <c r="AD48">
-        <v>267292</v>
+        <v>115691</v>
       </c>
       <c r="AE48">
-        <v>121675</v>
+        <v>115690</v>
       </c>
       <c r="AF48">
-        <v>118685</v>
+        <v>117684</v>
       </c>
       <c r="AG48">
-        <v>123669</v>
+        <v>120667</v>
       </c>
       <c r="AH48">
-        <v>118687</v>
+        <v>115691</v>
       </c>
       <c r="AI48">
-        <v>122662</v>
+        <v>120072</v>
       </c>
       <c r="AJ48">
-        <v>119680</v>
+        <v>116688</v>
       </c>
       <c r="AK48">
-        <v>121680</v>
+        <v>118672</v>
       </c>
       <c r="AL48" s="2">
         <f t="shared" si="2"/>
-        <v>151096.9</v>
+        <v>132881.79999999999</v>
       </c>
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.25">
@@ -9233,252 +9244,288 @@
       <c r="P49" s="6"/>
       <c r="Y49" s="2"/>
       <c r="AA49">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="AB49">
-        <v>289189</v>
+        <v>279253</v>
       </c>
       <c r="AC49">
-        <v>122671</v>
+        <v>117686</v>
       </c>
       <c r="AD49">
-        <v>283253</v>
+        <v>267292</v>
       </c>
       <c r="AE49">
         <v>121675</v>
       </c>
       <c r="AF49">
-        <v>121673</v>
+        <v>118685</v>
       </c>
       <c r="AG49">
-        <v>127664</v>
+        <v>123669</v>
       </c>
       <c r="AH49">
-        <v>122673</v>
+        <v>118687</v>
       </c>
       <c r="AI49">
-        <v>123656</v>
+        <v>122662</v>
       </c>
       <c r="AJ49">
-        <v>122672</v>
+        <v>119680</v>
       </c>
       <c r="AK49">
-        <v>123663</v>
+        <v>121680</v>
       </c>
       <c r="AL49" s="2">
         <f t="shared" si="2"/>
-        <v>155878.9</v>
+        <v>151096.9</v>
       </c>
     </row>
     <row r="50" spans="1:39" x14ac:dyDescent="0.25">
       <c r="L50" s="2"/>
       <c r="Y50" s="2"/>
       <c r="AA50">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="AB50">
-        <v>303185</v>
+        <v>289189</v>
       </c>
       <c r="AC50">
-        <v>121643</v>
+        <v>122671</v>
       </c>
       <c r="AD50">
-        <v>289227</v>
+        <v>283253</v>
       </c>
       <c r="AE50">
-        <v>124668</v>
+        <v>121675</v>
       </c>
       <c r="AF50">
-        <v>123669</v>
+        <v>121673</v>
       </c>
       <c r="AG50">
-        <v>125664</v>
+        <v>127664</v>
       </c>
       <c r="AH50">
-        <v>124661</v>
+        <v>122673</v>
       </c>
       <c r="AI50">
-        <v>125650</v>
+        <v>123656</v>
       </c>
       <c r="AJ50">
-        <v>124667</v>
+        <v>122672</v>
       </c>
       <c r="AK50">
-        <v>125665</v>
+        <v>123663</v>
       </c>
       <c r="AL50" s="2">
         <f t="shared" si="2"/>
-        <v>158869.9</v>
+        <v>155878.9</v>
       </c>
     </row>
     <row r="51" spans="1:39" x14ac:dyDescent="0.25">
       <c r="L51" s="2"/>
       <c r="Y51" s="2"/>
       <c r="AA51">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="AB51">
-        <v>293246</v>
+        <v>303185</v>
       </c>
       <c r="AC51">
+        <v>121643</v>
+      </c>
+      <c r="AD51">
+        <v>289227</v>
+      </c>
+      <c r="AE51">
+        <v>124668</v>
+      </c>
+      <c r="AF51">
+        <v>123669</v>
+      </c>
+      <c r="AG51">
+        <v>125664</v>
+      </c>
+      <c r="AH51">
+        <v>124661</v>
+      </c>
+      <c r="AI51">
+        <v>125650</v>
+      </c>
+      <c r="AJ51">
         <v>124667</v>
       </c>
-      <c r="AD51">
-        <v>293216</v>
-      </c>
-      <c r="AE51">
-        <v>128654</v>
-      </c>
-      <c r="AF51">
-        <v>127660</v>
-      </c>
-      <c r="AG51">
-        <v>130652</v>
-      </c>
-      <c r="AH51">
-        <v>128658</v>
-      </c>
-      <c r="AI51">
-        <v>126350</v>
-      </c>
-      <c r="AJ51">
-        <v>127659</v>
-      </c>
       <c r="AK51">
-        <v>129654</v>
+        <v>125665</v>
       </c>
       <c r="AL51" s="2">
         <f t="shared" si="2"/>
-        <v>161041.60000000001</v>
+        <v>158869.9</v>
       </c>
     </row>
     <row r="52" spans="1:39" x14ac:dyDescent="0.25">
       <c r="L52" s="2"/>
       <c r="Y52" s="2"/>
       <c r="AA52">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="AB52">
-        <v>136635</v>
+        <v>293246</v>
       </c>
       <c r="AC52">
-        <v>125664</v>
+        <v>124667</v>
       </c>
       <c r="AD52">
-        <v>301194</v>
+        <v>293216</v>
       </c>
       <c r="AE52">
-        <v>131655</v>
+        <v>128654</v>
       </c>
       <c r="AF52">
-        <v>131641</v>
+        <v>127660</v>
       </c>
       <c r="AG52">
-        <v>132644</v>
+        <v>130652</v>
       </c>
       <c r="AH52">
-        <v>129646</v>
+        <v>128658</v>
       </c>
       <c r="AI52">
-        <v>129642</v>
+        <v>126350</v>
       </c>
       <c r="AJ52">
-        <v>128638</v>
+        <v>127659</v>
       </c>
       <c r="AK52">
-        <v>133652</v>
+        <v>129654</v>
       </c>
       <c r="AL52" s="2">
         <f t="shared" si="2"/>
-        <v>148101.1</v>
+        <v>161041.60000000001</v>
       </c>
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.25">
       <c r="L53" s="2"/>
       <c r="Y53" s="2"/>
       <c r="AA53">
-        <v>490</v>
+        <v>480</v>
       </c>
       <c r="AB53">
-        <v>137715</v>
+        <v>136635</v>
       </c>
       <c r="AC53">
-        <v>128656</v>
+        <v>125664</v>
       </c>
       <c r="AD53">
-        <v>161552</v>
+        <v>301194</v>
       </c>
       <c r="AE53">
-        <v>134633</v>
+        <v>131655</v>
       </c>
       <c r="AF53">
-        <v>131649</v>
+        <v>131641</v>
       </c>
       <c r="AG53">
         <v>132644</v>
       </c>
       <c r="AH53">
-        <v>132644</v>
+        <v>129646</v>
       </c>
       <c r="AI53">
-        <v>131645</v>
+        <v>129642</v>
       </c>
       <c r="AJ53">
-        <v>135638</v>
+        <v>128638</v>
       </c>
       <c r="AK53">
-        <v>135638</v>
+        <v>133652</v>
       </c>
       <c r="AL53" s="2">
         <f t="shared" si="2"/>
-        <v>136241.4</v>
+        <v>148101.1</v>
       </c>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.25">
       <c r="L54" s="2"/>
       <c r="Y54" s="2"/>
       <c r="AA54">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="AB54">
-        <v>137626</v>
+        <v>137715</v>
       </c>
       <c r="AC54">
-        <v>131648</v>
+        <v>128656</v>
       </c>
       <c r="AD54">
-        <v>136633</v>
+        <v>161552</v>
       </c>
       <c r="AE54">
-        <v>135637</v>
+        <v>134633</v>
       </c>
       <c r="AF54">
-        <v>135637</v>
+        <v>131649</v>
       </c>
       <c r="AG54">
-        <v>260319</v>
+        <v>132644</v>
       </c>
       <c r="AH54">
-        <v>135637</v>
+        <v>132644</v>
       </c>
       <c r="AI54">
+        <v>131645</v>
+      </c>
+      <c r="AJ54">
         <v>135638</v>
       </c>
-      <c r="AJ54">
-        <v>135671</v>
-      </c>
       <c r="AK54">
-        <v>137238</v>
+        <v>135638</v>
       </c>
       <c r="AL54" s="2">
         <f t="shared" si="2"/>
-        <v>148168.4</v>
+        <v>136241.4</v>
       </c>
     </row>
     <row r="55" spans="1:39" x14ac:dyDescent="0.25">
       <c r="L55" s="2"/>
       <c r="Y55" s="2"/>
-      <c r="AL55" s="2"/>
+      <c r="AA55">
+        <v>500</v>
+      </c>
+      <c r="AB55">
+        <v>137626</v>
+      </c>
+      <c r="AC55">
+        <v>131648</v>
+      </c>
+      <c r="AD55">
+        <v>136633</v>
+      </c>
+      <c r="AE55">
+        <v>135637</v>
+      </c>
+      <c r="AF55">
+        <v>135637</v>
+      </c>
+      <c r="AG55">
+        <v>260319</v>
+      </c>
+      <c r="AH55">
+        <v>135637</v>
+      </c>
+      <c r="AI55">
+        <v>135638</v>
+      </c>
+      <c r="AJ55">
+        <v>135671</v>
+      </c>
+      <c r="AK55">
+        <v>137238</v>
+      </c>
+      <c r="AL55" s="2">
+        <f t="shared" si="2"/>
+        <v>148168.4</v>
+      </c>
     </row>
     <row r="56" spans="1:39" x14ac:dyDescent="0.25">
       <c r="L56" s="2"/>
@@ -9486,83 +9533,83 @@
       <c r="AL56" s="2"/>
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="13"/>
-      <c r="K59" s="13"/>
-      <c r="L59" s="13"/>
-      <c r="M59" s="13"/>
-      <c r="N59" s="13"/>
-      <c r="O59" s="13"/>
-      <c r="P59" s="13"/>
-      <c r="Q59" s="13"/>
-      <c r="R59" s="13"/>
-      <c r="S59" s="13"/>
-      <c r="T59" s="13"/>
-      <c r="U59" s="13"/>
-      <c r="V59" s="13"/>
-      <c r="W59" s="13"/>
-      <c r="X59" s="13"/>
-      <c r="Y59" s="13"/>
-      <c r="Z59" s="13"/>
-      <c r="AA59" s="13"/>
-      <c r="AB59" s="13"/>
-      <c r="AC59" s="13"/>
-      <c r="AD59" s="13"/>
-      <c r="AE59" s="13"/>
-      <c r="AF59" s="13"/>
-      <c r="AG59" s="13"/>
-      <c r="AH59" s="13"/>
-      <c r="AI59" s="13"/>
-      <c r="AJ59" s="13"/>
-      <c r="AK59" s="13"/>
-      <c r="AL59" s="13"/>
-      <c r="AM59" s="13"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="14"/>
+      <c r="K59" s="14"/>
+      <c r="L59" s="14"/>
+      <c r="M59" s="14"/>
+      <c r="N59" s="14"/>
+      <c r="O59" s="14"/>
+      <c r="P59" s="14"/>
+      <c r="Q59" s="14"/>
+      <c r="R59" s="14"/>
+      <c r="S59" s="14"/>
+      <c r="T59" s="14"/>
+      <c r="U59" s="14"/>
+      <c r="V59" s="14"/>
+      <c r="W59" s="14"/>
+      <c r="X59" s="14"/>
+      <c r="Y59" s="14"/>
+      <c r="Z59" s="14"/>
+      <c r="AA59" s="14"/>
+      <c r="AB59" s="14"/>
+      <c r="AC59" s="14"/>
+      <c r="AD59" s="14"/>
+      <c r="AE59" s="14"/>
+      <c r="AF59" s="14"/>
+      <c r="AG59" s="14"/>
+      <c r="AH59" s="14"/>
+      <c r="AI59" s="14"/>
+      <c r="AJ59" s="14"/>
+      <c r="AK59" s="14"/>
+      <c r="AL59" s="14"/>
+      <c r="AM59" s="14"/>
     </row>
     <row r="61" spans="1:39" x14ac:dyDescent="0.25">
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
-      <c r="E61" s="12" t="s">
+      <c r="E61" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
       <c r="O61" s="9"/>
       <c r="P61" s="9"/>
       <c r="Q61" s="9"/>
-      <c r="R61" s="12" t="s">
+      <c r="R61" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="S61" s="12"/>
-      <c r="T61" s="12"/>
-      <c r="U61" s="12"/>
-      <c r="V61" s="12"/>
+      <c r="S61" s="13"/>
+      <c r="T61" s="13"/>
+      <c r="U61" s="13"/>
+      <c r="V61" s="13"/>
       <c r="W61" s="10"/>
       <c r="X61" s="10"/>
       <c r="AB61" s="9"/>
       <c r="AC61" s="9"/>
       <c r="AD61" s="9"/>
-      <c r="AE61" s="12" t="s">
+      <c r="AE61" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="AF61" s="12"/>
-      <c r="AG61" s="12"/>
-      <c r="AH61" s="12"/>
-      <c r="AI61" s="12"/>
+      <c r="AF61" s="13"/>
+      <c r="AG61" s="13"/>
+      <c r="AH61" s="13"/>
+      <c r="AI61" s="13"/>
       <c r="AJ61" s="10"/>
       <c r="AK61" s="10"/>
       <c r="AM61" s="9"/>
@@ -13626,7 +13673,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A1:AL1"/>
     <mergeCell ref="R3:V3"/>
     <mergeCell ref="E3:I3"/>
@@ -13635,6 +13682,7 @@
     <mergeCell ref="R61:V61"/>
     <mergeCell ref="AE61:AI61"/>
     <mergeCell ref="AE3:AI3"/>
+    <mergeCell ref="AB4:AD4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -13646,7 +13694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="J8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="B56" sqref="B56:L57"/>
     </sheetView>
   </sheetViews>
@@ -13664,82 +13712,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="11"/>
-      <c r="AI1" s="11"/>
-      <c r="AJ1" s="11"/>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
-      <c r="R2" s="12" t="s">
+      <c r="R2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
       <c r="W2" s="10"/>
       <c r="X2" s="10"/>
       <c r="AB2" s="9"/>
       <c r="AC2" s="9"/>
       <c r="AD2" s="9"/>
-      <c r="AE2" s="12" t="s">
+      <c r="AE2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="12"/>
-      <c r="AI2" s="12"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="13"/>
+      <c r="AI2" s="13"/>
       <c r="AJ2" s="10"/>
       <c r="AK2" s="10"/>
     </row>
@@ -17848,82 +17896,82 @@
       </c>
     </row>
     <row r="54" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
-      <c r="O54" s="14"/>
-      <c r="P54" s="14"/>
-      <c r="Q54" s="14"/>
-      <c r="R54" s="14"/>
-      <c r="S54" s="14"/>
-      <c r="T54" s="14"/>
-      <c r="U54" s="14"/>
-      <c r="V54" s="14"/>
-      <c r="W54" s="14"/>
-      <c r="X54" s="14"/>
-      <c r="Y54" s="14"/>
-      <c r="Z54" s="14"/>
-      <c r="AA54" s="14"/>
-      <c r="AB54" s="14"/>
-      <c r="AC54" s="14"/>
-      <c r="AD54" s="14"/>
-      <c r="AE54" s="14"/>
-      <c r="AF54" s="14"/>
-      <c r="AG54" s="14"/>
-      <c r="AH54" s="14"/>
-      <c r="AI54" s="14"/>
-      <c r="AJ54" s="14"/>
-      <c r="AK54" s="14"/>
-      <c r="AL54" s="14"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
+      <c r="M54" s="15"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
+      <c r="S54" s="15"/>
+      <c r="T54" s="15"/>
+      <c r="U54" s="15"/>
+      <c r="V54" s="15"/>
+      <c r="W54" s="15"/>
+      <c r="X54" s="15"/>
+      <c r="Y54" s="15"/>
+      <c r="Z54" s="15"/>
+      <c r="AA54" s="15"/>
+      <c r="AB54" s="15"/>
+      <c r="AC54" s="15"/>
+      <c r="AD54" s="15"/>
+      <c r="AE54" s="15"/>
+      <c r="AF54" s="15"/>
+      <c r="AG54" s="15"/>
+      <c r="AH54" s="15"/>
+      <c r="AI54" s="15"/>
+      <c r="AJ54" s="15"/>
+      <c r="AK54" s="15"/>
+      <c r="AL54" s="15"/>
     </row>
     <row r="56" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
-      <c r="E56" s="12" t="s">
+      <c r="E56" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
       <c r="J56" s="10"/>
       <c r="K56" s="10"/>
       <c r="O56" s="9"/>
       <c r="P56" s="9"/>
       <c r="Q56" s="9"/>
-      <c r="R56" s="12" t="s">
+      <c r="R56" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="S56" s="12"/>
-      <c r="T56" s="12"/>
-      <c r="U56" s="12"/>
-      <c r="V56" s="12"/>
+      <c r="S56" s="13"/>
+      <c r="T56" s="13"/>
+      <c r="U56" s="13"/>
+      <c r="V56" s="13"/>
       <c r="W56" s="10"/>
       <c r="X56" s="10"/>
       <c r="AB56" s="9"/>
       <c r="AC56" s="9"/>
       <c r="AD56" s="9"/>
-      <c r="AE56" s="12" t="s">
+      <c r="AE56" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="AF56" s="12"/>
-      <c r="AG56" s="12"/>
-      <c r="AH56" s="12"/>
-      <c r="AI56" s="12"/>
+      <c r="AF56" s="13"/>
+      <c r="AG56" s="13"/>
+      <c r="AH56" s="13"/>
+      <c r="AI56" s="13"/>
       <c r="AJ56" s="10"/>
       <c r="AK56" s="10"/>
     </row>
@@ -21987,14 +22035,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="AE56:AI56"/>
+    <mergeCell ref="R56:V56"/>
+    <mergeCell ref="E56:I56"/>
     <mergeCell ref="A1:AL1"/>
     <mergeCell ref="A54:AL54"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="R2:V2"/>
     <mergeCell ref="AE2:AI2"/>
-    <mergeCell ref="AE56:AI56"/>
-    <mergeCell ref="R56:V56"/>
-    <mergeCell ref="E56:I56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>